<commit_message>
Bug Fixes and new templates
</commit_message>
<xml_diff>
--- a/Docs/Opentrons Program Templates.xlsx
+++ b/Docs/Opentrons Program Templates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dennis\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://adminliveunc-my.sharepoint.com/personal/dennis_ad_unc_edu/Documents/Projects/Programs/Opentrons_Programs/Docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6CB10FB7-93AB-481A-8DDB-8A30EB088550}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="38" documentId="8_{6CB10FB7-93AB-481A-8DDB-8A30EB088550}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{85DD19A2-418C-4639-83EF-AD60654DC915}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="4240" yWindow="4150" windowWidth="34160" windowHeight="16850" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ddPCR" sheetId="5" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="160">
   <si>
     <t>Source Well</t>
   </si>
@@ -138,15 +138,6 @@
     <t>p10_multi</t>
   </si>
   <si>
-    <t># Pipette Tip Racks</t>
-  </si>
-  <si>
-    <t>--LeftPipetteTipRackSlot</t>
-  </si>
-  <si>
-    <t>--RightPipetteTipRackSlot</t>
-  </si>
-  <si>
     <t>Labware Name</t>
   </si>
   <si>
@@ -159,12 +150,6 @@
     <t>p300_single_gen2</t>
   </si>
   <si>
-    <t>Slot number.  Separate multiple with commas.  Example 1,2,3</t>
-  </si>
-  <si>
-    <t>Slot number.  Separate multiple with commas.  Example 1,2,4</t>
-  </si>
-  <si>
     <t># Slot Assignments</t>
   </si>
   <si>
@@ -351,9 +336,6 @@
     <t>5 mL conical tubes in one of the 15 well Opentrons racks</t>
   </si>
   <si>
-    <t>Always a 2x mix.  Since ddPCR supermix can be 4x we may change this</t>
-  </si>
-  <si>
     <t>Enter Volume in uL</t>
   </si>
   <si>
@@ -519,16 +501,22 @@
     <t>opentrons_96_filtertiprack_20ul</t>
   </si>
   <si>
-    <t xml:space="preserve"> v0.5.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> v0.4.1</t>
-  </si>
-  <si>
     <t># The positive control volume used is always the maximum volume allowed.</t>
   </si>
   <si>
-    <t xml:space="preserve"> v0.2.1</t>
+    <t># First Pipette Tip</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> v0.3.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> v0.6.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> v0.5.0</t>
+  </si>
+  <si>
+    <t>Always a 2x mix.</t>
   </si>
 </sst>
 </file>
@@ -560,13 +548,6 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -574,13 +555,6 @@
     </font>
     <font>
       <sz val="8"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -696,8 +670,21 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -745,8 +732,14 @@
         <bgColor theme="4" tint="0.79998168889431442"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="8">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -827,172 +820,238 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="10" fillId="8" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="17" fillId="5" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="8" fillId="8" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="15" fillId="5" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="17" fillId="6" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="19" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="180"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="6" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="21" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1000,52 +1059,7 @@
     <cellStyle name="Accent4" xfId="1" builtinId="41"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="25">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="22">
     <dxf>
       <fill>
         <patternFill>
@@ -1283,6 +1297,30 @@
     <dxf>
       <numFmt numFmtId="165" formatCode="0.0"/>
     </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1297,46 +1335,46 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{0AFC3E1F-23DC-4281-9692-1635ECE808ED}" name="Table14" displayName="Table14" ref="A78:F174" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A78:F174" xr:uid="{E9F71635-090B-4C48-B890-1CC5A8BA778F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{0AFC3E1F-23DC-4281-9692-1635ECE808ED}" name="Table14" displayName="Table14" ref="A76:F172" totalsRowShown="0" headerRowDxfId="21">
+  <autoFilter ref="A76:F172" xr:uid="{E9F71635-090B-4C48-B890-1CC5A8BA778F}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{1C94D97C-CFBE-4070-B57B-40D584ADAD4C}" name="# Source Slot"/>
     <tableColumn id="2" xr3:uid="{7F951B2F-B449-4323-9BA7-A6CCBE2503A2}" name="Source Well"/>
     <tableColumn id="3" xr3:uid="{92E3F929-8373-433B-85FD-B9AAAC53CEBC}" name="Sample Name"/>
-    <tableColumn id="4" xr3:uid="{591C18FD-B808-47C9-9CB4-E7688E5D4F2F}" name="Concentration ng/uL" dataDxfId="24"/>
-    <tableColumn id="5" xr3:uid="{D1888A8E-4AA2-4C96-A740-71BA0E6A02D8}" name="Target(s)" dataDxfId="23"/>
-    <tableColumn id="6" xr3:uid="{C4F4ADEA-237D-43B7-8280-EDDE7908D4FA}" name="Replicates" dataDxfId="22"/>
+    <tableColumn id="4" xr3:uid="{591C18FD-B808-47C9-9CB4-E7688E5D4F2F}" name="Concentration ng/uL" dataDxfId="20"/>
+    <tableColumn id="5" xr3:uid="{D1888A8E-4AA2-4C96-A740-71BA0E6A02D8}" name="Target(s)" dataDxfId="19"/>
+    <tableColumn id="6" xr3:uid="{C4F4ADEA-237D-43B7-8280-EDDE7908D4FA}" name="Replicates" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6E2D2C82-AED1-4EFD-B514-45C88869B632}" name="Table1" displayName="Table1" ref="A47:F455" totalsRowShown="0" headerRowDxfId="21">
-  <autoFilter ref="A47:F455" xr:uid="{E9F71635-090B-4C48-B890-1CC5A8BA778F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6E2D2C82-AED1-4EFD-B514-45C88869B632}" name="Table1" displayName="Table1" ref="A45:F453" totalsRowShown="0" headerRowDxfId="17">
+  <autoFilter ref="A45:F453" xr:uid="{E9F71635-090B-4C48-B890-1CC5A8BA778F}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{869EDE9B-E883-4A3E-BC84-177627B77820}" name="# Source Slot"/>
     <tableColumn id="2" xr3:uid="{BFF29CE8-BC36-441D-BF7C-4D3ECA705071}" name="Source Well"/>
     <tableColumn id="3" xr3:uid="{BE3B5A50-56B7-458D-A1B8-EA325514A953}" name="Sample"/>
-    <tableColumn id="4" xr3:uid="{51C9CB7B-3C83-4DF7-B90E-3B3B2F0517EB}" name="Concentration ng/uL" dataDxfId="20"/>
-    <tableColumn id="5" xr3:uid="{F1CA2FD2-DD2B-44E5-934D-9BDE08DCFF66}" name="Destination Slot" dataDxfId="19"/>
-    <tableColumn id="6" xr3:uid="{7F589CB2-9FD4-4968-8CE1-91953E95F345}" name="Destination Well" dataDxfId="18"/>
+    <tableColumn id="4" xr3:uid="{51C9CB7B-3C83-4DF7-B90E-3B3B2F0517EB}" name="Concentration ng/uL" dataDxfId="16"/>
+    <tableColumn id="5" xr3:uid="{F1CA2FD2-DD2B-44E5-934D-9BDE08DCFF66}" name="Destination Slot" dataDxfId="15"/>
+    <tableColumn id="6" xr3:uid="{7F589CB2-9FD4-4968-8CE1-91953E95F345}" name="Destination Well" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4A1EA636-4A66-4384-BAA4-76D238021771}" name="Table13" displayName="Table13" ref="A70:G478" totalsRowShown="0" headerRowDxfId="17">
-  <autoFilter ref="A70:G478" xr:uid="{E9F71635-090B-4C48-B890-1CC5A8BA778F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4A1EA636-4A66-4384-BAA4-76D238021771}" name="Table13" displayName="Table13" ref="A69:G477" totalsRowShown="0" headerRowDxfId="13">
+  <autoFilter ref="A69:G477" xr:uid="{E9F71635-090B-4C48-B890-1CC5A8BA778F}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{F86BB3DB-CF90-48B8-8F35-E42977442672}" name="# Source Slot"/>
     <tableColumn id="2" xr3:uid="{C0F53F8F-C6A8-4F67-BF04-2D1C3AE40DC7}" name="Source Well"/>
     <tableColumn id="8" xr3:uid="{466B28CD-7413-41AF-A6D9-1A9460F0F6F4}" name="Index"/>
     <tableColumn id="3" xr3:uid="{FB50DE30-1861-4AAD-B46A-522A9F77B092}" name="Sample"/>
-    <tableColumn id="4" xr3:uid="{624B6C14-EDFA-405E-9149-7A4DAA0A5782}" name="Concentration ng/uL" dataDxfId="16"/>
-    <tableColumn id="5" xr3:uid="{A82E5DDD-FDEB-4967-8780-CF48E4C9A4DF}" name="Destination Slot" dataDxfId="15"/>
-    <tableColumn id="6" xr3:uid="{28DE797A-4F93-44BF-AC9A-BA038C116648}" name="Destination Well" dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{624B6C14-EDFA-405E-9149-7A4DAA0A5782}" name="Concentration ng/uL" dataDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{A82E5DDD-FDEB-4967-8780-CF48E4C9A4DF}" name="Destination Slot" dataDxfId="11"/>
+    <tableColumn id="6" xr3:uid="{28DE797A-4F93-44BF-AC9A-BA038C116648}" name="Destination Well" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1543,10 +1581,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F252"/>
+  <dimension ref="A1:F250"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView topLeftCell="A46" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="L30" sqref="L30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1559,15 +1597,15 @@
     <col min="6" max="6" width="20.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="67" t="s">
-        <v>152</v>
-      </c>
-      <c r="B1" s="68" t="s">
-        <v>163</v>
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.4">
+      <c r="A1" s="84" t="s">
+        <v>146</v>
+      </c>
+      <c r="B1" s="85" t="s">
+        <v>156</v>
       </c>
       <c r="C1" s="54" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D1" s="54"/>
       <c r="E1" s="54"/>
@@ -1575,11 +1613,11 @@
     </row>
     <row r="2" spans="1:6" ht="13" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="54" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D2" s="54"/>
       <c r="E2" s="54"/>
@@ -1595,19 +1633,19 @@
       <c r="A4" s="2"/>
     </row>
     <row r="5" spans="1:6" ht="6.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="12"/>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
+      <c r="A5" s="10"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
     </row>
     <row r="6" spans="1:6" ht="13" x14ac:dyDescent="0.3">
-      <c r="A6" s="26" t="s">
-        <v>42</v>
+      <c r="A6" s="23" t="s">
+        <v>37</v>
       </c>
       <c r="B6" s="55" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C6" s="55"/>
       <c r="D6" s="55"/>
@@ -1615,138 +1653,138 @@
       <c r="F6" s="55"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="53"/>
-      <c r="C7" s="53"/>
-      <c r="D7" s="53"/>
-      <c r="E7" s="53"/>
-      <c r="F7" s="53"/>
+      <c r="B7" s="52"/>
+      <c r="C7" s="52"/>
+      <c r="D7" s="52"/>
+      <c r="E7" s="52"/>
+      <c r="F7" s="52"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="56"/>
-      <c r="C8" s="56"/>
-      <c r="D8" s="56"/>
-      <c r="E8" s="56"/>
-      <c r="F8" s="56"/>
+      <c r="B8" s="51"/>
+      <c r="C8" s="51"/>
+      <c r="D8" s="51"/>
+      <c r="E8" s="51"/>
+      <c r="F8" s="51"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="24" t="s">
+      <c r="A9" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="53"/>
-      <c r="C9" s="53"/>
-      <c r="D9" s="53"/>
-      <c r="E9" s="53"/>
-      <c r="F9" s="53"/>
+      <c r="B9" s="52"/>
+      <c r="C9" s="52"/>
+      <c r="D9" s="52"/>
+      <c r="E9" s="52"/>
+      <c r="F9" s="52"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="56"/>
-      <c r="C10" s="56"/>
-      <c r="D10" s="56"/>
-      <c r="E10" s="56"/>
-      <c r="F10" s="56"/>
+      <c r="B10" s="51"/>
+      <c r="C10" s="51"/>
+      <c r="D10" s="51"/>
+      <c r="E10" s="51"/>
+      <c r="F10" s="51"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="24" t="s">
+      <c r="A11" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="53"/>
-      <c r="C11" s="53"/>
-      <c r="D11" s="53"/>
-      <c r="E11" s="53"/>
-      <c r="F11" s="53"/>
+      <c r="B11" s="52"/>
+      <c r="C11" s="52"/>
+      <c r="D11" s="52"/>
+      <c r="E11" s="52"/>
+      <c r="F11" s="52"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="56"/>
-      <c r="C12" s="56"/>
-      <c r="D12" s="56"/>
-      <c r="E12" s="56"/>
-      <c r="F12" s="56"/>
+      <c r="B12" s="51"/>
+      <c r="C12" s="51"/>
+      <c r="D12" s="51"/>
+      <c r="E12" s="51"/>
+      <c r="F12" s="51"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="24" t="s">
+      <c r="A13" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="53"/>
-      <c r="C13" s="53"/>
-      <c r="D13" s="53"/>
-      <c r="E13" s="53"/>
-      <c r="F13" s="53"/>
+      <c r="B13" s="52"/>
+      <c r="C13" s="52"/>
+      <c r="D13" s="52"/>
+      <c r="E13" s="52"/>
+      <c r="F13" s="52"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="56"/>
-      <c r="C14" s="56"/>
-      <c r="D14" s="56"/>
-      <c r="E14" s="56"/>
-      <c r="F14" s="56"/>
+      <c r="B14" s="51"/>
+      <c r="C14" s="51"/>
+      <c r="D14" s="51"/>
+      <c r="E14" s="51"/>
+      <c r="F14" s="51"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="24" t="s">
+      <c r="A15" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="53"/>
-      <c r="C15" s="53"/>
-      <c r="D15" s="53"/>
-      <c r="E15" s="53"/>
-      <c r="F15" s="53"/>
+      <c r="B15" s="52"/>
+      <c r="C15" s="52"/>
+      <c r="D15" s="52"/>
+      <c r="E15" s="52"/>
+      <c r="F15" s="52"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="56"/>
-      <c r="C16" s="56"/>
-      <c r="D16" s="56"/>
-      <c r="E16" s="56"/>
-      <c r="F16" s="56"/>
+      <c r="B16" s="51"/>
+      <c r="C16" s="51"/>
+      <c r="D16" s="51"/>
+      <c r="E16" s="51"/>
+      <c r="F16" s="51"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="24" t="s">
+      <c r="A17" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="53"/>
-      <c r="C17" s="53"/>
-      <c r="D17" s="53"/>
-      <c r="E17" s="53"/>
-      <c r="F17" s="53"/>
+      <c r="B17" s="52"/>
+      <c r="C17" s="52"/>
+      <c r="D17" s="52"/>
+      <c r="E17" s="52"/>
+      <c r="F17" s="52"/>
     </row>
     <row r="18" spans="1:6" ht="6.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="12"/>
-      <c r="B18" s="13"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-    </row>
-    <row r="19" spans="1:6" s="15" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="14"/>
+      <c r="A18" s="10"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+    </row>
+    <row r="19" spans="1:6" s="13" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="12"/>
     </row>
     <row r="20" spans="1:6" s="8" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A20" s="71" t="s">
-        <v>43</v>
-      </c>
-      <c r="B20" s="69"/>
+      <c r="A20" s="43" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="41"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B21" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -1754,415 +1792,409 @@
         <v>27</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="6.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="12"/>
-      <c r="B23" s="13"/>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
+      <c r="A23" s="10"/>
+      <c r="B23" s="11"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="C24" s="2"/>
     </row>
-    <row r="25" spans="1:6" s="70" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A25" s="72" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="B26" s="18"/>
-      <c r="C26" s="57" t="s">
-        <v>40</v>
-      </c>
-      <c r="D26" s="57"/>
-      <c r="E26" s="57"/>
-      <c r="F26" s="57"/>
-    </row>
-    <row r="27" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="B27" s="20"/>
-      <c r="C27" s="57"/>
-      <c r="D27" s="57"/>
-      <c r="E27" s="57"/>
-      <c r="F27" s="57"/>
-    </row>
-    <row r="28" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="17" t="s">
-        <v>118</v>
-      </c>
-      <c r="B28" s="20" t="s">
+    <row r="25" spans="1:6" s="42" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A25" s="44" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="B26" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="C28" s="57" t="s">
-        <v>120</v>
-      </c>
-      <c r="D28" s="57"/>
-      <c r="E28" s="57"/>
-      <c r="F28" s="57"/>
-    </row>
-    <row r="29" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="14" t="s">
-        <v>119</v>
-      </c>
-      <c r="B29" s="18" t="s">
+      <c r="C26" s="53" t="s">
+        <v>114</v>
+      </c>
+      <c r="D26" s="53"/>
+      <c r="E26" s="53"/>
+      <c r="F26" s="53"/>
+    </row>
+    <row r="27" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="B27" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="C29" s="57"/>
-      <c r="D29" s="57"/>
-      <c r="E29" s="57"/>
-      <c r="F29" s="57"/>
-    </row>
-    <row r="30" spans="1:6" ht="6.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="12"/>
-      <c r="B30" s="13"/>
-      <c r="C30" s="13"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
-    </row>
-    <row r="31" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="17"/>
-      <c r="B31" s="20"/>
-      <c r="C31" s="19"/>
-    </row>
-    <row r="32" spans="1:6" s="8" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A32" s="71" t="s">
+      <c r="C27" s="53"/>
+      <c r="D27" s="53"/>
+      <c r="E27" s="53"/>
+      <c r="F27" s="53"/>
+    </row>
+    <row r="28" spans="1:6" ht="6.65" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="10"/>
+      <c r="B28" s="11"/>
+      <c r="C28" s="11"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="11"/>
+      <c r="F28" s="11"/>
+    </row>
+    <row r="29" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="14"/>
+      <c r="B29" s="17"/>
+      <c r="C29" s="16"/>
+    </row>
+    <row r="30" spans="1:6" s="8" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A30" s="43" t="s">
         <v>23</v>
       </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B31" s="6"/>
+      <c r="C31" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B32" s="5"/>
+      <c r="C32" s="2"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B33" s="6"/>
+        <v>101</v>
+      </c>
+      <c r="B33" s="5"/>
       <c r="C33" s="2" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B34" s="5"/>
       <c r="C34" s="2"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B35" s="5"/>
       <c r="C35" s="2" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="B36" s="5"/>
-      <c r="C36" s="2"/>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="B37" s="5"/>
-      <c r="C37" s="2" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" ht="6.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="12"/>
-      <c r="B38" s="13"/>
-      <c r="C38" s="13"/>
-      <c r="D38" s="13"/>
-      <c r="E38" s="13"/>
-      <c r="F38" s="13"/>
-    </row>
-    <row r="40" spans="1:6" s="8" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A40" s="73" t="s">
-        <v>58</v>
-      </c>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="6.65" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="10"/>
+      <c r="B36" s="11"/>
+      <c r="C36" s="11"/>
+      <c r="D36" s="11"/>
+      <c r="E36" s="11"/>
+      <c r="F36" s="11"/>
+    </row>
+    <row r="38" spans="1:6" s="8" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A38" s="45" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="B39" s="30"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="B40" s="30"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="B41" s="38"/>
+        <v>145</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="B42" s="38"/>
+      <c r="A42" s="3"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B43" s="7"/>
+      <c r="C43" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B44" s="7"/>
+      <c r="C44" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="6.65" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="10"/>
+      <c r="B45" s="11"/>
+      <c r="C45" s="11"/>
+      <c r="D45" s="11"/>
+      <c r="E45" s="11"/>
+      <c r="F45" s="11"/>
+    </row>
+    <row r="47" spans="1:6" s="8" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A47" s="43" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="31"/>
+      <c r="B49" s="32"/>
+      <c r="C49" s="33"/>
+    </row>
+    <row r="50" spans="1:4" s="47" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+      <c r="A50" s="46" t="s">
+        <v>150</v>
+      </c>
+      <c r="B50" s="56" t="s">
+        <v>148</v>
+      </c>
+      <c r="C50" s="56"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="34" t="s">
+        <v>117</v>
+      </c>
+      <c r="B51" s="57"/>
+      <c r="C51" s="57"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="35" t="s">
+        <v>118</v>
+      </c>
+      <c r="B52" s="58"/>
+      <c r="C52" s="59"/>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="34" t="s">
+        <v>119</v>
+      </c>
+      <c r="B53" s="57"/>
+      <c r="C53" s="57"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="35" t="s">
+        <v>120</v>
+      </c>
+      <c r="B54" s="58"/>
+      <c r="C54" s="59"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="34" t="s">
+        <v>121</v>
+      </c>
+      <c r="B55" s="57"/>
+      <c r="C55" s="57"/>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="35" t="s">
+        <v>122</v>
+      </c>
+      <c r="B56" s="58"/>
+      <c r="C56" s="59"/>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="34" t="s">
+        <v>123</v>
+      </c>
+      <c r="B57" s="57"/>
+      <c r="C57" s="57"/>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="35" t="s">
+        <v>124</v>
+      </c>
+      <c r="B58" s="58"/>
+      <c r="C58" s="59"/>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="34" t="s">
+        <v>125</v>
+      </c>
+      <c r="B59" s="57"/>
+      <c r="C59" s="57"/>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="36" t="s">
+        <v>126</v>
+      </c>
+      <c r="B60" s="60"/>
+      <c r="C60" s="61"/>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="29"/>
+    </row>
+    <row r="62" spans="1:4" ht="14" x14ac:dyDescent="0.3">
+      <c r="A62" s="38" t="s">
         <v>151</v>
       </c>
-      <c r="B43" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="3"/>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B45" s="7"/>
-      <c r="C45" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B46" s="7"/>
-      <c r="C46" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" ht="6.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="12"/>
-      <c r="B47" s="13"/>
-      <c r="C47" s="13"/>
-      <c r="D47" s="13"/>
-      <c r="E47" s="13"/>
-      <c r="F47" s="13"/>
-    </row>
-    <row r="49" spans="1:3" s="8" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A49" s="71" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="3" t="s">
+      <c r="B62" s="62" t="s">
         <v>148</v>
       </c>
-      <c r="C50" s="2" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="39"/>
-      <c r="B51" s="40"/>
-      <c r="C51" s="41"/>
-    </row>
-    <row r="52" spans="1:3" s="76" customFormat="1" ht="14" x14ac:dyDescent="0.3">
-      <c r="A52" s="74" t="s">
-        <v>156</v>
-      </c>
-      <c r="B52" s="75" t="s">
+      <c r="C62" s="62"/>
+    </row>
+    <row r="63" spans="1:4" ht="14" x14ac:dyDescent="0.3">
+      <c r="A63" s="40" t="s">
+        <v>127</v>
+      </c>
+      <c r="B63" s="63"/>
+      <c r="C63" s="63"/>
+      <c r="D63" s="2" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B64" s="64"/>
+      <c r="C64" s="64"/>
+      <c r="D64" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="C52" s="75"/>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="42" t="s">
-        <v>123</v>
-      </c>
-      <c r="B53" s="52"/>
-      <c r="C53" s="52"/>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="43" t="s">
-        <v>124</v>
-      </c>
-      <c r="B54" s="65"/>
-      <c r="C54" s="66"/>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="42" t="s">
-        <v>125</v>
-      </c>
-      <c r="B55" s="52"/>
-      <c r="C55" s="52"/>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="43" t="s">
-        <v>126</v>
-      </c>
-      <c r="B56" s="65"/>
-      <c r="C56" s="66"/>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="42" t="s">
-        <v>127</v>
-      </c>
-      <c r="B57" s="52"/>
-      <c r="C57" s="52"/>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="43" t="s">
-        <v>128</v>
-      </c>
-      <c r="B58" s="65"/>
-      <c r="C58" s="66"/>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" s="42" t="s">
+    </row>
+    <row r="65" spans="1:6" ht="14" x14ac:dyDescent="0.3">
+      <c r="A65" s="40" t="s">
         <v>129</v>
       </c>
-      <c r="B59" s="52"/>
-      <c r="C59" s="52"/>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" s="43" t="s">
-        <v>130</v>
-      </c>
-      <c r="B60" s="65"/>
-      <c r="C60" s="66"/>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" s="42" t="s">
-        <v>131</v>
-      </c>
-      <c r="B61" s="52"/>
-      <c r="C61" s="52"/>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" s="44" t="s">
-        <v>132</v>
-      </c>
-      <c r="B62" s="63"/>
-      <c r="C62" s="64"/>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" s="37"/>
-    </row>
-    <row r="64" spans="1:3" ht="14" x14ac:dyDescent="0.3">
-      <c r="A64" s="46" t="s">
-        <v>157</v>
-      </c>
-      <c r="B64" s="51" t="s">
-        <v>154</v>
-      </c>
-      <c r="C64" s="51"/>
-    </row>
-    <row r="65" spans="1:6" ht="14" x14ac:dyDescent="0.3">
-      <c r="A65" s="62" t="s">
-        <v>133</v>
-      </c>
-      <c r="B65" s="48"/>
-      <c r="C65" s="48"/>
-      <c r="D65" s="2" t="s">
-        <v>158</v>
-      </c>
+      <c r="B65" s="63"/>
+      <c r="C65" s="63"/>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="B66" s="50"/>
-      <c r="C66" s="50"/>
-      <c r="D66" s="2" t="s">
-        <v>162</v>
-      </c>
+        <v>130</v>
+      </c>
+      <c r="B66" s="64"/>
+      <c r="C66" s="64"/>
     </row>
     <row r="67" spans="1:6" ht="14" x14ac:dyDescent="0.3">
-      <c r="A67" s="62" t="s">
-        <v>135</v>
-      </c>
-      <c r="B67" s="48"/>
-      <c r="C67" s="48"/>
+      <c r="A67" s="40" t="s">
+        <v>131</v>
+      </c>
+      <c r="B67" s="63"/>
+      <c r="C67" s="63"/>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="B68" s="50"/>
-      <c r="C68" s="50"/>
+        <v>132</v>
+      </c>
+      <c r="B68" s="64"/>
+      <c r="C68" s="64"/>
     </row>
     <row r="69" spans="1:6" ht="14" x14ac:dyDescent="0.3">
-      <c r="A69" s="62" t="s">
-        <v>137</v>
-      </c>
-      <c r="B69" s="48"/>
-      <c r="C69" s="48"/>
+      <c r="A69" s="40" t="s">
+        <v>133</v>
+      </c>
+      <c r="B69" s="63"/>
+      <c r="C69" s="63"/>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B70" s="64"/>
+      <c r="C70" s="64"/>
+    </row>
+    <row r="71" spans="1:6" ht="14" x14ac:dyDescent="0.3">
+      <c r="A71" s="40" t="s">
+        <v>135</v>
+      </c>
+      <c r="B71" s="63"/>
+      <c r="C71" s="63"/>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72" s="37" t="s">
+        <v>136</v>
+      </c>
+      <c r="B72" s="65"/>
+      <c r="C72" s="65"/>
+    </row>
+    <row r="73" spans="1:6" ht="6.65" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="10"/>
+      <c r="B73" s="11"/>
+      <c r="C73" s="11"/>
+      <c r="D73" s="11"/>
+      <c r="E73" s="11"/>
+      <c r="F73" s="11"/>
+    </row>
+    <row r="75" spans="1:6" s="8" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A75" s="45" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" s="47" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+      <c r="A76" s="48" t="s">
+        <v>24</v>
+      </c>
+      <c r="B76" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="C76" s="50" t="s">
+        <v>137</v>
+      </c>
+      <c r="D76" s="50" t="s">
+        <v>4</v>
+      </c>
+      <c r="E76" s="50" t="s">
         <v>138</v>
       </c>
-      <c r="B70" s="50"/>
-      <c r="C70" s="50"/>
-    </row>
-    <row r="71" spans="1:6" ht="14" x14ac:dyDescent="0.3">
-      <c r="A71" s="62" t="s">
+      <c r="F76" s="50" t="s">
         <v>139</v>
       </c>
-      <c r="B71" s="48"/>
-      <c r="C71" s="48"/>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="B72" s="50"/>
-      <c r="C72" s="50"/>
-    </row>
-    <row r="73" spans="1:6" ht="14" x14ac:dyDescent="0.3">
-      <c r="A73" s="62" t="s">
-        <v>141</v>
-      </c>
-      <c r="B73" s="48"/>
-      <c r="C73" s="48"/>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74" s="45" t="s">
-        <v>142</v>
-      </c>
-      <c r="B74" s="49"/>
-      <c r="C74" s="49"/>
-    </row>
-    <row r="75" spans="1:6" ht="6.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="12"/>
-      <c r="B75" s="13"/>
-      <c r="C75" s="13"/>
-      <c r="D75" s="13"/>
-      <c r="E75" s="13"/>
-      <c r="F75" s="13"/>
-    </row>
-    <row r="77" spans="1:6" s="8" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A77" s="73" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" s="76" customFormat="1" ht="14" x14ac:dyDescent="0.3">
-      <c r="A78" s="77" t="s">
-        <v>24</v>
-      </c>
-      <c r="B78" s="78" t="s">
-        <v>0</v>
-      </c>
-      <c r="C78" s="79" t="s">
-        <v>143</v>
-      </c>
-      <c r="D78" s="79" t="s">
-        <v>4</v>
-      </c>
-      <c r="E78" s="79" t="s">
-        <v>144</v>
-      </c>
-      <c r="F78" s="79" t="s">
-        <v>145</v>
-      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77" s="6"/>
+      <c r="B77" s="5"/>
+      <c r="C77" s="2"/>
+      <c r="D77" s="7"/>
+      <c r="E77" s="6"/>
+      <c r="F77" s="5"/>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78" s="6"/>
+      <c r="B78" s="5"/>
+      <c r="C78" s="2"/>
+      <c r="D78" s="7"/>
+      <c r="E78" s="5"/>
+      <c r="F78" s="5"/>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="6"/>
@@ -2177,24 +2209,22 @@
       <c r="B80" s="5"/>
       <c r="C80" s="2"/>
       <c r="D80" s="7"/>
-      <c r="E80" s="5"/>
+      <c r="E80" s="6"/>
       <c r="F80" s="5"/>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="6"/>
-      <c r="B81" s="5"/>
-      <c r="C81" s="2"/>
+      <c r="B81" s="6"/>
       <c r="D81" s="7"/>
       <c r="E81" s="6"/>
-      <c r="F81" s="5"/>
+      <c r="F81" s="6"/>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="6"/>
-      <c r="B82" s="5"/>
-      <c r="C82" s="2"/>
+      <c r="B82" s="6"/>
       <c r="D82" s="7"/>
       <c r="E82" s="6"/>
-      <c r="F82" s="5"/>
+      <c r="F82" s="6"/>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="6"/>
@@ -2827,16 +2857,10 @@
       <c r="F172" s="6"/>
     </row>
     <row r="173" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A173" s="6"/>
-      <c r="B173" s="6"/>
-      <c r="D173" s="7"/>
       <c r="E173" s="6"/>
       <c r="F173" s="6"/>
     </row>
     <row r="174" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A174" s="6"/>
-      <c r="B174" s="6"/>
-      <c r="D174" s="7"/>
       <c r="E174" s="6"/>
       <c r="F174" s="6"/>
     </row>
@@ -3144,79 +3168,65 @@
       <c r="E250" s="6"/>
       <c r="F250" s="6"/>
     </row>
-    <row r="251" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E251" s="6"/>
-      <c r="F251" s="6"/>
-    </row>
-    <row r="252" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E252" s="6"/>
-      <c r="F252" s="6"/>
-    </row>
   </sheetData>
-  <mergeCells count="38">
+  <mergeCells count="37">
+    <mergeCell ref="B71:C71"/>
+    <mergeCell ref="B72:C72"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="B9:F9"/>
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="B6:F6"/>
+    <mergeCell ref="B7:F7"/>
+    <mergeCell ref="B8:F8"/>
     <mergeCell ref="B16:F16"/>
     <mergeCell ref="B17:F17"/>
     <mergeCell ref="C26:F27"/>
-    <mergeCell ref="C28:F29"/>
     <mergeCell ref="B10:F10"/>
     <mergeCell ref="B11:F11"/>
     <mergeCell ref="B12:F12"/>
     <mergeCell ref="B13:F13"/>
     <mergeCell ref="B14:F14"/>
     <mergeCell ref="B15:F15"/>
-    <mergeCell ref="B9:F9"/>
-    <mergeCell ref="C1:F1"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="B6:F6"/>
-    <mergeCell ref="B7:F7"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="B61:C61"/>
-    <mergeCell ref="B62:C62"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="B73:C73"/>
-    <mergeCell ref="B74:C74"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="B71:C71"/>
-    <mergeCell ref="B72:C72"/>
   </mergeCells>
-  <phoneticPr fontId="15" type="noConversion"/>
-  <conditionalFormatting sqref="D79:D174">
-    <cfRule type="expression" dxfId="13" priority="4">
-      <formula>($B$45/$D79)&gt;(0.5*$B$46)</formula>
+  <phoneticPr fontId="13" type="noConversion"/>
+  <conditionalFormatting sqref="D77:D172">
+    <cfRule type="expression" dxfId="9" priority="4">
+      <formula>($B$43/$D77)&gt;(0.5*$B$44)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B3 B21:B22 B33:B37 B41:B42 B45:B46">
-    <cfRule type="containsBlanks" dxfId="12" priority="3">
+  <conditionalFormatting sqref="B2:B3 B21:B22 B31:B35 B39:B40 B43:B44 B26:B27">
+    <cfRule type="containsBlanks" dxfId="8" priority="3">
       <formula>LEN(TRIM(B2))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B26:B29">
-    <cfRule type="containsBlanks" dxfId="11" priority="2">
-      <formula>LEN(TRIM(B26))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B50">
-    <cfRule type="containsBlanks" dxfId="10" priority="1">
-      <formula>LEN(TRIM(B50))=0</formula>
+  <conditionalFormatting sqref="B48">
+    <cfRule type="containsBlanks" dxfId="7" priority="1">
+      <formula>LEN(TRIM(B48))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Slot must be between 1 and 11" sqref="B31 B26:B28" xr:uid="{7EA488CB-C77F-4490-92FA-1821AC567FF6}"/>
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B41:B42 B45:B46" xr:uid="{727FCE64-D09B-4D4D-B81E-FAB7FB2E5C88}">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Slot must be between 1 and 11" sqref="B29 B26" xr:uid="{7EA488CB-C77F-4490-92FA-1821AC567FF6}"/>
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B39:B40 B43:B44" xr:uid="{727FCE64-D09B-4D4D-B81E-FAB7FB2E5C88}">
       <formula1>0</formula1>
     </dataValidation>
   </dataValidations>
@@ -3248,10 +3258,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B096AE39-CBE9-438B-8EF5-43BA511A3359}">
-  <dimension ref="A1:I564"/>
+  <dimension ref="A1:I562"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView topLeftCell="A27" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="H51" sqref="H51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -3266,15 +3276,15 @@
     <col min="8" max="8" width="20.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="14" x14ac:dyDescent="0.3">
-      <c r="A1" s="36" t="s">
-        <v>97</v>
-      </c>
-      <c r="B1" s="35" t="s">
-        <v>160</v>
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.4">
+      <c r="A1" s="84" t="s">
+        <v>92</v>
+      </c>
+      <c r="B1" s="85" t="s">
+        <v>157</v>
       </c>
       <c r="C1" s="54" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D1" s="54"/>
       <c r="E1" s="54"/>
@@ -3286,7 +3296,7 @@
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="54" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D2" s="54"/>
       <c r="E2" s="54"/>
@@ -3302,19 +3312,19 @@
       <c r="A4" s="2"/>
     </row>
     <row r="5" spans="1:6" ht="6.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="12"/>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
+      <c r="A5" s="10"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
     </row>
     <row r="6" spans="1:6" ht="13" x14ac:dyDescent="0.3">
-      <c r="A6" s="26" t="s">
-        <v>42</v>
+      <c r="A6" s="67" t="s">
+        <v>37</v>
       </c>
       <c r="B6" s="55" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C6" s="55"/>
       <c r="D6" s="55"/>
@@ -3322,129 +3332,129 @@
       <c r="F6" s="55"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="53"/>
-      <c r="C7" s="53"/>
-      <c r="D7" s="53"/>
-      <c r="E7" s="53"/>
-      <c r="F7" s="53"/>
+      <c r="B7" s="52"/>
+      <c r="C7" s="52"/>
+      <c r="D7" s="52"/>
+      <c r="E7" s="52"/>
+      <c r="F7" s="52"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="56"/>
-      <c r="C8" s="56"/>
-      <c r="D8" s="56"/>
-      <c r="E8" s="56"/>
-      <c r="F8" s="56"/>
+      <c r="B8" s="51"/>
+      <c r="C8" s="51"/>
+      <c r="D8" s="51"/>
+      <c r="E8" s="51"/>
+      <c r="F8" s="51"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="24" t="s">
+      <c r="A9" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="53"/>
-      <c r="C9" s="53"/>
-      <c r="D9" s="53"/>
-      <c r="E9" s="53"/>
-      <c r="F9" s="53"/>
+      <c r="B9" s="52"/>
+      <c r="C9" s="52"/>
+      <c r="D9" s="52"/>
+      <c r="E9" s="52"/>
+      <c r="F9" s="52"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="56"/>
-      <c r="C10" s="56"/>
-      <c r="D10" s="56"/>
-      <c r="E10" s="56"/>
-      <c r="F10" s="56"/>
+      <c r="B10" s="51"/>
+      <c r="C10" s="51"/>
+      <c r="D10" s="51"/>
+      <c r="E10" s="51"/>
+      <c r="F10" s="51"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="24" t="s">
+      <c r="A11" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="53"/>
-      <c r="C11" s="53"/>
-      <c r="D11" s="53"/>
-      <c r="E11" s="53"/>
-      <c r="F11" s="53"/>
+      <c r="B11" s="52"/>
+      <c r="C11" s="52"/>
+      <c r="D11" s="52"/>
+      <c r="E11" s="52"/>
+      <c r="F11" s="52"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="56"/>
-      <c r="C12" s="56"/>
-      <c r="D12" s="56"/>
-      <c r="E12" s="56"/>
-      <c r="F12" s="56"/>
+      <c r="B12" s="51"/>
+      <c r="C12" s="51"/>
+      <c r="D12" s="51"/>
+      <c r="E12" s="51"/>
+      <c r="F12" s="51"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="24" t="s">
+      <c r="A13" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="53"/>
-      <c r="C13" s="53"/>
-      <c r="D13" s="53"/>
-      <c r="E13" s="53"/>
-      <c r="F13" s="53"/>
+      <c r="B13" s="52"/>
+      <c r="C13" s="52"/>
+      <c r="D13" s="52"/>
+      <c r="E13" s="52"/>
+      <c r="F13" s="52"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="56"/>
-      <c r="C14" s="56"/>
-      <c r="D14" s="56"/>
-      <c r="E14" s="56"/>
-      <c r="F14" s="56"/>
+      <c r="B14" s="51"/>
+      <c r="C14" s="51"/>
+      <c r="D14" s="51"/>
+      <c r="E14" s="51"/>
+      <c r="F14" s="51"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="24" t="s">
+      <c r="A15" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="53"/>
-      <c r="C15" s="53"/>
-      <c r="D15" s="53"/>
-      <c r="E15" s="53"/>
-      <c r="F15" s="53"/>
+      <c r="B15" s="52"/>
+      <c r="C15" s="52"/>
+      <c r="D15" s="52"/>
+      <c r="E15" s="52"/>
+      <c r="F15" s="52"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="56"/>
-      <c r="C16" s="56"/>
-      <c r="D16" s="56"/>
-      <c r="E16" s="56"/>
-      <c r="F16" s="56"/>
+      <c r="B16" s="51"/>
+      <c r="C16" s="51"/>
+      <c r="D16" s="51"/>
+      <c r="E16" s="51"/>
+      <c r="F16" s="51"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="24" t="s">
+      <c r="A17" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="53"/>
-      <c r="C17" s="53"/>
-      <c r="D17" s="53"/>
-      <c r="E17" s="53"/>
-      <c r="F17" s="53"/>
+      <c r="B17" s="52"/>
+      <c r="C17" s="52"/>
+      <c r="D17" s="52"/>
+      <c r="E17" s="52"/>
+      <c r="F17" s="52"/>
     </row>
     <row r="18" spans="1:6" ht="6.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="12"/>
-      <c r="B18" s="13"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-    </row>
-    <row r="19" spans="1:6" s="15" customFormat="1" ht="6.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="14"/>
-    </row>
-    <row r="20" spans="1:6" ht="13" x14ac:dyDescent="0.3">
-      <c r="A20" s="10" t="s">
-        <v>43</v>
+      <c r="A18" s="10"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+    </row>
+    <row r="19" spans="1:6" s="13" customFormat="1" ht="6.65" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="12"/>
+    </row>
+    <row r="20" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A20" s="43" t="s">
+        <v>38</v>
       </c>
       <c r="B20" s="6"/>
       <c r="C20" s="2"/>
@@ -3454,7 +3464,7 @@
         <v>26</v>
       </c>
       <c r="B21" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -3462,213 +3472,205 @@
         <v>27</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="6.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="12"/>
-      <c r="B23" s="13"/>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
+      <c r="A23" s="10"/>
+      <c r="B23" s="11"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="C24" s="2"/>
     </row>
-    <row r="25" spans="1:6" s="15" customFormat="1" ht="13" x14ac:dyDescent="0.3">
-      <c r="A25" s="16" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="B26" s="18"/>
-      <c r="C26" s="57" t="s">
-        <v>40</v>
-      </c>
-      <c r="D26" s="57"/>
-      <c r="E26" s="57"/>
-      <c r="F26" s="57"/>
-    </row>
-    <row r="27" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="B27" s="20"/>
-      <c r="C27" s="57"/>
-      <c r="D27" s="57"/>
-      <c r="E27" s="57"/>
-      <c r="F27" s="57"/>
-    </row>
-    <row r="28" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="17" t="s">
-        <v>118</v>
-      </c>
-      <c r="B28" s="20" t="s">
+    <row r="25" spans="1:6" s="13" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A25" s="44" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="B26" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="C28" s="57" t="s">
-        <v>120</v>
-      </c>
-      <c r="D28" s="57"/>
-      <c r="E28" s="57"/>
-      <c r="F28" s="57"/>
-    </row>
-    <row r="29" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="14" t="s">
-        <v>119</v>
-      </c>
-      <c r="B29" s="18" t="s">
+      <c r="C26" s="53" t="s">
+        <v>114</v>
+      </c>
+      <c r="D26" s="53"/>
+      <c r="E26" s="53"/>
+      <c r="F26" s="53"/>
+    </row>
+    <row r="27" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="B27" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="C29" s="57"/>
-      <c r="D29" s="57"/>
-      <c r="E29" s="57"/>
-      <c r="F29" s="57"/>
-    </row>
-    <row r="30" spans="1:6" ht="6.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="12"/>
-      <c r="B30" s="13"/>
-      <c r="C30" s="13"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
-    </row>
-    <row r="31" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="17"/>
-      <c r="B31" s="20"/>
-      <c r="C31" s="19"/>
-    </row>
-    <row r="32" spans="1:6" ht="13" x14ac:dyDescent="0.3">
-      <c r="A32" s="10" t="s">
+      <c r="C27" s="53"/>
+      <c r="D27" s="53"/>
+      <c r="E27" s="53"/>
+      <c r="F27" s="53"/>
+    </row>
+    <row r="28" spans="1:6" ht="6.65" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="10"/>
+      <c r="B28" s="11"/>
+      <c r="C28" s="11"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="11"/>
+      <c r="F28" s="11"/>
+    </row>
+    <row r="29" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="14"/>
+      <c r="B29" s="17"/>
+      <c r="C29" s="16"/>
+    </row>
+    <row r="30" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A30" s="43" t="s">
         <v>23</v>
       </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B31" s="6"/>
+      <c r="C31" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B32" s="5"/>
+      <c r="C32" s="2"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B33" s="6"/>
+        <v>101</v>
+      </c>
+      <c r="B33" s="5"/>
       <c r="C33" s="2" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B34" s="5"/>
-      <c r="C34" s="2"/>
+      <c r="C34" s="2" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B35" s="5"/>
       <c r="C35" s="2" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="B36" s="5"/>
-      <c r="C36" s="2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="B37" s="5"/>
-      <c r="C37" s="2" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" ht="6.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="12"/>
-      <c r="B38" s="13"/>
-      <c r="C38" s="13"/>
-      <c r="D38" s="13"/>
-      <c r="E38" s="13"/>
-      <c r="F38" s="13"/>
-    </row>
-    <row r="40" spans="1:9" ht="13" x14ac:dyDescent="0.3">
-      <c r="A40" s="11" t="s">
-        <v>58</v>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="6.65" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="10"/>
+      <c r="B36" s="11"/>
+      <c r="C36" s="11"/>
+      <c r="D36" s="11"/>
+      <c r="E36" s="11"/>
+      <c r="F36" s="11"/>
+    </row>
+    <row r="38" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A38" s="45" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B39" s="7"/>
+      <c r="C39" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B40" s="7"/>
+      <c r="C40" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B41" s="7"/>
+        <v>39</v>
+      </c>
       <c r="C41" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B42" s="7"/>
-      <c r="C42" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" ht="6.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="12"/>
-      <c r="B44" s="13"/>
-      <c r="C44" s="13"/>
-      <c r="D44" s="13"/>
-      <c r="E44" s="13"/>
-      <c r="F44" s="13"/>
-    </row>
-    <row r="46" spans="1:9" ht="13" x14ac:dyDescent="0.3">
-      <c r="A46" s="11" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" ht="13" x14ac:dyDescent="0.3">
-      <c r="A47" s="21" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="6.65" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="10"/>
+      <c r="B42" s="11"/>
+      <c r="C42" s="11"/>
+      <c r="D42" s="11"/>
+      <c r="E42" s="11"/>
+      <c r="F42" s="11"/>
+    </row>
+    <row r="44" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A44" s="45" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="13" x14ac:dyDescent="0.3">
+      <c r="A45" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="B47" s="22" t="s">
+      <c r="B45" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C47" s="23" t="s">
+      <c r="C45" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="D47" s="23" t="s">
+      <c r="D45" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="E47" s="23" t="s">
+      <c r="E45" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="F47" s="23" t="s">
+      <c r="F45" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="G47" s="25"/>
-      <c r="H47" s="25"/>
-      <c r="I47" s="1"/>
+      <c r="I45" s="1"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" s="6"/>
+      <c r="B46" s="6"/>
+      <c r="D46" s="7"/>
+      <c r="E46" s="6"/>
+      <c r="F46" s="5"/>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" s="6"/>
+      <c r="B47" s="5"/>
+      <c r="C47" s="2"/>
+      <c r="D47" s="7"/>
+      <c r="E47" s="6"/>
+      <c r="F47" s="5"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="6"/>
-      <c r="B48" s="6"/>
+      <c r="B48" s="5"/>
+      <c r="C48" s="2"/>
       <c r="D48" s="7"/>
       <c r="E48" s="6"/>
       <c r="F48" s="5"/>
@@ -3683,19 +3685,17 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="6"/>
-      <c r="B50" s="5"/>
-      <c r="C50" s="2"/>
+      <c r="B50" s="6"/>
       <c r="D50" s="7"/>
       <c r="E50" s="6"/>
-      <c r="F50" s="5"/>
+      <c r="F50" s="6"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="6"/>
-      <c r="B51" s="5"/>
-      <c r="C51" s="2"/>
+      <c r="B51" s="6"/>
       <c r="D51" s="7"/>
       <c r="E51" s="6"/>
-      <c r="F51" s="5"/>
+      <c r="F51" s="6"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="6"/>
@@ -4510,14 +4510,12 @@
       <c r="F167" s="6"/>
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A168" s="6"/>
       <c r="B168" s="6"/>
       <c r="D168" s="7"/>
       <c r="E168" s="6"/>
       <c r="F168" s="6"/>
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A169" s="6"/>
       <c r="B169" s="6"/>
       <c r="D169" s="7"/>
       <c r="E169" s="6"/>
@@ -4650,13 +4648,11 @@
       <c r="F190" s="6"/>
     </row>
     <row r="191" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B191" s="6"/>
       <c r="D191" s="7"/>
       <c r="E191" s="6"/>
       <c r="F191" s="6"/>
     </row>
     <row r="192" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B192" s="6"/>
       <c r="D192" s="7"/>
       <c r="E192" s="6"/>
       <c r="F192" s="6"/>
@@ -5967,12 +5963,10 @@
       <c r="F453" s="6"/>
     </row>
     <row r="454" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D454" s="7"/>
       <c r="E454" s="6"/>
       <c r="F454" s="6"/>
     </row>
     <row r="455" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D455" s="7"/>
       <c r="E455" s="6"/>
       <c r="F455" s="6"/>
     </row>
@@ -6404,17 +6398,8 @@
       <c r="E562" s="6"/>
       <c r="F562" s="6"/>
     </row>
-    <row r="563" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E563" s="6"/>
-      <c r="F563" s="6"/>
-    </row>
-    <row r="564" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E564" s="6"/>
-      <c r="F564" s="6"/>
-    </row>
   </sheetData>
-  <mergeCells count="16">
-    <mergeCell ref="C28:F29"/>
+  <mergeCells count="15">
     <mergeCell ref="C26:F27"/>
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="C2:F2"/>
@@ -6431,27 +6416,22 @@
     <mergeCell ref="B10:F10"/>
     <mergeCell ref="B11:F11"/>
   </mergeCells>
-  <phoneticPr fontId="5" type="noConversion"/>
-  <conditionalFormatting sqref="D48:D455">
-    <cfRule type="expression" dxfId="9" priority="3">
-      <formula>($B$41/$D48)&gt;(0.5*$B$42)</formula>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <conditionalFormatting sqref="D46:D453">
+    <cfRule type="expression" dxfId="6" priority="3">
+      <formula>($B$39/$D46)&gt;(0.5*$B$40)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B3 B21:B22 B33:B37 B41:B43">
-    <cfRule type="containsBlanks" dxfId="8" priority="2">
+  <conditionalFormatting sqref="B2:B3 B21:B22 B31:B35 B39:B41 B26:B27">
+    <cfRule type="containsBlanks" dxfId="5" priority="2">
       <formula>LEN(TRIM(B2))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B26:B29">
-    <cfRule type="containsBlanks" dxfId="7" priority="1">
-      <formula>LEN(TRIM(B26))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B41:B42" xr:uid="{1FDB8583-4725-454C-B804-F0E3C49A8048}">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B39:B40" xr:uid="{1FDB8583-4725-454C-B804-F0E3C49A8048}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Slot must be between 1 and 11" sqref="B31 B26:B28" xr:uid="{A1CCD96F-92EF-46C5-BC01-61873CD50A4F}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Slot must be between 1 and 11" sqref="B29 B26" xr:uid="{A1CCD96F-92EF-46C5-BC01-61873CD50A4F}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="256" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -6481,10 +6461,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{547A22CE-6B5B-419C-B571-1556B7859EB9}">
-  <dimension ref="A1:J587"/>
+  <dimension ref="A1:J586"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView topLeftCell="A43" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -6499,31 +6479,31 @@
     <col min="9" max="9" width="20.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="14" x14ac:dyDescent="0.3">
-      <c r="A1" s="36" t="s">
-        <v>112</v>
-      </c>
-      <c r="B1" s="35" t="s">
-        <v>161</v>
-      </c>
-      <c r="C1" s="28" t="s">
-        <v>45</v>
-      </c>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
+    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.4">
+      <c r="A1" s="84" t="s">
+        <v>106</v>
+      </c>
+      <c r="B1" s="85" t="s">
+        <v>158</v>
+      </c>
+      <c r="C1" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
     </row>
     <row r="2" spans="1:7" ht="13" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="3"/>
-      <c r="C2" s="28" t="s">
-        <v>55</v>
-      </c>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
+      <c r="C2" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -6536,20 +6516,20 @@
       <c r="A4" s="2"/>
     </row>
     <row r="5" spans="1:7" ht="6.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="12"/>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
+      <c r="A5" s="10"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
     </row>
     <row r="6" spans="1:7" ht="13" x14ac:dyDescent="0.3">
-      <c r="A6" s="26" t="s">
-        <v>42</v>
+      <c r="A6" s="23" t="s">
+        <v>37</v>
       </c>
       <c r="B6" s="55" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C6" s="55"/>
       <c r="D6" s="55"/>
@@ -6558,143 +6538,143 @@
       <c r="G6" s="55"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="53"/>
-      <c r="C7" s="53"/>
-      <c r="D7" s="53"/>
-      <c r="E7" s="53"/>
-      <c r="F7" s="53"/>
-      <c r="G7" s="53"/>
+      <c r="B7" s="52"/>
+      <c r="C7" s="52"/>
+      <c r="D7" s="52"/>
+      <c r="E7" s="52"/>
+      <c r="F7" s="52"/>
+      <c r="G7" s="52"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="56"/>
-      <c r="C8" s="56"/>
-      <c r="D8" s="56"/>
-      <c r="E8" s="56"/>
-      <c r="F8" s="56"/>
-      <c r="G8" s="56"/>
+      <c r="B8" s="51"/>
+      <c r="C8" s="51"/>
+      <c r="D8" s="51"/>
+      <c r="E8" s="51"/>
+      <c r="F8" s="51"/>
+      <c r="G8" s="51"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="24" t="s">
+      <c r="A9" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="53"/>
-      <c r="C9" s="53"/>
-      <c r="D9" s="53"/>
-      <c r="E9" s="53"/>
-      <c r="F9" s="53"/>
-      <c r="G9" s="53"/>
+      <c r="B9" s="52"/>
+      <c r="C9" s="52"/>
+      <c r="D9" s="52"/>
+      <c r="E9" s="52"/>
+      <c r="F9" s="52"/>
+      <c r="G9" s="52"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="56"/>
-      <c r="C10" s="56"/>
-      <c r="D10" s="56"/>
-      <c r="E10" s="56"/>
-      <c r="F10" s="56"/>
-      <c r="G10" s="56"/>
+      <c r="B10" s="51"/>
+      <c r="C10" s="51"/>
+      <c r="D10" s="51"/>
+      <c r="E10" s="51"/>
+      <c r="F10" s="51"/>
+      <c r="G10" s="51"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="24" t="s">
+      <c r="A11" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="53"/>
-      <c r="C11" s="53"/>
-      <c r="D11" s="53"/>
-      <c r="E11" s="53"/>
-      <c r="F11" s="53"/>
-      <c r="G11" s="53"/>
+      <c r="B11" s="52"/>
+      <c r="C11" s="52"/>
+      <c r="D11" s="52"/>
+      <c r="E11" s="52"/>
+      <c r="F11" s="52"/>
+      <c r="G11" s="52"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="56"/>
-      <c r="C12" s="56"/>
-      <c r="D12" s="56"/>
-      <c r="E12" s="56"/>
-      <c r="F12" s="56"/>
-      <c r="G12" s="56"/>
+      <c r="B12" s="51"/>
+      <c r="C12" s="51"/>
+      <c r="D12" s="51"/>
+      <c r="E12" s="51"/>
+      <c r="F12" s="51"/>
+      <c r="G12" s="51"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="24" t="s">
+      <c r="A13" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="53"/>
-      <c r="C13" s="53"/>
-      <c r="D13" s="53"/>
-      <c r="E13" s="53"/>
-      <c r="F13" s="53"/>
-      <c r="G13" s="53"/>
+      <c r="B13" s="52"/>
+      <c r="C13" s="52"/>
+      <c r="D13" s="52"/>
+      <c r="E13" s="52"/>
+      <c r="F13" s="52"/>
+      <c r="G13" s="52"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="56"/>
-      <c r="C14" s="56"/>
-      <c r="D14" s="56"/>
-      <c r="E14" s="56"/>
-      <c r="F14" s="56"/>
-      <c r="G14" s="56"/>
+      <c r="B14" s="51"/>
+      <c r="C14" s="51"/>
+      <c r="D14" s="51"/>
+      <c r="E14" s="51"/>
+      <c r="F14" s="51"/>
+      <c r="G14" s="51"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="24" t="s">
+      <c r="A15" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="53"/>
-      <c r="C15" s="53"/>
-      <c r="D15" s="53"/>
-      <c r="E15" s="53"/>
-      <c r="F15" s="53"/>
-      <c r="G15" s="53"/>
+      <c r="B15" s="52"/>
+      <c r="C15" s="52"/>
+      <c r="D15" s="52"/>
+      <c r="E15" s="52"/>
+      <c r="F15" s="52"/>
+      <c r="G15" s="52"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="56"/>
-      <c r="C16" s="56"/>
-      <c r="D16" s="56"/>
-      <c r="E16" s="56"/>
-      <c r="F16" s="56"/>
-      <c r="G16" s="56"/>
+      <c r="B16" s="51"/>
+      <c r="C16" s="51"/>
+      <c r="D16" s="51"/>
+      <c r="E16" s="51"/>
+      <c r="F16" s="51"/>
+      <c r="G16" s="51"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="24" t="s">
+      <c r="A17" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="53"/>
-      <c r="C17" s="53"/>
-      <c r="D17" s="53"/>
-      <c r="E17" s="53"/>
-      <c r="F17" s="53"/>
-      <c r="G17" s="53"/>
+      <c r="B17" s="52"/>
+      <c r="C17" s="52"/>
+      <c r="D17" s="52"/>
+      <c r="E17" s="52"/>
+      <c r="F17" s="52"/>
+      <c r="G17" s="52"/>
     </row>
     <row r="18" spans="1:7" ht="6.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="12"/>
-      <c r="B18" s="13"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
-    </row>
-    <row r="19" spans="1:7" s="15" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="14"/>
-    </row>
-    <row r="20" spans="1:7" ht="13" x14ac:dyDescent="0.25">
-      <c r="A20" s="59" t="s">
-        <v>43</v>
-      </c>
-      <c r="B20" s="59"/>
+      <c r="A18" s="10"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+    </row>
+    <row r="19" spans="1:7" s="13" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="12"/>
+    </row>
+    <row r="20" spans="1:7" ht="15.5" x14ac:dyDescent="0.25">
+      <c r="A20" s="83" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="83"/>
       <c r="C20" s="6"/>
       <c r="D20" s="2"/>
     </row>
@@ -6703,7 +6683,7 @@
         <v>26</v>
       </c>
       <c r="B21" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -6711,447 +6691,438 @@
         <v>27</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C22" s="2"/>
     </row>
     <row r="23" spans="1:7" ht="6.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="12"/>
-      <c r="B23" s="13"/>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
+      <c r="A23" s="10"/>
+      <c r="B23" s="11"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="D24" s="2"/>
     </row>
-    <row r="25" spans="1:7" s="15" customFormat="1" ht="13" x14ac:dyDescent="0.3">
-      <c r="A25" s="16" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="B26" s="18"/>
-      <c r="C26" s="30" t="s">
-        <v>40</v>
-      </c>
-      <c r="E26" s="30"/>
-      <c r="F26" s="30"/>
-      <c r="G26" s="30"/>
-    </row>
-    <row r="27" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="B27" s="20"/>
-      <c r="C27" s="30" t="s">
-        <v>41</v>
-      </c>
-      <c r="E27" s="30"/>
-      <c r="F27" s="30"/>
-      <c r="G27" s="30"/>
-    </row>
-    <row r="28" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="17" t="s">
-        <v>118</v>
-      </c>
-      <c r="B28" s="20" t="s">
+    <row r="25" spans="1:7" s="13" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A25" s="44" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="B26" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="C28" s="57" t="s">
-        <v>120</v>
-      </c>
-      <c r="D28" s="57"/>
-      <c r="E28" s="57"/>
-      <c r="F28" s="57"/>
-    </row>
-    <row r="29" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="14" t="s">
-        <v>119</v>
-      </c>
-      <c r="B29" s="18" t="s">
+      <c r="C26" s="53" t="s">
+        <v>114</v>
+      </c>
+      <c r="D26" s="53"/>
+      <c r="E26" s="53"/>
+      <c r="F26" s="53"/>
+    </row>
+    <row r="27" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="B27" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="C29" s="57"/>
-      <c r="D29" s="57"/>
-      <c r="E29" s="57"/>
-      <c r="F29" s="57"/>
-    </row>
-    <row r="30" spans="1:7" ht="6.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="12"/>
-      <c r="B30" s="13"/>
-      <c r="C30" s="13"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="13"/>
-    </row>
-    <row r="31" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="17"/>
-      <c r="B31" s="20"/>
-      <c r="C31" s="20"/>
-      <c r="D31" s="19"/>
-    </row>
-    <row r="32" spans="1:7" ht="13" x14ac:dyDescent="0.3">
-      <c r="A32" s="60" t="s">
+      <c r="C27" s="53"/>
+      <c r="D27" s="53"/>
+      <c r="E27" s="53"/>
+      <c r="F27" s="53"/>
+    </row>
+    <row r="28" spans="1:7" ht="6.65" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="10"/>
+      <c r="B28" s="11"/>
+      <c r="C28" s="11"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="11"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="11"/>
+    </row>
+    <row r="29" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="14"/>
+      <c r="B29" s="17"/>
+      <c r="C29" s="17"/>
+      <c r="D29" s="16"/>
+    </row>
+    <row r="30" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A30" s="82" t="s">
         <v>23</v>
       </c>
-      <c r="B32" s="60"/>
-      <c r="C32" s="60"/>
+      <c r="B30" s="82"/>
+      <c r="C30" s="82"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="2"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B32" s="5"/>
+      <c r="C32" s="2"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B33" s="6"/>
-      <c r="C33" s="6"/>
-      <c r="D33" s="2"/>
+        <v>101</v>
+      </c>
+      <c r="B33" s="5"/>
+      <c r="C33" s="2" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B34" s="5"/>
-      <c r="C34" s="2"/>
+      <c r="C34" s="2" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B35" s="5"/>
       <c r="C35" s="2" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>96</v>
+        <v>55</v>
       </c>
       <c r="B36" s="5"/>
-      <c r="C36" s="2" t="s">
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+    </row>
+    <row r="37" spans="1:4" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="74"/>
+      <c r="B37" s="75"/>
+      <c r="C37" s="76"/>
+      <c r="D37" s="2"/>
+    </row>
+    <row r="38" spans="1:4" ht="13.5" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="80" t="s">
+        <v>103</v>
+      </c>
+      <c r="B38" s="81" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="B37" s="5"/>
-      <c r="C37" s="2" t="s">
+      <c r="C38" s="77" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
+      <c r="D38" s="72"/>
+    </row>
+    <row r="39" spans="1:4" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="27" t="s">
+        <v>70</v>
+      </c>
+      <c r="B39" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="C39" s="78"/>
+      <c r="D39" s="72"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="B40" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="C40" s="78"/>
+      <c r="D40" s="72"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="27" t="s">
+        <v>72</v>
+      </c>
+      <c r="B41" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="C41" s="78"/>
+      <c r="D41" s="72"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="B42" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="C42" s="78"/>
+      <c r="D42" s="72"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="27" t="s">
+        <v>74</v>
+      </c>
+      <c r="B43" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="C43" s="78"/>
+      <c r="D43" s="72"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="27" t="s">
+        <v>75</v>
+      </c>
+      <c r="B44" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="C44" s="78"/>
+      <c r="D44" s="72"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="B45" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="C45" s="78"/>
+      <c r="D45" s="72"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="27" t="s">
+        <v>77</v>
+      </c>
+      <c r="B46" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="C46" s="78"/>
+      <c r="D46" s="72"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="27" t="s">
+        <v>78</v>
+      </c>
+      <c r="B47" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="B38" s="5"/>
-      <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="3"/>
-      <c r="B39" s="5"/>
-      <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="B40" s="5" t="s">
+      <c r="C47" s="78"/>
+      <c r="D47" s="72"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="B48" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="C48" s="78"/>
+      <c r="D48" s="72"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" s="27" t="s">
+        <v>80</v>
+      </c>
+      <c r="B49" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="C49" s="78"/>
+      <c r="D49" s="72"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="B50" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="C50" s="78"/>
+      <c r="D50" s="72"/>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" s="27" t="s">
+        <v>82</v>
+      </c>
+      <c r="B51" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="C51" s="78"/>
+      <c r="D51" s="72"/>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" s="27" t="s">
+        <v>83</v>
+      </c>
+      <c r="B52" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="C52" s="78"/>
+      <c r="D52" s="72"/>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" s="27" t="s">
+        <v>84</v>
+      </c>
+      <c r="B53" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="C53" s="78"/>
+      <c r="D53" s="72"/>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="B54" s="28" t="s">
+        <v>67</v>
+      </c>
+      <c r="C54" s="78"/>
+      <c r="D54" s="72"/>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" s="27" t="s">
+        <v>86</v>
+      </c>
+      <c r="B55" s="28" t="s">
+        <v>68</v>
+      </c>
+      <c r="C55" s="78"/>
+      <c r="D55" s="72"/>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" s="27" t="s">
+        <v>89</v>
+      </c>
+      <c r="B56" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="C56" s="78"/>
+      <c r="D56" s="72"/>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="B57" s="28" t="s">
         <v>110</v>
       </c>
-      <c r="C40" s="2"/>
-      <c r="D40" s="2"/>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="33" t="s">
-        <v>75</v>
-      </c>
-      <c r="B41" s="34" t="s">
-        <v>2</v>
-      </c>
-      <c r="C41" s="58" t="s">
+      <c r="C57" s="78"/>
+      <c r="D57" s="72"/>
+    </row>
+    <row r="58" spans="1:7" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="68" t="s">
+        <v>88</v>
+      </c>
+      <c r="B58" s="69" t="s">
         <v>111</v>
       </c>
-      <c r="D41" s="2"/>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="33" t="s">
-        <v>76</v>
-      </c>
-      <c r="B42" s="34" t="s">
-        <v>29</v>
-      </c>
-      <c r="C42" s="58"/>
-      <c r="D42" s="2"/>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="33" t="s">
-        <v>77</v>
-      </c>
-      <c r="B43" s="34" t="s">
-        <v>49</v>
-      </c>
-      <c r="C43" s="58"/>
-      <c r="D43" s="2"/>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="33" t="s">
-        <v>78</v>
-      </c>
-      <c r="B44" s="34" t="s">
-        <v>50</v>
-      </c>
-      <c r="C44" s="58"/>
-      <c r="D44" s="2"/>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="33" t="s">
-        <v>79</v>
-      </c>
-      <c r="B45" s="34" t="s">
-        <v>61</v>
-      </c>
-      <c r="C45" s="58"/>
-      <c r="D45" s="2"/>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="33" t="s">
-        <v>80</v>
-      </c>
-      <c r="B46" s="34" t="s">
-        <v>62</v>
-      </c>
-      <c r="C46" s="58"/>
-      <c r="D46" s="2"/>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="33" t="s">
-        <v>81</v>
-      </c>
-      <c r="B47" s="34" t="s">
-        <v>63</v>
-      </c>
-      <c r="C47" s="58"/>
-      <c r="D47" s="2"/>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="33" t="s">
-        <v>82</v>
-      </c>
-      <c r="B48" s="34" t="s">
-        <v>64</v>
-      </c>
-      <c r="C48" s="58"/>
-      <c r="D48" s="2"/>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="33" t="s">
-        <v>83</v>
-      </c>
-      <c r="B49" s="34" t="s">
-        <v>65</v>
-      </c>
-      <c r="C49" s="58"/>
-      <c r="D49" s="2"/>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="33" t="s">
-        <v>84</v>
-      </c>
-      <c r="B50" s="34" t="s">
-        <v>66</v>
-      </c>
-      <c r="C50" s="58"/>
-      <c r="D50" s="2"/>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="33" t="s">
-        <v>85</v>
-      </c>
-      <c r="B51" s="34" t="s">
-        <v>67</v>
-      </c>
-      <c r="C51" s="58"/>
-      <c r="D51" s="2"/>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="33" t="s">
-        <v>86</v>
-      </c>
-      <c r="B52" s="34" t="s">
-        <v>68</v>
-      </c>
-      <c r="C52" s="58"/>
-      <c r="D52" s="2"/>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="33" t="s">
-        <v>87</v>
-      </c>
-      <c r="B53" s="34" t="s">
-        <v>69</v>
-      </c>
-      <c r="C53" s="58"/>
-      <c r="D53" s="2"/>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" s="33" t="s">
-        <v>88</v>
-      </c>
-      <c r="B54" s="34" t="s">
-        <v>70</v>
-      </c>
-      <c r="C54" s="58"/>
-      <c r="D54" s="2"/>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" s="33" t="s">
-        <v>89</v>
-      </c>
-      <c r="B55" s="34" t="s">
-        <v>71</v>
-      </c>
-      <c r="C55" s="58"/>
-      <c r="D55" s="2"/>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" s="33" t="s">
-        <v>90</v>
-      </c>
-      <c r="B56" s="34" t="s">
-        <v>72</v>
-      </c>
-      <c r="C56" s="58"/>
-      <c r="D56" s="2"/>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A57" s="33" t="s">
-        <v>91</v>
-      </c>
-      <c r="B57" s="34" t="s">
-        <v>73</v>
-      </c>
-      <c r="C57" s="58"/>
-      <c r="D57" s="2"/>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" s="33" t="s">
-        <v>94</v>
-      </c>
-      <c r="B58" s="34" t="s">
-        <v>74</v>
-      </c>
-      <c r="C58" s="58"/>
-      <c r="D58" s="2"/>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59" s="33" t="s">
-        <v>92</v>
-      </c>
-      <c r="B59" s="34" t="s">
-        <v>116</v>
-      </c>
-      <c r="C59" s="58"/>
-      <c r="D59" s="2"/>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A60" s="31" t="s">
-        <v>93</v>
-      </c>
-      <c r="B60" s="32" t="s">
-        <v>117</v>
-      </c>
-      <c r="C60" s="58"/>
-    </row>
-    <row r="61" spans="1:7" ht="6.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="12"/>
-      <c r="B61" s="13"/>
-      <c r="C61" s="13"/>
-      <c r="D61" s="13"/>
-      <c r="E61" s="13"/>
-      <c r="F61" s="13"/>
-      <c r="G61" s="13"/>
-    </row>
-    <row r="63" spans="1:7" ht="13" x14ac:dyDescent="0.3">
-      <c r="A63" s="11" t="s">
-        <v>58</v>
+      <c r="C58" s="79"/>
+      <c r="D58" s="73"/>
+    </row>
+    <row r="59" spans="1:7" s="70" customFormat="1" ht="13" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="71"/>
+      <c r="B59" s="71"/>
+      <c r="C59" s="71"/>
+    </row>
+    <row r="60" spans="1:7" ht="6.65" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="10"/>
+      <c r="B60" s="11"/>
+      <c r="C60" s="11"/>
+      <c r="D60" s="11"/>
+      <c r="E60" s="11"/>
+      <c r="F60" s="11"/>
+      <c r="G60" s="11"/>
+    </row>
+    <row r="62" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A62" s="45" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B63" s="7"/>
+      <c r="C63" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B64" s="7"/>
       <c r="C64" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A65" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B65" s="7"/>
-      <c r="C65" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A66" s="3"/>
-      <c r="C66" s="2"/>
-    </row>
-    <row r="67" spans="1:10" ht="6.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="12"/>
-      <c r="B67" s="13"/>
-      <c r="C67" s="13"/>
-      <c r="D67" s="13"/>
-      <c r="E67" s="13"/>
-      <c r="F67" s="13"/>
-      <c r="G67" s="13"/>
+      <c r="A65" s="3"/>
+      <c r="C65" s="2"/>
+    </row>
+    <row r="66" spans="1:10" ht="6.65" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="10"/>
+      <c r="B66" s="11"/>
+      <c r="C66" s="11"/>
+      <c r="D66" s="11"/>
+      <c r="E66" s="11"/>
+      <c r="F66" s="11"/>
+      <c r="G66" s="11"/>
+    </row>
+    <row r="68" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A68" s="45" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="69" spans="1:10" ht="13" x14ac:dyDescent="0.3">
-      <c r="A69" s="11" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="70" spans="1:10" ht="13" x14ac:dyDescent="0.3">
-      <c r="A70" s="21" t="s">
+      <c r="A69" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="B70" s="22" t="s">
+      <c r="B69" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C70" s="29" t="s">
-        <v>59</v>
-      </c>
-      <c r="D70" s="23" t="s">
+      <c r="C69" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="D69" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E70" s="23" t="s">
+      <c r="E69" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="F70" s="23" t="s">
+      <c r="F69" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="G70" s="23" t="s">
+      <c r="G69" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="H70" s="25"/>
-      <c r="I70" s="25"/>
-      <c r="J70" s="1"/>
+      <c r="H69" s="22"/>
+      <c r="I69" s="22"/>
+      <c r="J69" s="1"/>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A70" s="6"/>
+      <c r="B70" s="6"/>
+      <c r="C70" s="6"/>
+      <c r="E70" s="7"/>
+      <c r="F70" s="6"/>
+      <c r="G70" s="5"/>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="6"/>
-      <c r="B71" s="6"/>
-      <c r="C71" s="6"/>
+      <c r="B71" s="5"/>
+      <c r="C71" s="5"/>
+      <c r="D71" s="2"/>
       <c r="E71" s="7"/>
       <c r="F71" s="6"/>
       <c r="G71" s="5"/>
@@ -7176,12 +7147,11 @@
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="6"/>
-      <c r="B74" s="5"/>
-      <c r="C74" s="5"/>
-      <c r="D74" s="2"/>
+      <c r="B74" s="6"/>
+      <c r="C74" s="6"/>
       <c r="E74" s="7"/>
       <c r="F74" s="6"/>
-      <c r="G74" s="5"/>
+      <c r="G74" s="6"/>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="6"/>
@@ -8120,7 +8090,6 @@
       <c r="G191" s="6"/>
     </row>
     <row r="192" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A192" s="6"/>
       <c r="B192" s="6"/>
       <c r="C192" s="6"/>
       <c r="E192" s="7"/>
@@ -8282,8 +8251,6 @@
       <c r="G214" s="6"/>
     </row>
     <row r="215" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B215" s="6"/>
-      <c r="C215" s="6"/>
       <c r="E215" s="7"/>
       <c r="F215" s="6"/>
       <c r="G215" s="6"/>
@@ -9599,7 +9566,6 @@
       <c r="G477" s="6"/>
     </row>
     <row r="478" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E478" s="7"/>
       <c r="F478" s="6"/>
       <c r="G478" s="6"/>
     </row>
@@ -10035,19 +10001,15 @@
       <c r="F586" s="6"/>
       <c r="G586" s="6"/>
     </row>
-    <row r="587" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F587" s="6"/>
-      <c r="G587" s="6"/>
-    </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="C38:C58"/>
     <mergeCell ref="B6:G6"/>
     <mergeCell ref="B7:G7"/>
     <mergeCell ref="B8:G8"/>
     <mergeCell ref="B9:G9"/>
-    <mergeCell ref="C41:C60"/>
     <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A32:C32"/>
+    <mergeCell ref="A30:C30"/>
     <mergeCell ref="B16:G16"/>
     <mergeCell ref="B17:G17"/>
     <mergeCell ref="B10:G10"/>
@@ -10056,42 +10018,37 @@
     <mergeCell ref="B13:G13"/>
     <mergeCell ref="B14:G14"/>
     <mergeCell ref="B15:G15"/>
-    <mergeCell ref="C28:F29"/>
+    <mergeCell ref="C26:F27"/>
   </mergeCells>
-  <phoneticPr fontId="15" type="noConversion"/>
-  <conditionalFormatting sqref="E71:E478">
-    <cfRule type="expression" dxfId="6" priority="6">
-      <formula>($B$64/$E71)&gt;(0.5*$B$65)</formula>
+  <phoneticPr fontId="13" type="noConversion"/>
+  <conditionalFormatting sqref="E70:E477">
+    <cfRule type="expression" dxfId="4" priority="6">
+      <formula>($B$63/$E70)&gt;(0.5*$B$64)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B3 B21:B22 B33 B38">
-    <cfRule type="containsBlanks" dxfId="5" priority="5">
+  <conditionalFormatting sqref="B2:B3 B21:B22 B31 B36 B26:B27">
+    <cfRule type="containsBlanks" dxfId="3" priority="5">
       <formula>LEN(TRIM(B2))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B64:B65">
-    <cfRule type="containsBlanks" dxfId="4" priority="4">
-      <formula>LEN(TRIM(B64))=0</formula>
+  <conditionalFormatting sqref="B63:B64">
+    <cfRule type="containsBlanks" dxfId="2" priority="4">
+      <formula>LEN(TRIM(B63))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C71:C478">
-    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text=" ">
-      <formula>NOT(ISERROR(SEARCH(" ",C71)))</formula>
+  <conditionalFormatting sqref="C70:C477">
+    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text=" ">
+      <formula>NOT(ISERROR(SEARCH(" ",C70)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B34:B37">
-    <cfRule type="containsBlanks" dxfId="2" priority="2">
-      <formula>LEN(TRIM(B34))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B26:B29">
-    <cfRule type="containsBlanks" dxfId="1" priority="1">
-      <formula>LEN(TRIM(B26))=0</formula>
+  <conditionalFormatting sqref="B32:B35">
+    <cfRule type="containsBlanks" dxfId="0" priority="2">
+      <formula>LEN(TRIM(B32))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Slot must be between 1 and 11" sqref="B31:C31 B26:C27 B28" xr:uid="{518D2AD7-0BE3-4C3E-882D-CFABDAF43CEF}"/>
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B64:C65" xr:uid="{F7B8CC61-EB73-4AB1-89AA-99624CE8C7EC}">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Slot must be between 1 and 11" sqref="B29:C29 B26" xr:uid="{518D2AD7-0BE3-4C3E-882D-CFABDAF43CEF}"/>
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B63:C64" xr:uid="{F7B8CC61-EB73-4AB1-89AA-99624CE8C7EC}">
       <formula1>0</formula1>
     </dataValidation>
   </dataValidations>
@@ -10131,8 +10088,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CBCE2FF-AC7E-47F6-AFA7-5759B53B3059}">
   <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -10142,32 +10099,32 @@
     <col min="4" max="4" width="22.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="27" customFormat="1" ht="18" x14ac:dyDescent="0.4">
-      <c r="A1" s="61" t="s">
-        <v>57</v>
-      </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
+    <row r="1" spans="1:4" s="24" customFormat="1" ht="18" x14ac:dyDescent="0.4">
+      <c r="A1" s="66" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
     </row>
     <row r="2" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="9" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" s="8" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="8" t="s">
@@ -10176,7 +10133,7 @@
     </row>
     <row r="4" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A4" s="8" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
@@ -10186,52 +10143,52 @@
     </row>
     <row r="5" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A5" s="8" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
       <c r="D5" s="8" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="47" t="s">
-        <v>159</v>
-      </c>
-      <c r="B6" s="47" t="s">
-        <v>99</v>
+      <c r="A6" s="39" t="s">
+        <v>153</v>
+      </c>
+      <c r="B6" s="39" t="s">
+        <v>94</v>
       </c>
       <c r="C6" s="8"/>
       <c r="D6" s="8" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="47" t="s">
+      <c r="A7" s="39" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="47" t="s">
-        <v>54</v>
+      <c r="B7" s="39" t="s">
+        <v>49</v>
       </c>
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
     </row>
     <row r="8" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A8" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" s="8" t="s">
         <v>48</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>53</v>
       </c>
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
     </row>
     <row r="9" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A9" s="8" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C9" s="8"/>
       <c r="D9" s="8"/>
@@ -10241,7 +10198,7 @@
         <v>31</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
@@ -10251,27 +10208,27 @@
         <v>30</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
     </row>
     <row r="12" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A12" s="8" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
     </row>
     <row r="13" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A13" s="8" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="C13" s="8"/>
       <c r="D13" s="8"/>
@@ -10448,6 +10405,6 @@
     <mergeCell ref="A1:D1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fix rounding error and update template
</commit_message>
<xml_diff>
--- a/Docs/Opentrons Program Templates.xlsx
+++ b/Docs/Opentrons Program Templates.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://adminliveunc-my.sharepoint.com/personal/dennis_ad_unc_edu/Documents/Projects/Programs/Opentrons_Programs/Docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="75" documentId="8_{6CB10FB7-93AB-481A-8DDB-8A30EB088550}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{13B10F34-2402-4894-8D0A-1DFB72AF83BD}"/>
+  <xr:revisionPtr revIDLastSave="33" documentId="8_{EF6BFD9A-6ED8-462D-A0F5-E40DF4AE02BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4D86AF48-E1CA-4187-85D9-81F722AB1389}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="ddPCR" sheetId="5" r:id="rId1"/>
+    <sheet name="ddPCR" sheetId="6" r:id="rId1"/>
     <sheet name="Generic PCR" sheetId="2" r:id="rId2"/>
     <sheet name="Illumina Indexing" sheetId="4" r:id="rId3"/>
     <sheet name="Linked Values" sheetId="3" r:id="rId4"/>
@@ -22,22 +22,11 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Linked Values'!$A$2:$B$2</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="151">
   <si>
     <t>Source Well</t>
   </si>
@@ -318,9 +307,6 @@
     <t># Generic PCR Setup</t>
   </si>
   <si>
-    <t>opentrons_96_tiprack_20ul</t>
-  </si>
-  <si>
     <t>Pipette tips for p20</t>
   </si>
   <si>
@@ -360,9 +346,6 @@
     <t># Illumina Indexing</t>
   </si>
   <si>
-    <t>opentrons_24_tuberack_nest_0.5ml_screwcap</t>
-  </si>
-  <si>
     <t>vwrmicrocentrifugetube1.5ml_24_tuberack_1500ul</t>
   </si>
   <si>
@@ -387,9 +370,6 @@
     <t>opentrons_24_tuberack_generic_2ml_screwcap</t>
   </si>
   <si>
-    <t># Primers + Probes</t>
-  </si>
-  <si>
     <t>--Target_1</t>
   </si>
   <si>
@@ -420,36 +400,6 @@
     <t>--Target_10</t>
   </si>
   <si>
-    <t>--PositiveControl_1</t>
-  </si>
-  <si>
-    <t>--PositiveControl_2</t>
-  </si>
-  <si>
-    <t>--PositiveControl_3</t>
-  </si>
-  <si>
-    <t>--PositiveControl_4</t>
-  </si>
-  <si>
-    <t>--PositiveControl_5</t>
-  </si>
-  <si>
-    <t>--PositiveControl_6</t>
-  </si>
-  <si>
-    <t>--PositiveControl_7</t>
-  </si>
-  <si>
-    <t>--PositiveControl_8</t>
-  </si>
-  <si>
-    <t>--PositiveControl_9</t>
-  </si>
-  <si>
-    <t>--PositiveControl_10</t>
-  </si>
-  <si>
     <t>Sample Name</t>
   </si>
   <si>
@@ -465,12 +415,6 @@
     <t>--DilutionPlateSlot</t>
   </si>
   <si>
-    <t>--TargetVolume</t>
-  </si>
-  <si>
-    <t>2x or 4x</t>
-  </si>
-  <si>
     <t>2x</t>
   </si>
   <si>
@@ -483,27 +427,12 @@
     <t>--User</t>
   </si>
   <si>
-    <t>Slot,Well,Name with no spaces</t>
-  </si>
-  <si>
-    <t>Float, volume of primer, probe, BSA mixture.</t>
-  </si>
-  <si>
     <t># Target</t>
   </si>
   <si>
-    <t># Positive Control</t>
-  </si>
-  <si>
-    <t># There must be one positive control for each Target</t>
-  </si>
-  <si>
     <t>opentrons_96_filtertiprack_20ul</t>
   </si>
   <si>
-    <t># The positive control volume used is always the maximum volume allowed.</t>
-  </si>
-  <si>
     <t># First Pipette Tip</t>
   </si>
   <si>
@@ -516,10 +445,40 @@
     <t>Millimeters, float</t>
   </si>
   <si>
-    <t xml:space="preserve"> v0.4.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> v0.7.0</t>
+    <t>Generally leave as 2x</t>
+  </si>
+  <si>
+    <t>screwcap_24_tuberack_500ul</t>
+  </si>
+  <si>
+    <t>Targets should be here as well</t>
+  </si>
+  <si>
+    <t>Target Name</t>
+  </si>
+  <si>
+    <t>Float, volume of primer, probe, BSA and Supermix mixture per well.</t>
+  </si>
+  <si>
+    <t>--ReagentVolume</t>
+  </si>
+  <si>
+    <t>Volume in Tube</t>
+  </si>
+  <si>
+    <t># Reagents</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> v0.6.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> v0.7.1</t>
+  </si>
+  <si>
+    <t>0.5 mL Screw Cap Tubes</t>
+  </si>
+  <si>
+    <t>2 mL Screw Cap Tubes</t>
   </si>
 </sst>
 </file>
@@ -530,18 +489,11 @@
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yyyy;@"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -627,28 +579,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="12"/>
       <color theme="9" tint="-0.249977111117893"/>
       <name val="Arial"/>
@@ -686,8 +616,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -710,17 +644,6 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
@@ -765,15 +688,6 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -881,192 +795,187 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="8" fillId="8" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="15" fillId="5" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="7" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="17" fillId="6" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="15" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="19" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="8" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="9" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="180"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="7" fillId="6" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="20% - Accent4" xfId="2" builtinId="42"/>
-    <cellStyle name="Accent4" xfId="1" builtinId="41"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="22">
@@ -1139,6 +1048,69 @@
           <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1268,69 +1240,6 @@
       </fill>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1345,46 +1254,46 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{0AFC3E1F-23DC-4281-9692-1635ECE808ED}" name="Table14" displayName="Table14" ref="A81:F177" totalsRowShown="0" headerRowDxfId="21">
-  <autoFilter ref="A81:F177" xr:uid="{E9F71635-090B-4C48-B890-1CC5A8BA778F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{DED5D25C-9472-45DF-A5A9-7AE013ADEDBE}" name="Table145" displayName="Table145" ref="A63:F159" totalsRowShown="0" headerRowDxfId="13">
+  <autoFilter ref="A63:F159" xr:uid="{E9F71635-090B-4C48-B890-1CC5A8BA778F}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{1C94D97C-CFBE-4070-B57B-40D584ADAD4C}" name="# Source Slot"/>
-    <tableColumn id="2" xr3:uid="{7F951B2F-B449-4323-9BA7-A6CCBE2503A2}" name="Source Well"/>
-    <tableColumn id="3" xr3:uid="{92E3F929-8373-433B-85FD-B9AAAC53CEBC}" name="Sample Name"/>
-    <tableColumn id="4" xr3:uid="{591C18FD-B808-47C9-9CB4-E7688E5D4F2F}" name="Concentration ng/uL" dataDxfId="20"/>
-    <tableColumn id="5" xr3:uid="{D1888A8E-4AA2-4C96-A740-71BA0E6A02D8}" name="Target(s)" dataDxfId="19"/>
-    <tableColumn id="6" xr3:uid="{C4F4ADEA-237D-43B7-8280-EDDE7908D4FA}" name="Replicates" dataDxfId="18"/>
+    <tableColumn id="1" xr3:uid="{6612BCA6-F4EF-4AEA-9AD0-76196FD98128}" name="# Source Slot"/>
+    <tableColumn id="2" xr3:uid="{5F3EDDD0-EEFB-4C72-BFFB-FE7C21AD55A4}" name="Source Well"/>
+    <tableColumn id="3" xr3:uid="{C4F715B5-092C-4402-8CEE-00EA82DFB39D}" name="Sample Name"/>
+    <tableColumn id="4" xr3:uid="{84ACEE16-885F-421C-9A1E-F0D15E2C7A09}" name="Concentration ng/uL" dataDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{2188F77B-A461-4751-ADE0-A1432AFC9E78}" name="Target(s)" dataDxfId="11"/>
+    <tableColumn id="6" xr3:uid="{C1FA056C-8826-486C-B642-AB895FD3075E}" name="Replicates" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6E2D2C82-AED1-4EFD-B514-45C88869B632}" name="Table1" displayName="Table1" ref="A50:F458" totalsRowShown="0" headerRowDxfId="17">
-  <autoFilter ref="A50:F458" xr:uid="{E9F71635-090B-4C48-B890-1CC5A8BA778F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6E2D2C82-AED1-4EFD-B514-45C88869B632}" name="Table1" displayName="Table1" ref="A51:F459" totalsRowShown="0" headerRowDxfId="21">
+  <autoFilter ref="A51:F459" xr:uid="{E9F71635-090B-4C48-B890-1CC5A8BA778F}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{869EDE9B-E883-4A3E-BC84-177627B77820}" name="# Source Slot"/>
     <tableColumn id="2" xr3:uid="{BFF29CE8-BC36-441D-BF7C-4D3ECA705071}" name="Source Well"/>
     <tableColumn id="3" xr3:uid="{BE3B5A50-56B7-458D-A1B8-EA325514A953}" name="Sample"/>
-    <tableColumn id="4" xr3:uid="{51C9CB7B-3C83-4DF7-B90E-3B3B2F0517EB}" name="Concentration ng/uL" dataDxfId="16"/>
-    <tableColumn id="5" xr3:uid="{F1CA2FD2-DD2B-44E5-934D-9BDE08DCFF66}" name="Destination Slot" dataDxfId="15"/>
-    <tableColumn id="6" xr3:uid="{7F589CB2-9FD4-4968-8CE1-91953E95F345}" name="Destination Well" dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{51C9CB7B-3C83-4DF7-B90E-3B3B2F0517EB}" name="Concentration ng/uL" dataDxfId="20"/>
+    <tableColumn id="5" xr3:uid="{F1CA2FD2-DD2B-44E5-934D-9BDE08DCFF66}" name="Destination Slot" dataDxfId="19"/>
+    <tableColumn id="6" xr3:uid="{7F589CB2-9FD4-4968-8CE1-91953E95F345}" name="Destination Well" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4A1EA636-4A66-4384-BAA4-76D238021771}" name="Table13" displayName="Table13" ref="A72:G480" totalsRowShown="0" headerRowDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4A1EA636-4A66-4384-BAA4-76D238021771}" name="Table13" displayName="Table13" ref="A72:G480" totalsRowShown="0" headerRowDxfId="17">
   <autoFilter ref="A72:G480" xr:uid="{E9F71635-090B-4C48-B890-1CC5A8BA778F}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{F86BB3DB-CF90-48B8-8F35-E42977442672}" name="# Source Slot"/>
     <tableColumn id="2" xr3:uid="{C0F53F8F-C6A8-4F67-BF04-2D1C3AE40DC7}" name="Source Well"/>
     <tableColumn id="8" xr3:uid="{466B28CD-7413-41AF-A6D9-1A9460F0F6F4}" name="Index"/>
     <tableColumn id="3" xr3:uid="{FB50DE30-1861-4AAD-B46A-522A9F77B092}" name="Sample"/>
-    <tableColumn id="4" xr3:uid="{624B6C14-EDFA-405E-9149-7A4DAA0A5782}" name="Concentration ng/uL" dataDxfId="12"/>
-    <tableColumn id="5" xr3:uid="{A82E5DDD-FDEB-4967-8780-CF48E4C9A4DF}" name="Destination Slot" dataDxfId="11"/>
-    <tableColumn id="6" xr3:uid="{28DE797A-4F93-44BF-AC9A-BA038C116648}" name="Destination Well" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{624B6C14-EDFA-405E-9149-7A4DAA0A5782}" name="Concentration ng/uL" dataDxfId="16"/>
+    <tableColumn id="5" xr3:uid="{A82E5DDD-FDEB-4967-8780-CF48E4C9A4DF}" name="Destination Slot" dataDxfId="15"/>
+    <tableColumn id="6" xr3:uid="{28DE797A-4F93-44BF-AC9A-BA038C116648}" name="Destination Well" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1587,14 +1496,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A7A34B6-9524-4D9B-A744-B5E5EBB879BB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9EDFB13-CC9D-4AE8-A510-666896E1D552}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F255"/>
+  <dimension ref="A1:F237"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="I48" sqref="I48"/>
+    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7:F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1608,30 +1517,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.4">
-      <c r="A1" s="65" t="s">
-        <v>146</v>
-      </c>
-      <c r="B1" s="66" t="s">
-        <v>159</v>
-      </c>
-      <c r="C1" s="78" t="s">
+      <c r="A1" s="61" t="s">
+        <v>131</v>
+      </c>
+      <c r="B1" s="62" t="s">
+        <v>136</v>
+      </c>
+      <c r="C1" s="70" t="s">
         <v>40</v>
       </c>
-      <c r="D1" s="78"/>
-      <c r="E1" s="78"/>
-      <c r="F1" s="78"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
     </row>
     <row r="2" spans="1:6" ht="13" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>147</v>
+        <v>132</v>
       </c>
       <c r="B2" s="3"/>
-      <c r="C2" s="78" t="s">
+      <c r="C2" s="70" t="s">
         <v>50</v>
       </c>
-      <c r="D2" s="78"/>
-      <c r="E2" s="78"/>
-      <c r="F2" s="78"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -1654,123 +1563,123 @@
       <c r="A6" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="B6" s="79" t="s">
+      <c r="B6" s="71" t="s">
         <v>51</v>
       </c>
-      <c r="C6" s="79"/>
-      <c r="D6" s="79"/>
-      <c r="E6" s="79"/>
-      <c r="F6" s="79"/>
+      <c r="C6" s="71"/>
+      <c r="D6" s="71"/>
+      <c r="E6" s="71"/>
+      <c r="F6" s="71"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="77"/>
-      <c r="C7" s="77"/>
-      <c r="D7" s="77"/>
-      <c r="E7" s="77"/>
-      <c r="F7" s="77"/>
+      <c r="B7" s="69"/>
+      <c r="C7" s="69"/>
+      <c r="D7" s="69"/>
+      <c r="E7" s="69"/>
+      <c r="F7" s="69"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="80"/>
-      <c r="C8" s="80"/>
-      <c r="D8" s="80"/>
-      <c r="E8" s="80"/>
-      <c r="F8" s="80"/>
+      <c r="B8" s="72"/>
+      <c r="C8" s="72"/>
+      <c r="D8" s="72"/>
+      <c r="E8" s="72"/>
+      <c r="F8" s="72"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="77"/>
-      <c r="C9" s="77"/>
-      <c r="D9" s="77"/>
-      <c r="E9" s="77"/>
-      <c r="F9" s="77"/>
+      <c r="B9" s="69"/>
+      <c r="C9" s="69"/>
+      <c r="D9" s="69"/>
+      <c r="E9" s="69"/>
+      <c r="F9" s="69"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="80"/>
-      <c r="C10" s="80"/>
-      <c r="D10" s="80"/>
-      <c r="E10" s="80"/>
-      <c r="F10" s="80"/>
+      <c r="B10" s="72"/>
+      <c r="C10" s="72"/>
+      <c r="D10" s="72"/>
+      <c r="E10" s="72"/>
+      <c r="F10" s="72"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="77"/>
-      <c r="C11" s="77"/>
-      <c r="D11" s="77"/>
-      <c r="E11" s="77"/>
-      <c r="F11" s="77"/>
+      <c r="B11" s="69"/>
+      <c r="C11" s="69"/>
+      <c r="D11" s="69"/>
+      <c r="E11" s="69"/>
+      <c r="F11" s="69"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="80"/>
-      <c r="C12" s="80"/>
-      <c r="D12" s="80"/>
-      <c r="E12" s="80"/>
-      <c r="F12" s="80"/>
+      <c r="B12" s="72"/>
+      <c r="C12" s="72"/>
+      <c r="D12" s="72"/>
+      <c r="E12" s="72"/>
+      <c r="F12" s="72"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="77"/>
-      <c r="C13" s="77"/>
-      <c r="D13" s="77"/>
-      <c r="E13" s="77"/>
-      <c r="F13" s="77"/>
+      <c r="B13" s="69"/>
+      <c r="C13" s="69"/>
+      <c r="D13" s="69"/>
+      <c r="E13" s="69"/>
+      <c r="F13" s="69"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="80"/>
-      <c r="C14" s="80"/>
-      <c r="D14" s="80"/>
-      <c r="E14" s="80"/>
-      <c r="F14" s="80"/>
+      <c r="B14" s="72"/>
+      <c r="C14" s="72"/>
+      <c r="D14" s="72"/>
+      <c r="E14" s="72"/>
+      <c r="F14" s="72"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="77"/>
-      <c r="C15" s="77"/>
-      <c r="D15" s="77"/>
-      <c r="E15" s="77"/>
-      <c r="F15" s="77"/>
+      <c r="B15" s="69"/>
+      <c r="C15" s="69"/>
+      <c r="D15" s="69"/>
+      <c r="E15" s="69"/>
+      <c r="F15" s="69"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="80"/>
-      <c r="C16" s="80"/>
-      <c r="D16" s="80"/>
-      <c r="E16" s="80"/>
-      <c r="F16" s="80"/>
+      <c r="B16" s="72"/>
+      <c r="C16" s="72"/>
+      <c r="D16" s="72"/>
+      <c r="E16" s="72"/>
+      <c r="F16" s="72"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="77"/>
-      <c r="C17" s="77"/>
-      <c r="D17" s="77"/>
-      <c r="E17" s="77"/>
-      <c r="F17" s="77"/>
+      <c r="B17" s="69"/>
+      <c r="C17" s="69"/>
+      <c r="D17" s="69"/>
+      <c r="E17" s="69"/>
+      <c r="F17" s="69"/>
     </row>
     <row r="18" spans="1:6" ht="6.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="10"/>
@@ -1784,10 +1693,10 @@
       <c r="A19" s="12"/>
     </row>
     <row r="20" spans="1:6" s="8" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A20" s="43" t="s">
+      <c r="A20" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="B20" s="41"/>
+      <c r="B20" s="37"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
@@ -1820,58 +1729,58 @@
       <c r="A25" s="3"/>
       <c r="C25" s="2"/>
     </row>
-    <row r="26" spans="1:6" s="42" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A26" s="44" t="s">
-        <v>155</v>
+    <row r="26" spans="1:6" s="38" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A26" s="40" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="27" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="14" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B27" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="C27" s="81" t="s">
-        <v>114</v>
-      </c>
-      <c r="D27" s="81"/>
-      <c r="E27" s="81"/>
-      <c r="F27" s="81"/>
+      <c r="C27" s="73" t="s">
+        <v>112</v>
+      </c>
+      <c r="D27" s="73"/>
+      <c r="E27" s="73"/>
+      <c r="F27" s="73"/>
     </row>
     <row r="28" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B28" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="C28" s="81"/>
-      <c r="D28" s="81"/>
-      <c r="E28" s="81"/>
-      <c r="F28" s="81"/>
-    </row>
-    <row r="29" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="88" t="s">
-        <v>157</v>
-      </c>
-      <c r="B29" s="33">
-        <v>0.75</v>
-      </c>
-      <c r="C29" s="51" t="s">
-        <v>158</v>
-      </c>
-      <c r="D29" s="51"/>
-      <c r="E29" s="51"/>
-      <c r="F29" s="51"/>
+      <c r="C28" s="73"/>
+      <c r="D28" s="73"/>
+      <c r="E28" s="73"/>
+      <c r="F28" s="73"/>
+    </row>
+    <row r="29" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="64" t="s">
+        <v>137</v>
+      </c>
+      <c r="B29" s="85">
+        <v>1</v>
+      </c>
+      <c r="C29" s="65" t="s">
+        <v>138</v>
+      </c>
+      <c r="D29" s="65"/>
+      <c r="E29" s="65"/>
+      <c r="F29" s="65"/>
     </row>
     <row r="30" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="12"/>
       <c r="B30"/>
-      <c r="C30" s="52"/>
-      <c r="D30" s="52"/>
-      <c r="E30" s="52"/>
-      <c r="F30" s="52"/>
+      <c r="C30" s="66"/>
+      <c r="D30" s="66"/>
+      <c r="E30" s="66"/>
+      <c r="F30" s="66"/>
     </row>
     <row r="31" spans="1:6" ht="6.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="10"/>
@@ -1881,55 +1790,48 @@
       <c r="E31" s="11"/>
       <c r="F31" s="11"/>
     </row>
-    <row r="32" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="14"/>
-      <c r="B32" s="17"/>
-      <c r="C32" s="16"/>
-    </row>
     <row r="33" spans="1:6" s="8" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A33" s="43" t="s">
-        <v>23</v>
+      <c r="A33" s="41" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B34" s="6"/>
-      <c r="C34" s="2" t="s">
-        <v>100</v>
+        <v>127</v>
+      </c>
+      <c r="B34" s="29">
+        <v>9</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="B35" s="5"/>
-      <c r="C35" s="2"/>
+        <v>128</v>
+      </c>
+      <c r="B35" s="29">
+        <v>6</v>
+      </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="B36" s="5"/>
-      <c r="C36" s="2" t="s">
-        <v>99</v>
-      </c>
+      <c r="A36" s="3"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="B37" s="5"/>
-      <c r="C37" s="2"/>
+        <v>19</v>
+      </c>
+      <c r="B37" s="7"/>
+      <c r="C37" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="B38" s="5"/>
+        <v>21</v>
+      </c>
+      <c r="B38" s="7">
+        <v>25</v>
+      </c>
       <c r="C38" s="2" t="s">
-        <v>99</v>
+        <v>22</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -1945,315 +1847,335 @@
       <c r="F40" s="11"/>
     </row>
     <row r="42" spans="1:6" s="8" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A42" s="45" t="s">
-        <v>53</v>
+      <c r="A42" s="39" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="B43" s="30"/>
+        <v>28</v>
+      </c>
+      <c r="B43" s="6"/>
+      <c r="C43" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D43" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="B44" s="30"/>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="B45" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="C45" s="2" t="s">
+      <c r="C44" s="2" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="3"/>
+      <c r="A46" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B46" s="68"/>
+      <c r="C46" s="2"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B47" s="7"/>
+        <v>100</v>
+      </c>
+      <c r="B47" s="68"/>
       <c r="C47" s="2" t="s">
-        <v>20</v>
+        <v>98</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B48" s="7"/>
-      <c r="C48" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="3"/>
-      <c r="C49" s="2"/>
-    </row>
-    <row r="50" spans="1:6" ht="6.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="10"/>
-      <c r="B50" s="11"/>
-      <c r="C50" s="11"/>
-      <c r="D50" s="11"/>
-      <c r="E50" s="11"/>
-      <c r="F50" s="11"/>
-    </row>
-    <row r="52" spans="1:6" s="8" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A52" s="43" t="s">
+      <c r="A48" s="30"/>
+      <c r="B48" s="31"/>
+      <c r="C48" s="32"/>
+    </row>
+    <row r="49" spans="1:6" s="43" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+      <c r="A49" s="42" t="s">
+        <v>133</v>
+      </c>
+      <c r="B49" s="67" t="s">
+        <v>103</v>
+      </c>
+      <c r="C49" s="67" t="s">
+        <v>142</v>
+      </c>
+      <c r="D49" s="67" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="33" t="s">
+        <v>114</v>
+      </c>
+      <c r="B50" s="80"/>
+      <c r="C50" s="80"/>
+      <c r="D50" s="86"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="34" t="s">
+        <v>115</v>
+      </c>
+      <c r="B51" s="83"/>
+      <c r="C51" s="84"/>
+      <c r="D51" s="87"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="33" t="s">
         <v>116</v>
       </c>
+      <c r="B52" s="80"/>
+      <c r="C52" s="80"/>
+      <c r="D52" s="86"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>149</v>
-      </c>
+      <c r="A53" s="34" t="s">
+        <v>117</v>
+      </c>
+      <c r="B53" s="83"/>
+      <c r="C53" s="84"/>
+      <c r="D53" s="87"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="31"/>
-      <c r="B54" s="32"/>
-      <c r="C54" s="33"/>
-    </row>
-    <row r="55" spans="1:6" s="47" customFormat="1" ht="14" x14ac:dyDescent="0.3">
-      <c r="A55" s="46" t="s">
-        <v>150</v>
-      </c>
-      <c r="B55" s="76" t="s">
-        <v>148</v>
-      </c>
-      <c r="C55" s="76"/>
+      <c r="A54" s="33" t="s">
+        <v>118</v>
+      </c>
+      <c r="B54" s="80"/>
+      <c r="C54" s="80"/>
+      <c r="D54" s="86"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="34" t="s">
+        <v>119</v>
+      </c>
+      <c r="B55" s="83"/>
+      <c r="C55" s="84"/>
+      <c r="D55" s="87"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="34" t="s">
-        <v>117</v>
-      </c>
-      <c r="B56" s="73"/>
-      <c r="C56" s="73"/>
+      <c r="A56" s="33" t="s">
+        <v>120</v>
+      </c>
+      <c r="B56" s="80"/>
+      <c r="C56" s="80"/>
+      <c r="D56" s="86"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="35" t="s">
-        <v>118</v>
-      </c>
-      <c r="B57" s="74"/>
-      <c r="C57" s="75"/>
+      <c r="A57" s="34" t="s">
+        <v>121</v>
+      </c>
+      <c r="B57" s="83"/>
+      <c r="C57" s="84"/>
+      <c r="D57" s="87"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="34" t="s">
-        <v>119</v>
-      </c>
-      <c r="B58" s="73"/>
-      <c r="C58" s="73"/>
+      <c r="A58" s="33" t="s">
+        <v>122</v>
+      </c>
+      <c r="B58" s="80"/>
+      <c r="C58" s="80"/>
+      <c r="D58" s="86"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="35" t="s">
-        <v>120</v>
-      </c>
-      <c r="B59" s="74"/>
-      <c r="C59" s="75"/>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="34" t="s">
-        <v>121</v>
-      </c>
-      <c r="B60" s="73"/>
-      <c r="C60" s="73"/>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="35" t="s">
-        <v>122</v>
-      </c>
-      <c r="B61" s="74"/>
-      <c r="C61" s="75"/>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="34" t="s">
         <v>123</v>
       </c>
-      <c r="B62" s="73"/>
-      <c r="C62" s="73"/>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="35" t="s">
+      <c r="B59" s="81"/>
+      <c r="C59" s="82"/>
+      <c r="D59" s="88"/>
+    </row>
+    <row r="60" spans="1:6" ht="6.65" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="10"/>
+      <c r="B60" s="11"/>
+      <c r="C60" s="11"/>
+      <c r="D60" s="11"/>
+      <c r="E60" s="11"/>
+      <c r="F60" s="11"/>
+    </row>
+    <row r="62" spans="1:6" s="8" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A62" s="41" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" s="43" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+      <c r="A63" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="B63" s="45" t="s">
+        <v>0</v>
+      </c>
+      <c r="C63" s="46" t="s">
         <v>124</v>
       </c>
-      <c r="B63" s="74"/>
-      <c r="C63" s="75"/>
+      <c r="D63" s="46" t="s">
+        <v>4</v>
+      </c>
+      <c r="E63" s="46" t="s">
+        <v>125</v>
+      </c>
+      <c r="F63" s="46" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="34" t="s">
-        <v>125</v>
-      </c>
-      <c r="B64" s="73"/>
-      <c r="C64" s="73"/>
+      <c r="A64" s="6"/>
+      <c r="B64" s="68"/>
+      <c r="C64" s="2"/>
+      <c r="D64" s="7"/>
+      <c r="E64" s="6"/>
+      <c r="F64" s="68"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" s="36" t="s">
-        <v>126</v>
-      </c>
-      <c r="B65" s="70"/>
-      <c r="C65" s="71"/>
+      <c r="A65" s="6"/>
+      <c r="B65" s="68"/>
+      <c r="C65" s="2"/>
+      <c r="D65" s="7"/>
+      <c r="E65" s="68"/>
+      <c r="F65" s="68"/>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" s="29"/>
-    </row>
-    <row r="67" spans="1:6" ht="14" x14ac:dyDescent="0.3">
-      <c r="A67" s="38" t="s">
-        <v>151</v>
-      </c>
-      <c r="B67" s="72" t="s">
-        <v>148</v>
-      </c>
-      <c r="C67" s="72"/>
-    </row>
-    <row r="68" spans="1:6" ht="14" x14ac:dyDescent="0.3">
-      <c r="A68" s="40" t="s">
-        <v>127</v>
-      </c>
-      <c r="B68" s="67"/>
-      <c r="C68" s="67"/>
-      <c r="D68" s="2" t="s">
-        <v>152</v>
-      </c>
+      <c r="A66" s="6"/>
+      <c r="B66" s="68"/>
+      <c r="C66" s="2"/>
+      <c r="D66" s="7"/>
+      <c r="E66" s="6"/>
+      <c r="F66" s="68"/>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" s="6"/>
+      <c r="B67" s="68"/>
+      <c r="C67" s="2"/>
+      <c r="D67" s="7"/>
+      <c r="E67" s="6"/>
+      <c r="F67" s="68"/>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" s="6"/>
+      <c r="B68" s="6"/>
+      <c r="D68" s="7"/>
+      <c r="E68" s="6"/>
+      <c r="F68" s="6"/>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="B69" s="69"/>
-      <c r="C69" s="69"/>
-      <c r="D69" s="2" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" ht="14" x14ac:dyDescent="0.3">
-      <c r="A70" s="40" t="s">
-        <v>129</v>
-      </c>
-      <c r="B70" s="67"/>
-      <c r="C70" s="67"/>
+      <c r="A69" s="6"/>
+      <c r="B69" s="6"/>
+      <c r="D69" s="7"/>
+      <c r="E69" s="6"/>
+      <c r="F69" s="6"/>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70" s="6"/>
+      <c r="B70" s="6"/>
+      <c r="D70" s="7"/>
+      <c r="E70" s="6"/>
+      <c r="F70" s="6"/>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="B71" s="69"/>
-      <c r="C71" s="69"/>
-    </row>
-    <row r="72" spans="1:6" ht="14" x14ac:dyDescent="0.3">
-      <c r="A72" s="40" t="s">
-        <v>131</v>
-      </c>
-      <c r="B72" s="67"/>
-      <c r="C72" s="67"/>
+      <c r="A71" s="6"/>
+      <c r="B71" s="6"/>
+      <c r="D71" s="7"/>
+      <c r="E71" s="6"/>
+      <c r="F71" s="6"/>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72" s="6"/>
+      <c r="B72" s="6"/>
+      <c r="D72" s="7"/>
+      <c r="E72" s="6"/>
+      <c r="F72" s="6"/>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="B73" s="69"/>
-      <c r="C73" s="69"/>
-    </row>
-    <row r="74" spans="1:6" ht="14" x14ac:dyDescent="0.3">
-      <c r="A74" s="40" t="s">
-        <v>133</v>
-      </c>
-      <c r="B74" s="67"/>
-      <c r="C74" s="67"/>
+      <c r="A73" s="6"/>
+      <c r="B73" s="6"/>
+      <c r="D73" s="7"/>
+      <c r="E73" s="6"/>
+      <c r="F73" s="6"/>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74" s="6"/>
+      <c r="B74" s="6"/>
+      <c r="D74" s="7"/>
+      <c r="E74" s="6"/>
+      <c r="F74" s="6"/>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A75" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="B75" s="69"/>
-      <c r="C75" s="69"/>
-    </row>
-    <row r="76" spans="1:6" ht="14" x14ac:dyDescent="0.3">
-      <c r="A76" s="40" t="s">
-        <v>135</v>
-      </c>
-      <c r="B76" s="67"/>
-      <c r="C76" s="67"/>
+      <c r="A75" s="6"/>
+      <c r="B75" s="6"/>
+      <c r="D75" s="7"/>
+      <c r="E75" s="6"/>
+      <c r="F75" s="6"/>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A76" s="6"/>
+      <c r="B76" s="6"/>
+      <c r="D76" s="7"/>
+      <c r="E76" s="6"/>
+      <c r="F76" s="6"/>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A77" s="37" t="s">
-        <v>136</v>
-      </c>
-      <c r="B77" s="68"/>
-      <c r="C77" s="68"/>
-    </row>
-    <row r="78" spans="1:6" ht="6.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="10"/>
-      <c r="B78" s="11"/>
-      <c r="C78" s="11"/>
-      <c r="D78" s="11"/>
-      <c r="E78" s="11"/>
-      <c r="F78" s="11"/>
-    </row>
-    <row r="80" spans="1:6" s="8" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A80" s="45" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" s="47" customFormat="1" ht="14" x14ac:dyDescent="0.3">
-      <c r="A81" s="48" t="s">
-        <v>24</v>
-      </c>
-      <c r="B81" s="49" t="s">
-        <v>0</v>
-      </c>
-      <c r="C81" s="50" t="s">
-        <v>137</v>
-      </c>
-      <c r="D81" s="50" t="s">
-        <v>4</v>
-      </c>
-      <c r="E81" s="50" t="s">
-        <v>138</v>
-      </c>
-      <c r="F81" s="50" t="s">
-        <v>139</v>
-      </c>
+      <c r="A77" s="6"/>
+      <c r="B77" s="6"/>
+      <c r="D77" s="7"/>
+      <c r="E77" s="6"/>
+      <c r="F77" s="6"/>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78" s="6"/>
+      <c r="B78" s="6"/>
+      <c r="D78" s="7"/>
+      <c r="E78" s="6"/>
+      <c r="F78" s="6"/>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79" s="6"/>
+      <c r="B79" s="6"/>
+      <c r="D79" s="7"/>
+      <c r="E79" s="6"/>
+      <c r="F79" s="6"/>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A80" s="6"/>
+      <c r="B80" s="6"/>
+      <c r="D80" s="7"/>
+      <c r="E80" s="6"/>
+      <c r="F80" s="6"/>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A81" s="6"/>
+      <c r="B81" s="6"/>
+      <c r="D81" s="7"/>
+      <c r="E81" s="6"/>
+      <c r="F81" s="6"/>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="6"/>
-      <c r="B82" s="5"/>
-      <c r="C82" s="2"/>
+      <c r="B82" s="6"/>
       <c r="D82" s="7"/>
       <c r="E82" s="6"/>
-      <c r="F82" s="5"/>
+      <c r="F82" s="6"/>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="6"/>
-      <c r="B83" s="5"/>
-      <c r="C83" s="2"/>
+      <c r="B83" s="6"/>
       <c r="D83" s="7"/>
-      <c r="E83" s="5"/>
-      <c r="F83" s="5"/>
+      <c r="E83" s="6"/>
+      <c r="F83" s="6"/>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="6"/>
-      <c r="B84" s="5"/>
-      <c r="C84" s="2"/>
+      <c r="B84" s="6"/>
       <c r="D84" s="7"/>
       <c r="E84" s="6"/>
-      <c r="F84" s="5"/>
+      <c r="F84" s="6"/>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="6"/>
-      <c r="B85" s="5"/>
-      <c r="C85" s="2"/>
+      <c r="B85" s="6"/>
       <c r="D85" s="7"/>
       <c r="E85" s="6"/>
-      <c r="F85" s="5"/>
+      <c r="F85" s="6"/>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="6"/>
@@ -2774,188 +2696,134 @@
       <c r="F159" s="6"/>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A160" s="6"/>
-      <c r="B160" s="6"/>
-      <c r="D160" s="7"/>
       <c r="E160" s="6"/>
       <c r="F160" s="6"/>
     </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A161" s="6"/>
-      <c r="B161" s="6"/>
-      <c r="D161" s="7"/>
+    <row r="161" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E161" s="6"/>
       <c r="F161" s="6"/>
     </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A162" s="6"/>
-      <c r="B162" s="6"/>
-      <c r="D162" s="7"/>
+    <row r="162" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E162" s="6"/>
       <c r="F162" s="6"/>
     </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A163" s="6"/>
-      <c r="B163" s="6"/>
-      <c r="D163" s="7"/>
+    <row r="163" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E163" s="6"/>
       <c r="F163" s="6"/>
     </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A164" s="6"/>
-      <c r="B164" s="6"/>
-      <c r="D164" s="7"/>
+    <row r="164" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E164" s="6"/>
       <c r="F164" s="6"/>
     </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A165" s="6"/>
-      <c r="B165" s="6"/>
-      <c r="D165" s="7"/>
+    <row r="165" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E165" s="6"/>
       <c r="F165" s="6"/>
     </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A166" s="6"/>
-      <c r="B166" s="6"/>
-      <c r="D166" s="7"/>
+    <row r="166" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E166" s="6"/>
       <c r="F166" s="6"/>
     </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A167" s="6"/>
-      <c r="B167" s="6"/>
-      <c r="D167" s="7"/>
+    <row r="167" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E167" s="6"/>
       <c r="F167" s="6"/>
     </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A168" s="6"/>
-      <c r="B168" s="6"/>
-      <c r="D168" s="7"/>
+    <row r="168" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E168" s="6"/>
       <c r="F168" s="6"/>
     </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A169" s="6"/>
-      <c r="B169" s="6"/>
-      <c r="D169" s="7"/>
+    <row r="169" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E169" s="6"/>
       <c r="F169" s="6"/>
     </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A170" s="6"/>
-      <c r="B170" s="6"/>
-      <c r="D170" s="7"/>
+    <row r="170" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E170" s="6"/>
       <c r="F170" s="6"/>
     </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A171" s="6"/>
-      <c r="B171" s="6"/>
-      <c r="D171" s="7"/>
+    <row r="171" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E171" s="6"/>
       <c r="F171" s="6"/>
     </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A172" s="6"/>
-      <c r="B172" s="6"/>
-      <c r="D172" s="7"/>
+    <row r="172" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E172" s="6"/>
       <c r="F172" s="6"/>
     </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A173" s="6"/>
-      <c r="B173" s="6"/>
-      <c r="D173" s="7"/>
+    <row r="173" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E173" s="6"/>
       <c r="F173" s="6"/>
     </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A174" s="6"/>
-      <c r="B174" s="6"/>
-      <c r="D174" s="7"/>
+    <row r="174" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E174" s="6"/>
       <c r="F174" s="6"/>
     </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A175" s="6"/>
-      <c r="B175" s="6"/>
-      <c r="D175" s="7"/>
+    <row r="175" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E175" s="6"/>
       <c r="F175" s="6"/>
     </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A176" s="6"/>
-      <c r="B176" s="6"/>
-      <c r="D176" s="7"/>
+    <row r="176" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E176" s="6"/>
       <c r="F176" s="6"/>
     </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A177" s="6"/>
-      <c r="B177" s="6"/>
-      <c r="D177" s="7"/>
+    <row r="177" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E177" s="6"/>
       <c r="F177" s="6"/>
     </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="178" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E178" s="6"/>
       <c r="F178" s="6"/>
     </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="179" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E179" s="6"/>
       <c r="F179" s="6"/>
     </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="180" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E180" s="6"/>
       <c r="F180" s="6"/>
     </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="181" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E181" s="6"/>
       <c r="F181" s="6"/>
     </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="182" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E182" s="6"/>
       <c r="F182" s="6"/>
     </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="183" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E183" s="6"/>
       <c r="F183" s="6"/>
     </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="184" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E184" s="6"/>
       <c r="F184" s="6"/>
     </row>
-    <row r="185" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="185" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E185" s="6"/>
       <c r="F185" s="6"/>
     </row>
-    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="186" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E186" s="6"/>
       <c r="F186" s="6"/>
     </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="187" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E187" s="6"/>
       <c r="F187" s="6"/>
     </row>
-    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="188" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E188" s="6"/>
       <c r="F188" s="6"/>
     </row>
-    <row r="189" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="189" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E189" s="6"/>
       <c r="F189" s="6"/>
     </row>
-    <row r="190" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="190" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E190" s="6"/>
       <c r="F190" s="6"/>
     </row>
-    <row r="191" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="191" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E191" s="6"/>
       <c r="F191" s="6"/>
     </row>
-    <row r="192" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="192" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E192" s="6"/>
       <c r="F192" s="6"/>
     </row>
@@ -3139,80 +3007,8 @@
       <c r="E237" s="6"/>
       <c r="F237" s="6"/>
     </row>
-    <row r="238" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E238" s="6"/>
-      <c r="F238" s="6"/>
-    </row>
-    <row r="239" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E239" s="6"/>
-      <c r="F239" s="6"/>
-    </row>
-    <row r="240" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E240" s="6"/>
-      <c r="F240" s="6"/>
-    </row>
-    <row r="241" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E241" s="6"/>
-      <c r="F241" s="6"/>
-    </row>
-    <row r="242" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E242" s="6"/>
-      <c r="F242" s="6"/>
-    </row>
-    <row r="243" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E243" s="6"/>
-      <c r="F243" s="6"/>
-    </row>
-    <row r="244" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E244" s="6"/>
-      <c r="F244" s="6"/>
-    </row>
-    <row r="245" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E245" s="6"/>
-      <c r="F245" s="6"/>
-    </row>
-    <row r="246" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E246" s="6"/>
-      <c r="F246" s="6"/>
-    </row>
-    <row r="247" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E247" s="6"/>
-      <c r="F247" s="6"/>
-    </row>
-    <row r="248" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E248" s="6"/>
-      <c r="F248" s="6"/>
-    </row>
-    <row r="249" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E249" s="6"/>
-      <c r="F249" s="6"/>
-    </row>
-    <row r="250" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E250" s="6"/>
-      <c r="F250" s="6"/>
-    </row>
-    <row r="251" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E251" s="6"/>
-      <c r="F251" s="6"/>
-    </row>
-    <row r="252" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E252" s="6"/>
-      <c r="F252" s="6"/>
-    </row>
-    <row r="253" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E253" s="6"/>
-      <c r="F253" s="6"/>
-    </row>
-    <row r="254" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E254" s="6"/>
-      <c r="F254" s="6"/>
-    </row>
-    <row r="255" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E255" s="6"/>
-      <c r="F255" s="6"/>
-    </row>
   </sheetData>
-  <mergeCells count="37">
+  <mergeCells count="15">
     <mergeCell ref="B16:F16"/>
     <mergeCell ref="B17:F17"/>
     <mergeCell ref="C27:F28"/>
@@ -3222,56 +3018,33 @@
     <mergeCell ref="B13:F13"/>
     <mergeCell ref="B14:F14"/>
     <mergeCell ref="B15:F15"/>
-    <mergeCell ref="B9:F9"/>
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="C2:F2"/>
     <mergeCell ref="B6:F6"/>
     <mergeCell ref="B7:F7"/>
     <mergeCell ref="B8:F8"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="B61:C61"/>
-    <mergeCell ref="B62:C62"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="B76:C76"/>
-    <mergeCell ref="B77:C77"/>
-    <mergeCell ref="B71:C71"/>
-    <mergeCell ref="B72:C72"/>
-    <mergeCell ref="B73:C73"/>
-    <mergeCell ref="B74:C74"/>
-    <mergeCell ref="B75:C75"/>
+    <mergeCell ref="B9:F9"/>
   </mergeCells>
-  <phoneticPr fontId="13" type="noConversion"/>
-  <conditionalFormatting sqref="D82:D177">
-    <cfRule type="expression" dxfId="9" priority="4">
-      <formula>($B$47/$D82)&gt;(0.5*$B$48)</formula>
+  <conditionalFormatting sqref="D64:D159">
+    <cfRule type="expression" dxfId="9" priority="3">
+      <formula>($B$37/$D64)&gt;(0.5*$B$38)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B3 B21:B22 B34:B38 B43:B44 B47:B48 B27:B28">
-    <cfRule type="containsBlanks" dxfId="8" priority="3">
+  <conditionalFormatting sqref="B2:B3 B21:B22 B34:B35 B37:B38 B27:B28 B46:B47 B43">
+    <cfRule type="containsBlanks" dxfId="8" priority="2">
       <formula>LEN(TRIM(B2))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B53">
+  <conditionalFormatting sqref="B44">
     <cfRule type="containsBlanks" dxfId="7" priority="1">
-      <formula>LEN(TRIM(B53))=0</formula>
+      <formula>LEN(TRIM(B44))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Slot must be between 1 and 11" sqref="B32 B27" xr:uid="{7EA488CB-C77F-4490-92FA-1821AC567FF6}"/>
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B43:B44 B47:B48" xr:uid="{727FCE64-D09B-4D4D-B81E-FAB7FB2E5C88}">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B34:B35 B37:B38" xr:uid="{B2A947F0-E894-4D3B-A808-2C4D31EEFB25}">
       <formula1>0</formula1>
     </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Slot must be between 1 and 11" sqref="B27" xr:uid="{F32CB6B4-0A41-4F22-9FB0-4ADFE2222E0A}"/>
   </dataValidations>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="5" scale="83" fitToHeight="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -3281,17 +3054,17 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{ACF75BDF-171F-406B-A877-2A1B68FBA80E}">
-          <x14:formula1>
-            <xm:f>'Linked Values'!$A$3:$A$13</xm:f>
-          </x14:formula1>
-          <xm:sqref>B7:F17</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{906E5868-2E53-46D6-80D5-045DE1983AE6}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{1DA6AA3B-7DA5-4EF1-947E-BB913217EFC3}">
           <x14:formula1>
             <xm:f>'Linked Values'!$D$3:$D$6</xm:f>
           </x14:formula1>
           <xm:sqref>B21:B22</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{D0F7A710-9AB2-4682-9835-26809308D3E2}">
+          <x14:formula1>
+            <xm:f>'Linked Values'!$A$3:$A$14</xm:f>
+          </x14:formula1>
+          <xm:sqref>B7:F17</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3301,17 +3074,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B096AE39-CBE9-438B-8EF5-43BA511A3359}">
-  <dimension ref="A1:I567"/>
+  <dimension ref="A1:I568"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView topLeftCell="A2" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="H41" sqref="H41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.453125" customWidth="1"/>
     <col min="2" max="2" width="16.81640625" customWidth="1"/>
-    <col min="3" max="3" width="19.7265625" customWidth="1"/>
+    <col min="3" max="3" width="24.54296875" customWidth="1"/>
     <col min="4" max="4" width="22.1796875" customWidth="1"/>
     <col min="5" max="5" width="19.26953125" customWidth="1"/>
     <col min="6" max="6" width="20.54296875" customWidth="1"/>
@@ -3320,30 +3093,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.4">
-      <c r="A1" s="65" t="s">
+      <c r="A1" s="61" t="s">
         <v>92</v>
       </c>
-      <c r="B1" s="66" t="s">
-        <v>160</v>
-      </c>
-      <c r="C1" s="78" t="s">
+      <c r="B1" s="62" t="s">
+        <v>148</v>
+      </c>
+      <c r="C1" s="70" t="s">
         <v>40</v>
       </c>
-      <c r="D1" s="78"/>
-      <c r="E1" s="78"/>
-      <c r="F1" s="78"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
     </row>
     <row r="2" spans="1:6" ht="13" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="3"/>
-      <c r="C2" s="78" t="s">
+      <c r="C2" s="70" t="s">
         <v>50</v>
       </c>
-      <c r="D2" s="78"/>
-      <c r="E2" s="78"/>
-      <c r="F2" s="78"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -3363,126 +3136,126 @@
       <c r="F5" s="11"/>
     </row>
     <row r="6" spans="1:6" ht="13" x14ac:dyDescent="0.3">
-      <c r="A6" s="53" t="s">
+      <c r="A6" s="49" t="s">
         <v>37</v>
       </c>
-      <c r="B6" s="79" t="s">
+      <c r="B6" s="71" t="s">
         <v>51</v>
       </c>
-      <c r="C6" s="79"/>
-      <c r="D6" s="79"/>
-      <c r="E6" s="79"/>
-      <c r="F6" s="79"/>
+      <c r="C6" s="71"/>
+      <c r="D6" s="71"/>
+      <c r="E6" s="71"/>
+      <c r="F6" s="71"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="77"/>
-      <c r="C7" s="77"/>
-      <c r="D7" s="77"/>
-      <c r="E7" s="77"/>
-      <c r="F7" s="77"/>
+      <c r="B7" s="69"/>
+      <c r="C7" s="69"/>
+      <c r="D7" s="69"/>
+      <c r="E7" s="69"/>
+      <c r="F7" s="69"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="80"/>
-      <c r="C8" s="80"/>
-      <c r="D8" s="80"/>
-      <c r="E8" s="80"/>
-      <c r="F8" s="80"/>
+      <c r="B8" s="72"/>
+      <c r="C8" s="72"/>
+      <c r="D8" s="72"/>
+      <c r="E8" s="72"/>
+      <c r="F8" s="72"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="77"/>
-      <c r="C9" s="77"/>
-      <c r="D9" s="77"/>
-      <c r="E9" s="77"/>
-      <c r="F9" s="77"/>
+      <c r="B9" s="69"/>
+      <c r="C9" s="69"/>
+      <c r="D9" s="69"/>
+      <c r="E9" s="69"/>
+      <c r="F9" s="69"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="80"/>
-      <c r="C10" s="80"/>
-      <c r="D10" s="80"/>
-      <c r="E10" s="80"/>
-      <c r="F10" s="80"/>
+      <c r="B10" s="72"/>
+      <c r="C10" s="72"/>
+      <c r="D10" s="72"/>
+      <c r="E10" s="72"/>
+      <c r="F10" s="72"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="77"/>
-      <c r="C11" s="77"/>
-      <c r="D11" s="77"/>
-      <c r="E11" s="77"/>
-      <c r="F11" s="77"/>
+      <c r="B11" s="69"/>
+      <c r="C11" s="69"/>
+      <c r="D11" s="69"/>
+      <c r="E11" s="69"/>
+      <c r="F11" s="69"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="80"/>
-      <c r="C12" s="80"/>
-      <c r="D12" s="80"/>
-      <c r="E12" s="80"/>
-      <c r="F12" s="80"/>
+      <c r="B12" s="72"/>
+      <c r="C12" s="72"/>
+      <c r="D12" s="72"/>
+      <c r="E12" s="72"/>
+      <c r="F12" s="72"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="77"/>
-      <c r="C13" s="77"/>
-      <c r="D13" s="77"/>
-      <c r="E13" s="77"/>
-      <c r="F13" s="77"/>
+      <c r="B13" s="69"/>
+      <c r="C13" s="69"/>
+      <c r="D13" s="69"/>
+      <c r="E13" s="69"/>
+      <c r="F13" s="69"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="80"/>
-      <c r="C14" s="80"/>
-      <c r="D14" s="80"/>
-      <c r="E14" s="80"/>
-      <c r="F14" s="80"/>
+      <c r="B14" s="72"/>
+      <c r="C14" s="72"/>
+      <c r="D14" s="72"/>
+      <c r="E14" s="72"/>
+      <c r="F14" s="72"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="77"/>
-      <c r="C15" s="77"/>
-      <c r="D15" s="77"/>
-      <c r="E15" s="77"/>
-      <c r="F15" s="77"/>
+      <c r="B15" s="69"/>
+      <c r="C15" s="69"/>
+      <c r="D15" s="69"/>
+      <c r="E15" s="69"/>
+      <c r="F15" s="69"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="80"/>
-      <c r="C16" s="80"/>
-      <c r="D16" s="80"/>
-      <c r="E16" s="80"/>
-      <c r="F16" s="80"/>
+      <c r="B16" s="72"/>
+      <c r="C16" s="72"/>
+      <c r="D16" s="72"/>
+      <c r="E16" s="72"/>
+      <c r="F16" s="72"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="77"/>
-      <c r="C17" s="77"/>
-      <c r="D17" s="77"/>
-      <c r="E17" s="77"/>
-      <c r="F17" s="77"/>
+      <c r="B17" s="69"/>
+      <c r="C17" s="69"/>
+      <c r="D17" s="69"/>
+      <c r="E17" s="69"/>
+      <c r="F17" s="69"/>
     </row>
     <row r="18" spans="1:6" ht="6.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="10"/>
@@ -3496,7 +3269,7 @@
       <c r="A19" s="12"/>
     </row>
     <row r="20" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A20" s="43" t="s">
+      <c r="A20" s="39" t="s">
         <v>38</v>
       </c>
       <c r="B20" s="6"/>
@@ -3535,57 +3308,57 @@
       <c r="C25" s="2"/>
     </row>
     <row r="26" spans="1:6" s="13" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A26" s="44" t="s">
-        <v>155</v>
+      <c r="A26" s="40" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="27" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="14" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B27" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="C27" s="81" t="s">
-        <v>114</v>
-      </c>
-      <c r="D27" s="81"/>
-      <c r="E27" s="81"/>
-      <c r="F27" s="81"/>
+      <c r="C27" s="73" t="s">
+        <v>112</v>
+      </c>
+      <c r="D27" s="73"/>
+      <c r="E27" s="73"/>
+      <c r="F27" s="73"/>
     </row>
     <row r="28" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="B28" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="B28" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="C28" s="81"/>
-      <c r="D28" s="81"/>
-      <c r="E28" s="81"/>
-      <c r="F28" s="81"/>
-    </row>
-    <row r="29" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="88" t="s">
-        <v>157</v>
-      </c>
-      <c r="B29" s="33">
-        <v>0.75</v>
-      </c>
-      <c r="C29" s="51" t="s">
-        <v>158</v>
-      </c>
-      <c r="D29" s="51"/>
-      <c r="E29" s="51"/>
-      <c r="F29" s="51"/>
+      <c r="C28" s="73"/>
+      <c r="D28" s="73"/>
+      <c r="E28" s="73"/>
+      <c r="F28" s="73"/>
+    </row>
+    <row r="29" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="64" t="s">
+        <v>137</v>
+      </c>
+      <c r="B29" s="85">
+        <v>1</v>
+      </c>
+      <c r="C29" s="47" t="s">
+        <v>138</v>
+      </c>
+      <c r="D29" s="47"/>
+      <c r="E29" s="47"/>
+      <c r="F29" s="47"/>
     </row>
     <row r="30" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="12"/>
       <c r="B30"/>
-      <c r="C30" s="52"/>
-      <c r="D30" s="52"/>
-      <c r="E30" s="52"/>
-      <c r="F30" s="52"/>
+      <c r="C30" s="48"/>
+      <c r="D30" s="48"/>
+      <c r="E30" s="48"/>
+      <c r="F30" s="48"/>
     </row>
     <row r="31" spans="1:6" ht="6.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="10"/>
@@ -3601,7 +3374,7 @@
       <c r="C32" s="16"/>
     </row>
     <row r="33" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A33" s="43" t="s">
+      <c r="A33" s="39" t="s">
         <v>23</v>
       </c>
     </row>
@@ -3611,7 +3384,7 @@
       </c>
       <c r="B34" s="6"/>
       <c r="C34" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -3623,11 +3396,11 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B36" s="5"/>
       <c r="C36" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -3639,11 +3412,11 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B38" s="5"/>
       <c r="C38" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -3659,7 +3432,7 @@
       <c r="F40" s="11"/>
     </row>
     <row r="42" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A42" s="45" t="s">
+      <c r="A42" s="41" t="s">
         <v>53</v>
       </c>
     </row>
@@ -3685,59 +3458,63 @@
       <c r="A45" s="3" t="s">
         <v>39</v>
       </c>
+      <c r="B45" s="2"/>
       <c r="C45" s="2" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="3"/>
-      <c r="C46" s="2"/>
-    </row>
-    <row r="47" spans="1:6" ht="6.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="10"/>
-      <c r="B47" s="11"/>
-      <c r="C47" s="11"/>
-      <c r="D47" s="11"/>
-      <c r="E47" s="11"/>
-      <c r="F47" s="11"/>
-    </row>
-    <row r="49" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A49" s="45" t="s">
+      <c r="A46" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="3"/>
+      <c r="C47" s="2"/>
+    </row>
+    <row r="48" spans="1:6" ht="6.65" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="10"/>
+      <c r="B48" s="11"/>
+      <c r="C48" s="11"/>
+      <c r="D48" s="11"/>
+      <c r="E48" s="11"/>
+      <c r="F48" s="11"/>
+    </row>
+    <row r="50" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A50" s="41" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="13" x14ac:dyDescent="0.3">
-      <c r="A50" s="18" t="s">
+    <row r="51" spans="1:9" ht="13" x14ac:dyDescent="0.3">
+      <c r="A51" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="B50" s="19" t="s">
+      <c r="B51" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C50" s="20" t="s">
+      <c r="C51" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="D50" s="20" t="s">
+      <c r="D51" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="E50" s="20" t="s">
+      <c r="E51" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="F50" s="20" t="s">
+      <c r="F51" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="I50" s="1"/>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A51" s="6"/>
-      <c r="B51" s="6"/>
-      <c r="D51" s="7"/>
-      <c r="E51" s="6"/>
-      <c r="F51" s="5"/>
+      <c r="I51" s="1"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="6"/>
-      <c r="B52" s="5"/>
-      <c r="C52" s="2"/>
+      <c r="B52" s="63"/>
       <c r="D52" s="7"/>
       <c r="E52" s="6"/>
       <c r="F52" s="5"/>
@@ -3760,157 +3537,158 @@
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="6"/>
-      <c r="B55" s="6"/>
+      <c r="B55" s="63"/>
+      <c r="C55" s="2"/>
       <c r="D55" s="7"/>
       <c r="E55" s="6"/>
-      <c r="F55" s="6"/>
+      <c r="F55" s="5"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="6"/>
-      <c r="B56" s="6"/>
+      <c r="B56" s="63"/>
       <c r="D56" s="7"/>
       <c r="E56" s="6"/>
-      <c r="F56" s="6"/>
+      <c r="F56" s="63"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="6"/>
-      <c r="B57" s="6"/>
+      <c r="B57" s="63"/>
       <c r="D57" s="7"/>
       <c r="E57" s="6"/>
-      <c r="F57" s="6"/>
+      <c r="F57" s="63"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="6"/>
-      <c r="B58" s="6"/>
+      <c r="B58" s="63"/>
       <c r="D58" s="7"/>
       <c r="E58" s="6"/>
-      <c r="F58" s="6"/>
+      <c r="F58" s="63"/>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="6"/>
-      <c r="B59" s="6"/>
+      <c r="B59" s="63"/>
       <c r="D59" s="7"/>
       <c r="E59" s="6"/>
-      <c r="F59" s="6"/>
+      <c r="F59" s="63"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="6"/>
-      <c r="B60" s="6"/>
+      <c r="B60" s="63"/>
       <c r="D60" s="7"/>
       <c r="E60" s="6"/>
-      <c r="F60" s="6"/>
+      <c r="F60" s="63"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="6"/>
-      <c r="B61" s="6"/>
+      <c r="B61" s="63"/>
       <c r="D61" s="7"/>
       <c r="E61" s="6"/>
-      <c r="F61" s="6"/>
+      <c r="F61" s="63"/>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="6"/>
-      <c r="B62" s="6"/>
+      <c r="B62" s="63"/>
       <c r="D62" s="7"/>
       <c r="E62" s="6"/>
-      <c r="F62" s="6"/>
+      <c r="F62" s="63"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="6"/>
-      <c r="B63" s="6"/>
+      <c r="B63" s="63"/>
       <c r="D63" s="7"/>
       <c r="E63" s="6"/>
-      <c r="F63" s="6"/>
+      <c r="F63" s="63"/>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="6"/>
-      <c r="B64" s="6"/>
+      <c r="B64" s="63"/>
       <c r="D64" s="7"/>
       <c r="E64" s="6"/>
-      <c r="F64" s="6"/>
+      <c r="F64" s="63"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="6"/>
-      <c r="B65" s="6"/>
+      <c r="B65" s="63"/>
       <c r="D65" s="7"/>
       <c r="E65" s="6"/>
-      <c r="F65" s="6"/>
+      <c r="F65" s="63"/>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="6"/>
-      <c r="B66" s="6"/>
+      <c r="B66" s="63"/>
       <c r="D66" s="7"/>
       <c r="E66" s="6"/>
-      <c r="F66" s="6"/>
+      <c r="F66" s="63"/>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="6"/>
-      <c r="B67" s="6"/>
+      <c r="B67" s="63"/>
       <c r="D67" s="7"/>
       <c r="E67" s="6"/>
-      <c r="F67" s="6"/>
+      <c r="F67" s="63"/>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="6"/>
-      <c r="B68" s="6"/>
+      <c r="B68" s="63"/>
       <c r="D68" s="7"/>
       <c r="E68" s="6"/>
-      <c r="F68" s="6"/>
+      <c r="F68" s="63"/>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="6"/>
-      <c r="B69" s="6"/>
+      <c r="B69" s="63"/>
       <c r="D69" s="7"/>
       <c r="E69" s="6"/>
-      <c r="F69" s="6"/>
+      <c r="F69" s="63"/>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="6"/>
-      <c r="B70" s="6"/>
+      <c r="B70" s="63"/>
       <c r="D70" s="7"/>
       <c r="E70" s="6"/>
-      <c r="F70" s="6"/>
+      <c r="F70" s="63"/>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="6"/>
-      <c r="B71" s="6"/>
+      <c r="B71" s="63"/>
       <c r="D71" s="7"/>
       <c r="E71" s="6"/>
-      <c r="F71" s="6"/>
+      <c r="F71" s="63"/>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="6"/>
-      <c r="B72" s="6"/>
+      <c r="B72" s="63"/>
       <c r="D72" s="7"/>
       <c r="E72" s="6"/>
-      <c r="F72" s="6"/>
+      <c r="F72" s="63"/>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="6"/>
-      <c r="B73" s="6"/>
+      <c r="B73" s="63"/>
       <c r="D73" s="7"/>
       <c r="E73" s="6"/>
-      <c r="F73" s="6"/>
+      <c r="F73" s="63"/>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="6"/>
-      <c r="B74" s="6"/>
+      <c r="B74" s="63"/>
       <c r="D74" s="7"/>
       <c r="E74" s="6"/>
-      <c r="F74" s="6"/>
+      <c r="F74" s="63"/>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="6"/>
-      <c r="B75" s="6"/>
+      <c r="B75" s="63"/>
       <c r="D75" s="7"/>
       <c r="E75" s="6"/>
-      <c r="F75" s="6"/>
+      <c r="F75" s="63"/>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="6"/>
-      <c r="B76" s="6"/>
+      <c r="B76" s="63"/>
       <c r="D76" s="7"/>
       <c r="E76" s="6"/>
-      <c r="F76" s="6"/>
+      <c r="F76" s="63"/>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="6"/>
@@ -4585,6 +4363,7 @@
       <c r="F172" s="6"/>
     </row>
     <row r="173" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A173" s="6"/>
       <c r="B173" s="6"/>
       <c r="D173" s="7"/>
       <c r="E173" s="6"/>
@@ -4723,6 +4502,7 @@
       <c r="F195" s="6"/>
     </row>
     <row r="196" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B196" s="6"/>
       <c r="D196" s="7"/>
       <c r="E196" s="6"/>
       <c r="F196" s="6"/>
@@ -6038,6 +5818,7 @@
       <c r="F458" s="6"/>
     </row>
     <row r="459" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D459" s="7"/>
       <c r="E459" s="6"/>
       <c r="F459" s="6"/>
     </row>
@@ -6472,6 +6253,10 @@
     <row r="567" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E567" s="6"/>
       <c r="F567" s="6"/>
+    </row>
+    <row r="568" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E568" s="6"/>
+      <c r="F568" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="15">
@@ -6491,13 +6276,13 @@
     <mergeCell ref="B10:F10"/>
     <mergeCell ref="B11:F11"/>
   </mergeCells>
-  <phoneticPr fontId="4" type="noConversion"/>
-  <conditionalFormatting sqref="D51:D458">
+  <phoneticPr fontId="3" type="noConversion"/>
+  <conditionalFormatting sqref="D52:D459">
     <cfRule type="expression" dxfId="6" priority="3">
-      <formula>($B$43/$D51)&gt;(0.5*$B$44)</formula>
+      <formula>($B$43/$D52)&gt;(0.5*$B$44)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B3 B21:B22 B34:B38 B43:B45 B27:B28">
+  <conditionalFormatting sqref="B2:B3 B21:B22 B34:B38 B43:B46 B27:B28">
     <cfRule type="containsBlanks" dxfId="5" priority="2">
       <formula>LEN(TRIM(B2))=0</formula>
     </cfRule>
@@ -6524,7 +6309,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{77DFBECE-7E49-49D8-BDA3-34A392C2D5A8}">
           <x14:formula1>
-            <xm:f>'Linked Values'!$A$3:$A$13</xm:f>
+            <xm:f>'Linked Values'!$A$3:$A$15</xm:f>
           </x14:formula1>
           <xm:sqref>B7:F17</xm:sqref>
         </x14:dataValidation>
@@ -6538,8 +6323,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{547A22CE-6B5B-419C-B571-1556B7859EB9}">
   <dimension ref="A1:J589"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="I33" sqref="I33"/>
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -6555,11 +6340,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.4">
-      <c r="A1" s="65" t="s">
-        <v>106</v>
-      </c>
-      <c r="B1" s="66" t="s">
-        <v>156</v>
+      <c r="A1" s="61" t="s">
+        <v>105</v>
+      </c>
+      <c r="B1" s="62" t="s">
+        <v>147</v>
       </c>
       <c r="C1" s="25" t="s">
         <v>40</v>
@@ -6603,135 +6388,135 @@
       <c r="A6" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="B6" s="79" t="s">
+      <c r="B6" s="71" t="s">
         <v>51</v>
       </c>
-      <c r="C6" s="79"/>
-      <c r="D6" s="79"/>
-      <c r="E6" s="79"/>
-      <c r="F6" s="79"/>
-      <c r="G6" s="79"/>
+      <c r="C6" s="71"/>
+      <c r="D6" s="71"/>
+      <c r="E6" s="71"/>
+      <c r="F6" s="71"/>
+      <c r="G6" s="71"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="77"/>
-      <c r="C7" s="77"/>
-      <c r="D7" s="77"/>
-      <c r="E7" s="77"/>
-      <c r="F7" s="77"/>
-      <c r="G7" s="77"/>
+      <c r="B7" s="69"/>
+      <c r="C7" s="69"/>
+      <c r="D7" s="69"/>
+      <c r="E7" s="69"/>
+      <c r="F7" s="69"/>
+      <c r="G7" s="69"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="80"/>
-      <c r="C8" s="80"/>
-      <c r="D8" s="80"/>
-      <c r="E8" s="80"/>
-      <c r="F8" s="80"/>
-      <c r="G8" s="80"/>
+      <c r="B8" s="72"/>
+      <c r="C8" s="72"/>
+      <c r="D8" s="72"/>
+      <c r="E8" s="72"/>
+      <c r="F8" s="72"/>
+      <c r="G8" s="72"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="77"/>
-      <c r="C9" s="77"/>
-      <c r="D9" s="77"/>
-      <c r="E9" s="77"/>
-      <c r="F9" s="77"/>
-      <c r="G9" s="77"/>
+      <c r="B9" s="69"/>
+      <c r="C9" s="69"/>
+      <c r="D9" s="69"/>
+      <c r="E9" s="69"/>
+      <c r="F9" s="69"/>
+      <c r="G9" s="69"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="80"/>
-      <c r="C10" s="80"/>
-      <c r="D10" s="80"/>
-      <c r="E10" s="80"/>
-      <c r="F10" s="80"/>
-      <c r="G10" s="80"/>
+      <c r="B10" s="72"/>
+      <c r="C10" s="72"/>
+      <c r="D10" s="72"/>
+      <c r="E10" s="72"/>
+      <c r="F10" s="72"/>
+      <c r="G10" s="72"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="77"/>
-      <c r="C11" s="77"/>
-      <c r="D11" s="77"/>
-      <c r="E11" s="77"/>
-      <c r="F11" s="77"/>
-      <c r="G11" s="77"/>
+      <c r="B11" s="69"/>
+      <c r="C11" s="69"/>
+      <c r="D11" s="69"/>
+      <c r="E11" s="69"/>
+      <c r="F11" s="69"/>
+      <c r="G11" s="69"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="80"/>
-      <c r="C12" s="80"/>
-      <c r="D12" s="80"/>
-      <c r="E12" s="80"/>
-      <c r="F12" s="80"/>
-      <c r="G12" s="80"/>
+      <c r="B12" s="72"/>
+      <c r="C12" s="72"/>
+      <c r="D12" s="72"/>
+      <c r="E12" s="72"/>
+      <c r="F12" s="72"/>
+      <c r="G12" s="72"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="77"/>
-      <c r="C13" s="77"/>
-      <c r="D13" s="77"/>
-      <c r="E13" s="77"/>
-      <c r="F13" s="77"/>
-      <c r="G13" s="77"/>
+      <c r="B13" s="69"/>
+      <c r="C13" s="69"/>
+      <c r="D13" s="69"/>
+      <c r="E13" s="69"/>
+      <c r="F13" s="69"/>
+      <c r="G13" s="69"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="80"/>
-      <c r="C14" s="80"/>
-      <c r="D14" s="80"/>
-      <c r="E14" s="80"/>
-      <c r="F14" s="80"/>
-      <c r="G14" s="80"/>
+      <c r="B14" s="72"/>
+      <c r="C14" s="72"/>
+      <c r="D14" s="72"/>
+      <c r="E14" s="72"/>
+      <c r="F14" s="72"/>
+      <c r="G14" s="72"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="77"/>
-      <c r="C15" s="77"/>
-      <c r="D15" s="77"/>
-      <c r="E15" s="77"/>
-      <c r="F15" s="77"/>
-      <c r="G15" s="77"/>
+      <c r="B15" s="69"/>
+      <c r="C15" s="69"/>
+      <c r="D15" s="69"/>
+      <c r="E15" s="69"/>
+      <c r="F15" s="69"/>
+      <c r="G15" s="69"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="80"/>
-      <c r="C16" s="80"/>
-      <c r="D16" s="80"/>
-      <c r="E16" s="80"/>
-      <c r="F16" s="80"/>
-      <c r="G16" s="80"/>
+      <c r="B16" s="72"/>
+      <c r="C16" s="72"/>
+      <c r="D16" s="72"/>
+      <c r="E16" s="72"/>
+      <c r="F16" s="72"/>
+      <c r="G16" s="72"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="77"/>
-      <c r="C17" s="77"/>
-      <c r="D17" s="77"/>
-      <c r="E17" s="77"/>
-      <c r="F17" s="77"/>
-      <c r="G17" s="77"/>
+      <c r="B17" s="69"/>
+      <c r="C17" s="69"/>
+      <c r="D17" s="69"/>
+      <c r="E17" s="69"/>
+      <c r="F17" s="69"/>
+      <c r="G17" s="69"/>
     </row>
     <row r="18" spans="1:7" ht="6.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="10"/>
@@ -6746,10 +6531,10 @@
       <c r="A19" s="12"/>
     </row>
     <row r="20" spans="1:7" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A20" s="85" t="s">
+      <c r="A20" s="77" t="s">
         <v>38</v>
       </c>
-      <c r="B20" s="85"/>
+      <c r="B20" s="77"/>
       <c r="C20" s="6"/>
       <c r="D20" s="2"/>
     </row>
@@ -6789,57 +6574,57 @@
       <c r="D25" s="2"/>
     </row>
     <row r="26" spans="1:7" s="13" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A26" s="44" t="s">
-        <v>155</v>
+      <c r="A26" s="40" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="27" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="14" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B27" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="C27" s="81" t="s">
-        <v>114</v>
-      </c>
-      <c r="D27" s="81"/>
-      <c r="E27" s="81"/>
-      <c r="F27" s="81"/>
+      <c r="C27" s="73" t="s">
+        <v>112</v>
+      </c>
+      <c r="D27" s="73"/>
+      <c r="E27" s="73"/>
+      <c r="F27" s="73"/>
     </row>
     <row r="28" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B28" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="C28" s="81"/>
-      <c r="D28" s="81"/>
-      <c r="E28" s="81"/>
-      <c r="F28" s="81"/>
-    </row>
-    <row r="29" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="88" t="s">
-        <v>157</v>
-      </c>
-      <c r="B29" s="33">
-        <v>0.75</v>
-      </c>
-      <c r="C29" s="51" t="s">
-        <v>158</v>
-      </c>
-      <c r="D29" s="51"/>
-      <c r="E29" s="51"/>
-      <c r="F29" s="51"/>
-    </row>
-    <row r="30" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="88"/>
-      <c r="B30" s="33"/>
-      <c r="C30" s="51"/>
-      <c r="D30" s="51"/>
-      <c r="E30" s="51"/>
-      <c r="F30" s="51"/>
+      <c r="C28" s="73"/>
+      <c r="D28" s="73"/>
+      <c r="E28" s="73"/>
+      <c r="F28" s="73"/>
+    </row>
+    <row r="29" spans="1:7" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="64" t="s">
+        <v>137</v>
+      </c>
+      <c r="B29" s="85">
+        <v>1</v>
+      </c>
+      <c r="C29" s="47" t="s">
+        <v>138</v>
+      </c>
+      <c r="D29" s="47"/>
+      <c r="E29" s="47"/>
+      <c r="F29" s="47"/>
+    </row>
+    <row r="30" spans="1:7" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="64"/>
+      <c r="B30" s="32"/>
+      <c r="C30" s="47"/>
+      <c r="D30" s="47"/>
+      <c r="E30" s="47"/>
+      <c r="F30" s="47"/>
     </row>
     <row r="31" spans="1:7" ht="6.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="10"/>
@@ -6857,11 +6642,11 @@
       <c r="D32" s="16"/>
     </row>
     <row r="33" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A33" s="86" t="s">
+      <c r="A33" s="78" t="s">
         <v>23</v>
       </c>
-      <c r="B33" s="86"/>
-      <c r="C33" s="86"/>
+      <c r="B33" s="78"/>
+      <c r="C33" s="78"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
@@ -6880,11 +6665,11 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B36" s="5"/>
       <c r="C36" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -6896,11 +6681,11 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B38" s="5"/>
       <c r="C38" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -6912,32 +6697,32 @@
       <c r="D39" s="2"/>
     </row>
     <row r="40" spans="1:4" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="60"/>
-      <c r="B40" s="61"/>
-      <c r="C40" s="62"/>
+      <c r="A40" s="56"/>
+      <c r="B40" s="57"/>
+      <c r="C40" s="58"/>
       <c r="D40" s="2"/>
     </row>
     <row r="41" spans="1:4" ht="13.5" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="63" t="s">
+      <c r="A41" s="59" t="s">
+        <v>102</v>
+      </c>
+      <c r="B41" s="60" t="s">
         <v>103</v>
       </c>
-      <c r="B41" s="64" t="s">
+      <c r="C41" s="74" t="s">
         <v>104</v>
       </c>
-      <c r="C41" s="82" t="s">
-        <v>105</v>
-      </c>
-      <c r="D41" s="58"/>
-    </row>
-    <row r="42" spans="1:4" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D41" s="54"/>
+    </row>
+    <row r="42" spans="1:4" ht="12.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="27" t="s">
         <v>70</v>
       </c>
       <c r="B42" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="C42" s="83"/>
-      <c r="D42" s="58"/>
+      <c r="C42" s="75"/>
+      <c r="D42" s="54"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="27" t="s">
@@ -6946,8 +6731,8 @@
       <c r="B43" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="C43" s="83"/>
-      <c r="D43" s="58"/>
+      <c r="C43" s="75"/>
+      <c r="D43" s="54"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="27" t="s">
@@ -6956,8 +6741,8 @@
       <c r="B44" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="C44" s="83"/>
-      <c r="D44" s="58"/>
+      <c r="C44" s="75"/>
+      <c r="D44" s="54"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="27" t="s">
@@ -6966,8 +6751,8 @@
       <c r="B45" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="C45" s="83"/>
-      <c r="D45" s="58"/>
+      <c r="C45" s="75"/>
+      <c r="D45" s="54"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="27" t="s">
@@ -6976,8 +6761,8 @@
       <c r="B46" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="C46" s="83"/>
-      <c r="D46" s="58"/>
+      <c r="C46" s="75"/>
+      <c r="D46" s="54"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="27" t="s">
@@ -6986,8 +6771,8 @@
       <c r="B47" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="C47" s="83"/>
-      <c r="D47" s="58"/>
+      <c r="C47" s="75"/>
+      <c r="D47" s="54"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="27" t="s">
@@ -6996,8 +6781,8 @@
       <c r="B48" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="C48" s="83"/>
-      <c r="D48" s="58"/>
+      <c r="C48" s="75"/>
+      <c r="D48" s="54"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="27" t="s">
@@ -7006,8 +6791,8 @@
       <c r="B49" s="28" t="s">
         <v>59</v>
       </c>
-      <c r="C49" s="83"/>
-      <c r="D49" s="58"/>
+      <c r="C49" s="75"/>
+      <c r="D49" s="54"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="27" t="s">
@@ -7016,8 +6801,8 @@
       <c r="B50" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="C50" s="83"/>
-      <c r="D50" s="58"/>
+      <c r="C50" s="75"/>
+      <c r="D50" s="54"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="27" t="s">
@@ -7026,8 +6811,8 @@
       <c r="B51" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="C51" s="83"/>
-      <c r="D51" s="58"/>
+      <c r="C51" s="75"/>
+      <c r="D51" s="54"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="27" t="s">
@@ -7036,8 +6821,8 @@
       <c r="B52" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="C52" s="83"/>
-      <c r="D52" s="58"/>
+      <c r="C52" s="75"/>
+      <c r="D52" s="54"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="27" t="s">
@@ -7046,8 +6831,8 @@
       <c r="B53" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="C53" s="83"/>
-      <c r="D53" s="58"/>
+      <c r="C53" s="75"/>
+      <c r="D53" s="54"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="27" t="s">
@@ -7056,8 +6841,8 @@
       <c r="B54" s="28" t="s">
         <v>64</v>
       </c>
-      <c r="C54" s="83"/>
-      <c r="D54" s="58"/>
+      <c r="C54" s="75"/>
+      <c r="D54" s="54"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="27" t="s">
@@ -7066,8 +6851,8 @@
       <c r="B55" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="C55" s="83"/>
-      <c r="D55" s="58"/>
+      <c r="C55" s="75"/>
+      <c r="D55" s="54"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="27" t="s">
@@ -7076,8 +6861,8 @@
       <c r="B56" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="C56" s="83"/>
-      <c r="D56" s="58"/>
+      <c r="C56" s="75"/>
+      <c r="D56" s="54"/>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="27" t="s">
@@ -7086,8 +6871,8 @@
       <c r="B57" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="C57" s="83"/>
-      <c r="D57" s="58"/>
+      <c r="C57" s="75"/>
+      <c r="D57" s="54"/>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="27" t="s">
@@ -7096,8 +6881,8 @@
       <c r="B58" s="28" t="s">
         <v>68</v>
       </c>
-      <c r="C58" s="83"/>
-      <c r="D58" s="58"/>
+      <c r="C58" s="75"/>
+      <c r="D58" s="54"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="27" t="s">
@@ -7106,33 +6891,33 @@
       <c r="B59" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="C59" s="83"/>
-      <c r="D59" s="58"/>
+      <c r="C59" s="75"/>
+      <c r="D59" s="54"/>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="27" t="s">
         <v>87</v>
       </c>
       <c r="B60" s="28" t="s">
-        <v>110</v>
-      </c>
-      <c r="C60" s="83"/>
-      <c r="D60" s="58"/>
+        <v>108</v>
+      </c>
+      <c r="C60" s="75"/>
+      <c r="D60" s="54"/>
     </row>
     <row r="61" spans="1:7" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="54" t="s">
+      <c r="A61" s="50" t="s">
         <v>88</v>
       </c>
-      <c r="B61" s="55" t="s">
-        <v>111</v>
-      </c>
-      <c r="C61" s="84"/>
-      <c r="D61" s="59"/>
-    </row>
-    <row r="62" spans="1:7" s="56" customFormat="1" ht="13" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="57"/>
-      <c r="B62" s="57"/>
-      <c r="C62" s="57"/>
+      <c r="B61" s="51" t="s">
+        <v>109</v>
+      </c>
+      <c r="C61" s="76"/>
+      <c r="D61" s="55"/>
+    </row>
+    <row r="62" spans="1:7" s="52" customFormat="1" ht="13" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="53"/>
+      <c r="B62" s="53"/>
+      <c r="C62" s="53"/>
     </row>
     <row r="63" spans="1:7" ht="6.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="10"/>
@@ -7144,7 +6929,7 @@
       <c r="G63" s="11"/>
     </row>
     <row r="65" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A65" s="45" t="s">
+      <c r="A65" s="41" t="s">
         <v>53</v>
       </c>
     </row>
@@ -7180,7 +6965,7 @@
       <c r="G69" s="11"/>
     </row>
     <row r="71" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A71" s="45" t="s">
+      <c r="A71" s="41" t="s">
         <v>42</v>
       </c>
     </row>
@@ -10120,7 +9905,7 @@
     <mergeCell ref="B15:G15"/>
     <mergeCell ref="C27:F28"/>
   </mergeCells>
-  <phoneticPr fontId="13" type="noConversion"/>
+  <phoneticPr fontId="12" type="noConversion"/>
   <conditionalFormatting sqref="E73:E480">
     <cfRule type="expression" dxfId="4" priority="6">
       <formula>($B$66/$E73)&gt;(0.5*$B$67)</formula>
@@ -10174,7 +9959,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{6B4F2C76-705B-43CC-89D4-F55E07A162C8}">
           <x14:formula1>
-            <xm:f>'Linked Values'!$A$3:$A$13</xm:f>
+            <xm:f>'Linked Values'!$A$3:$A$14</xm:f>
           </x14:formula1>
           <xm:sqref>B7:G17</xm:sqref>
         </x14:dataValidation>
@@ -10186,10 +9971,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CBCE2FF-AC7E-47F6-AFA7-5759B53B3059}">
-  <dimension ref="A1:D40"/>
+  <dimension ref="A1:D41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="A5" sqref="A5:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -10200,12 +9985,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="24" customFormat="1" ht="18" x14ac:dyDescent="0.4">
-      <c r="A1" s="87" t="s">
+      <c r="A1" s="79" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="87"/>
-      <c r="C1" s="87"/>
-      <c r="D1" s="87"/>
+      <c r="B1" s="79"/>
+      <c r="C1" s="79"/>
+      <c r="D1" s="79"/>
     </row>
     <row r="2" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
@@ -10221,10 +10006,10 @@
     </row>
     <row r="3" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>95</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>96</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="8" t="s">
@@ -10233,18 +10018,18 @@
     </row>
     <row r="4" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A4" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="B4" s="8"/>
+        <v>30</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>47</v>
+      </c>
       <c r="C4" s="8"/>
       <c r="D4" s="8" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="8" t="s">
-        <v>107</v>
-      </c>
+      <c r="A5" s="8"/>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
       <c r="D5" s="8" t="s">
@@ -10252,11 +10037,11 @@
       </c>
     </row>
     <row r="6" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="39" t="s">
-        <v>153</v>
-      </c>
-      <c r="B6" s="39" t="s">
-        <v>94</v>
+      <c r="A6" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="36" t="s">
+        <v>49</v>
       </c>
       <c r="C6" s="8"/>
       <c r="D6" s="8" t="s">
@@ -10264,11 +10049,11 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="39" t="s">
-        <v>31</v>
-      </c>
-      <c r="B7" s="39" t="s">
-        <v>49</v>
+      <c r="A7" s="36" t="s">
+        <v>134</v>
+      </c>
+      <c r="B7" s="36" t="s">
+        <v>93</v>
       </c>
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
@@ -10284,58 +10069,50 @@
       <c r="D8" s="8"/>
     </row>
     <row r="9" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>94</v>
-      </c>
       <c r="C9" s="8"/>
       <c r="D9" s="8"/>
     </row>
     <row r="10" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A10" s="8" t="s">
-        <v>31</v>
+        <v>140</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>49</v>
+        <v>149</v>
       </c>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
     </row>
     <row r="11" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A11" s="8" t="s">
-        <v>30</v>
+        <v>113</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>47</v>
+        <v>150</v>
       </c>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
     </row>
     <row r="12" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>109</v>
-      </c>
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
     </row>
     <row r="13" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A13" s="8" t="s">
-        <v>97</v>
+        <v>106</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="C13" s="8"/>
       <c r="D13" s="8"/>
     </row>
     <row r="14" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="8"/>
-      <c r="B14" s="8"/>
+      <c r="A14" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>97</v>
+      </c>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
     </row>
@@ -10494,6 +10271,10 @@
       <c r="B40" s="8"/>
       <c r="C40" s="8"/>
       <c r="D40" s="8"/>
+    </row>
+    <row r="41" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A41" s="8"/>
+      <c r="B41" s="8"/>
     </row>
   </sheetData>
   <autoFilter ref="A2:B2" xr:uid="{17BFE908-7FFA-4697-8D4E-ABB14ED1A3B9}">
@@ -10504,6 +10285,7 @@
   <mergeCells count="1">
     <mergeCell ref="A1:D1"/>
   </mergeCells>
+  <phoneticPr fontId="20" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Update API to 2.11
</commit_message>
<xml_diff>
--- a/Docs/Opentrons Program Templates.xlsx
+++ b/Docs/Opentrons Program Templates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://adminliveunc-my.sharepoint.com/personal/dennis_ad_unc_edu/Documents/Projects/Programs/Opentrons_Programs/Docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="39" documentId="8_{EF6BFD9A-6ED8-462D-A0F5-E40DF4AE02BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CE5AD7AC-8E6C-4A2E-87C9-AEA972B66591}"/>
+  <xr:revisionPtr revIDLastSave="45" documentId="8_{EF6BFD9A-6ED8-462D-A0F5-E40DF4AE02BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{98F43322-E1CB-481C-BB38-5D6875C62B72}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="152">
   <si>
     <t>Source Well</t>
   </si>
@@ -478,10 +478,10 @@
     <t>2 mL Screw Cap Tubes</t>
   </si>
   <si>
-    <t xml:space="preserve"> v0.8.0</t>
-  </si>
-  <si>
     <t>--WaterResWell</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> v0.8.1</t>
   </si>
 </sst>
 </file>
@@ -811,7 +811,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -944,13 +944,7 @@
     <xf numFmtId="2" fontId="7" fillId="6" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -958,6 +952,12 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="180"/>
@@ -977,74 +977,46 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="22">
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="0.0"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
       <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -1146,18 +1118,68 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
       <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1222,27 +1244,6 @@
       </fill>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1257,46 +1258,46 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{DED5D25C-9472-45DF-A5A9-7AE013ADEDBE}" name="Table145" displayName="Table145" ref="A63:F159" totalsRowShown="0" headerRowDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{DED5D25C-9472-45DF-A5A9-7AE013ADEDBE}" name="Table145" displayName="Table145" ref="A63:F159" totalsRowShown="0" headerRowDxfId="21">
   <autoFilter ref="A63:F159" xr:uid="{E9F71635-090B-4C48-B890-1CC5A8BA778F}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{6612BCA6-F4EF-4AEA-9AD0-76196FD98128}" name="# Source Slot"/>
     <tableColumn id="2" xr3:uid="{5F3EDDD0-EEFB-4C72-BFFB-FE7C21AD55A4}" name="Source Well"/>
     <tableColumn id="3" xr3:uid="{C4F715B5-092C-4402-8CEE-00EA82DFB39D}" name="Sample Name"/>
-    <tableColumn id="4" xr3:uid="{84ACEE16-885F-421C-9A1E-F0D15E2C7A09}" name="Concentration ng/uL" dataDxfId="17"/>
-    <tableColumn id="5" xr3:uid="{2188F77B-A461-4751-ADE0-A1432AFC9E78}" name="Target(s)" dataDxfId="16"/>
-    <tableColumn id="6" xr3:uid="{C1FA056C-8826-486C-B642-AB895FD3075E}" name="Replicates" dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{84ACEE16-885F-421C-9A1E-F0D15E2C7A09}" name="Concentration ng/uL" dataDxfId="20"/>
+    <tableColumn id="5" xr3:uid="{2188F77B-A461-4751-ADE0-A1432AFC9E78}" name="Target(s)" dataDxfId="19"/>
+    <tableColumn id="6" xr3:uid="{C1FA056C-8826-486C-B642-AB895FD3075E}" name="Replicates" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6E2D2C82-AED1-4EFD-B514-45C88869B632}" name="Table1" displayName="Table1" ref="A51:F459" totalsRowShown="0" headerRowDxfId="12">
-  <autoFilter ref="A51:F459" xr:uid="{E9F71635-090B-4C48-B890-1CC5A8BA778F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6E2D2C82-AED1-4EFD-B514-45C88869B632}" name="Table1" displayName="Table1" ref="A52:F460" totalsRowShown="0" headerRowDxfId="17">
+  <autoFilter ref="A52:F460" xr:uid="{E9F71635-090B-4C48-B890-1CC5A8BA778F}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{869EDE9B-E883-4A3E-BC84-177627B77820}" name="# Source Slot"/>
     <tableColumn id="2" xr3:uid="{BFF29CE8-BC36-441D-BF7C-4D3ECA705071}" name="Source Well"/>
     <tableColumn id="3" xr3:uid="{BE3B5A50-56B7-458D-A1B8-EA325514A953}" name="Sample"/>
-    <tableColumn id="4" xr3:uid="{51C9CB7B-3C83-4DF7-B90E-3B3B2F0517EB}" name="Concentration ng/uL" dataDxfId="11"/>
-    <tableColumn id="5" xr3:uid="{F1CA2FD2-DD2B-44E5-934D-9BDE08DCFF66}" name="Destination Slot" dataDxfId="10"/>
-    <tableColumn id="6" xr3:uid="{7F589CB2-9FD4-4968-8CE1-91953E95F345}" name="Destination Well" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{51C9CB7B-3C83-4DF7-B90E-3B3B2F0517EB}" name="Concentration ng/uL" dataDxfId="16"/>
+    <tableColumn id="5" xr3:uid="{F1CA2FD2-DD2B-44E5-934D-9BDE08DCFF66}" name="Destination Slot" dataDxfId="15"/>
+    <tableColumn id="6" xr3:uid="{7F589CB2-9FD4-4968-8CE1-91953E95F345}" name="Destination Well" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4A1EA636-4A66-4384-BAA4-76D238021771}" name="Table13" displayName="Table13" ref="A72:G480" totalsRowShown="0" headerRowDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4A1EA636-4A66-4384-BAA4-76D238021771}" name="Table13" displayName="Table13" ref="A72:G480" totalsRowShown="0" headerRowDxfId="13">
   <autoFilter ref="A72:G480" xr:uid="{E9F71635-090B-4C48-B890-1CC5A8BA778F}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{F86BB3DB-CF90-48B8-8F35-E42977442672}" name="# Source Slot"/>
     <tableColumn id="2" xr3:uid="{C0F53F8F-C6A8-4F67-BF04-2D1C3AE40DC7}" name="Source Well"/>
     <tableColumn id="8" xr3:uid="{466B28CD-7413-41AF-A6D9-1A9460F0F6F4}" name="Index"/>
     <tableColumn id="3" xr3:uid="{FB50DE30-1861-4AAD-B46A-522A9F77B092}" name="Sample"/>
-    <tableColumn id="4" xr3:uid="{624B6C14-EDFA-405E-9149-7A4DAA0A5782}" name="Concentration ng/uL" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{A82E5DDD-FDEB-4967-8780-CF48E4C9A4DF}" name="Destination Slot" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{28DE797A-4F93-44BF-AC9A-BA038C116648}" name="Destination Well" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{624B6C14-EDFA-405E-9149-7A4DAA0A5782}" name="Concentration ng/uL" dataDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{A82E5DDD-FDEB-4967-8780-CF48E4C9A4DF}" name="Destination Slot" dataDxfId="11"/>
+    <tableColumn id="6" xr3:uid="{28DE797A-4F93-44BF-AC9A-BA038C116648}" name="Destination Well" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1526,24 +1527,24 @@
       <c r="B1" s="62" t="s">
         <v>136</v>
       </c>
-      <c r="C1" s="81" t="s">
+      <c r="C1" s="79" t="s">
         <v>40</v>
       </c>
-      <c r="D1" s="81"/>
-      <c r="E1" s="81"/>
-      <c r="F1" s="81"/>
+      <c r="D1" s="79"/>
+      <c r="E1" s="79"/>
+      <c r="F1" s="79"/>
     </row>
     <row r="2" spans="1:6" ht="13" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>132</v>
       </c>
       <c r="B2" s="3"/>
-      <c r="C2" s="81" t="s">
+      <c r="C2" s="79" t="s">
         <v>50</v>
       </c>
-      <c r="D2" s="81"/>
-      <c r="E2" s="81"/>
-      <c r="F2" s="81"/>
+      <c r="D2" s="79"/>
+      <c r="E2" s="79"/>
+      <c r="F2" s="79"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -1566,123 +1567,123 @@
       <c r="A6" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="B6" s="82" t="s">
+      <c r="B6" s="80" t="s">
         <v>51</v>
       </c>
-      <c r="C6" s="82"/>
-      <c r="D6" s="82"/>
-      <c r="E6" s="82"/>
-      <c r="F6" s="82"/>
+      <c r="C6" s="80"/>
+      <c r="D6" s="80"/>
+      <c r="E6" s="80"/>
+      <c r="F6" s="80"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="79"/>
-      <c r="C7" s="79"/>
-      <c r="D7" s="79"/>
-      <c r="E7" s="79"/>
-      <c r="F7" s="79"/>
+      <c r="B7" s="78"/>
+      <c r="C7" s="78"/>
+      <c r="D7" s="78"/>
+      <c r="E7" s="78"/>
+      <c r="F7" s="78"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="78"/>
-      <c r="C8" s="78"/>
-      <c r="D8" s="78"/>
-      <c r="E8" s="78"/>
-      <c r="F8" s="78"/>
+      <c r="B8" s="81"/>
+      <c r="C8" s="81"/>
+      <c r="D8" s="81"/>
+      <c r="E8" s="81"/>
+      <c r="F8" s="81"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="79"/>
-      <c r="C9" s="79"/>
-      <c r="D9" s="79"/>
-      <c r="E9" s="79"/>
-      <c r="F9" s="79"/>
+      <c r="B9" s="78"/>
+      <c r="C9" s="78"/>
+      <c r="D9" s="78"/>
+      <c r="E9" s="78"/>
+      <c r="F9" s="78"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="78"/>
-      <c r="C10" s="78"/>
-      <c r="D10" s="78"/>
-      <c r="E10" s="78"/>
-      <c r="F10" s="78"/>
+      <c r="B10" s="81"/>
+      <c r="C10" s="81"/>
+      <c r="D10" s="81"/>
+      <c r="E10" s="81"/>
+      <c r="F10" s="81"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="79"/>
-      <c r="C11" s="79"/>
-      <c r="D11" s="79"/>
-      <c r="E11" s="79"/>
-      <c r="F11" s="79"/>
+      <c r="B11" s="78"/>
+      <c r="C11" s="78"/>
+      <c r="D11" s="78"/>
+      <c r="E11" s="78"/>
+      <c r="F11" s="78"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="78"/>
-      <c r="C12" s="78"/>
-      <c r="D12" s="78"/>
-      <c r="E12" s="78"/>
-      <c r="F12" s="78"/>
+      <c r="B12" s="81"/>
+      <c r="C12" s="81"/>
+      <c r="D12" s="81"/>
+      <c r="E12" s="81"/>
+      <c r="F12" s="81"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="79"/>
-      <c r="C13" s="79"/>
-      <c r="D13" s="79"/>
-      <c r="E13" s="79"/>
-      <c r="F13" s="79"/>
+      <c r="B13" s="78"/>
+      <c r="C13" s="78"/>
+      <c r="D13" s="78"/>
+      <c r="E13" s="78"/>
+      <c r="F13" s="78"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="78"/>
-      <c r="C14" s="78"/>
-      <c r="D14" s="78"/>
-      <c r="E14" s="78"/>
-      <c r="F14" s="78"/>
+      <c r="B14" s="81"/>
+      <c r="C14" s="81"/>
+      <c r="D14" s="81"/>
+      <c r="E14" s="81"/>
+      <c r="F14" s="81"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="79"/>
-      <c r="C15" s="79"/>
-      <c r="D15" s="79"/>
-      <c r="E15" s="79"/>
-      <c r="F15" s="79"/>
+      <c r="B15" s="78"/>
+      <c r="C15" s="78"/>
+      <c r="D15" s="78"/>
+      <c r="E15" s="78"/>
+      <c r="F15" s="78"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="78"/>
-      <c r="C16" s="78"/>
-      <c r="D16" s="78"/>
-      <c r="E16" s="78"/>
-      <c r="F16" s="78"/>
+      <c r="B16" s="81"/>
+      <c r="C16" s="81"/>
+      <c r="D16" s="81"/>
+      <c r="E16" s="81"/>
+      <c r="F16" s="81"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="79"/>
-      <c r="C17" s="79"/>
-      <c r="D17" s="79"/>
-      <c r="E17" s="79"/>
-      <c r="F17" s="79"/>
+      <c r="B17" s="78"/>
+      <c r="C17" s="78"/>
+      <c r="D17" s="78"/>
+      <c r="E17" s="78"/>
+      <c r="F17" s="78"/>
     </row>
     <row r="18" spans="1:6" ht="6.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="10"/>
@@ -1744,12 +1745,12 @@
       <c r="B27" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="C27" s="80" t="s">
+      <c r="C27" s="82" t="s">
         <v>112</v>
       </c>
-      <c r="D27" s="80"/>
-      <c r="E27" s="80"/>
-      <c r="F27" s="80"/>
+      <c r="D27" s="82"/>
+      <c r="E27" s="82"/>
+      <c r="F27" s="82"/>
     </row>
     <row r="28" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
@@ -1758,10 +1759,10 @@
       <c r="B28" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="C28" s="80"/>
-      <c r="D28" s="80"/>
-      <c r="E28" s="80"/>
-      <c r="F28" s="80"/>
+      <c r="C28" s="82"/>
+      <c r="D28" s="82"/>
+      <c r="E28" s="82"/>
+      <c r="F28" s="82"/>
     </row>
     <row r="29" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="64" t="s">
@@ -3008,12 +3009,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="B9:F9"/>
-    <mergeCell ref="C1:F1"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="B6:F6"/>
-    <mergeCell ref="B7:F7"/>
-    <mergeCell ref="B8:F8"/>
     <mergeCell ref="B16:F16"/>
     <mergeCell ref="B17:F17"/>
     <mergeCell ref="C27:F28"/>
@@ -3023,19 +3018,25 @@
     <mergeCell ref="B13:F13"/>
     <mergeCell ref="B14:F14"/>
     <mergeCell ref="B15:F15"/>
+    <mergeCell ref="B9:F9"/>
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="B6:F6"/>
+    <mergeCell ref="B7:F7"/>
+    <mergeCell ref="B8:F8"/>
   </mergeCells>
   <conditionalFormatting sqref="D64:D159">
-    <cfRule type="expression" dxfId="21" priority="3">
+    <cfRule type="expression" dxfId="9" priority="3">
       <formula>($B$37/$D64)&gt;(0.5*$B$38)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B3 B21:B22 B34:B35 B37:B38 B27:B28 B46:B47 B43">
-    <cfRule type="containsBlanks" dxfId="20" priority="2">
+    <cfRule type="containsBlanks" dxfId="8" priority="2">
       <formula>LEN(TRIM(B2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B44">
-    <cfRule type="containsBlanks" dxfId="19" priority="1">
+    <cfRule type="containsBlanks" dxfId="7" priority="1">
       <formula>LEN(TRIM(B44))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3073,10 +3074,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B096AE39-CBE9-438B-8EF5-43BA511A3359}">
-  <dimension ref="A1:I568"/>
+  <dimension ref="A1:I569"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -3096,26 +3097,26 @@
         <v>92</v>
       </c>
       <c r="B1" s="62" t="s">
-        <v>150</v>
-      </c>
-      <c r="C1" s="81" t="s">
+        <v>151</v>
+      </c>
+      <c r="C1" s="79" t="s">
         <v>40</v>
       </c>
-      <c r="D1" s="81"/>
-      <c r="E1" s="81"/>
-      <c r="F1" s="81"/>
+      <c r="D1" s="79"/>
+      <c r="E1" s="79"/>
+      <c r="F1" s="79"/>
     </row>
     <row r="2" spans="1:6" ht="13" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>132</v>
       </c>
       <c r="B2" s="3"/>
-      <c r="C2" s="81" t="s">
+      <c r="C2" s="79" t="s">
         <v>50</v>
       </c>
-      <c r="D2" s="81"/>
-      <c r="E2" s="81"/>
-      <c r="F2" s="81"/>
+      <c r="D2" s="79"/>
+      <c r="E2" s="79"/>
+      <c r="F2" s="79"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -3138,123 +3139,123 @@
       <c r="A6" s="49" t="s">
         <v>37</v>
       </c>
-      <c r="B6" s="82" t="s">
+      <c r="B6" s="80" t="s">
         <v>51</v>
       </c>
-      <c r="C6" s="82"/>
-      <c r="D6" s="82"/>
-      <c r="E6" s="82"/>
-      <c r="F6" s="82"/>
+      <c r="C6" s="80"/>
+      <c r="D6" s="80"/>
+      <c r="E6" s="80"/>
+      <c r="F6" s="80"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="79"/>
-      <c r="C7" s="79"/>
-      <c r="D7" s="79"/>
-      <c r="E7" s="79"/>
-      <c r="F7" s="79"/>
+      <c r="B7" s="78"/>
+      <c r="C7" s="78"/>
+      <c r="D7" s="78"/>
+      <c r="E7" s="78"/>
+      <c r="F7" s="78"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="78"/>
-      <c r="C8" s="78"/>
-      <c r="D8" s="78"/>
-      <c r="E8" s="78"/>
-      <c r="F8" s="78"/>
+      <c r="B8" s="81"/>
+      <c r="C8" s="81"/>
+      <c r="D8" s="81"/>
+      <c r="E8" s="81"/>
+      <c r="F8" s="81"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="79"/>
-      <c r="C9" s="79"/>
-      <c r="D9" s="79"/>
-      <c r="E9" s="79"/>
-      <c r="F9" s="79"/>
+      <c r="B9" s="78"/>
+      <c r="C9" s="78"/>
+      <c r="D9" s="78"/>
+      <c r="E9" s="78"/>
+      <c r="F9" s="78"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="78"/>
-      <c r="C10" s="78"/>
-      <c r="D10" s="78"/>
-      <c r="E10" s="78"/>
-      <c r="F10" s="78"/>
+      <c r="B10" s="81"/>
+      <c r="C10" s="81"/>
+      <c r="D10" s="81"/>
+      <c r="E10" s="81"/>
+      <c r="F10" s="81"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="79"/>
-      <c r="C11" s="79"/>
-      <c r="D11" s="79"/>
-      <c r="E11" s="79"/>
-      <c r="F11" s="79"/>
+      <c r="B11" s="78"/>
+      <c r="C11" s="78"/>
+      <c r="D11" s="78"/>
+      <c r="E11" s="78"/>
+      <c r="F11" s="78"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="78"/>
-      <c r="C12" s="78"/>
-      <c r="D12" s="78"/>
-      <c r="E12" s="78"/>
-      <c r="F12" s="78"/>
+      <c r="B12" s="81"/>
+      <c r="C12" s="81"/>
+      <c r="D12" s="81"/>
+      <c r="E12" s="81"/>
+      <c r="F12" s="81"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="79"/>
-      <c r="C13" s="79"/>
-      <c r="D13" s="79"/>
-      <c r="E13" s="79"/>
-      <c r="F13" s="79"/>
+      <c r="B13" s="78"/>
+      <c r="C13" s="78"/>
+      <c r="D13" s="78"/>
+      <c r="E13" s="78"/>
+      <c r="F13" s="78"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="78"/>
-      <c r="C14" s="78"/>
-      <c r="D14" s="78"/>
-      <c r="E14" s="78"/>
-      <c r="F14" s="78"/>
+      <c r="B14" s="81"/>
+      <c r="C14" s="81"/>
+      <c r="D14" s="81"/>
+      <c r="E14" s="81"/>
+      <c r="F14" s="81"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="79"/>
-      <c r="C15" s="79"/>
-      <c r="D15" s="79"/>
-      <c r="E15" s="79"/>
-      <c r="F15" s="79"/>
+      <c r="B15" s="78"/>
+      <c r="C15" s="78"/>
+      <c r="D15" s="78"/>
+      <c r="E15" s="78"/>
+      <c r="F15" s="78"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="78"/>
-      <c r="C16" s="78"/>
-      <c r="D16" s="78"/>
-      <c r="E16" s="78"/>
-      <c r="F16" s="78"/>
+      <c r="B16" s="81"/>
+      <c r="C16" s="81"/>
+      <c r="D16" s="81"/>
+      <c r="E16" s="81"/>
+      <c r="F16" s="81"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="79"/>
-      <c r="C17" s="79"/>
-      <c r="D17" s="79"/>
-      <c r="E17" s="79"/>
-      <c r="F17" s="79"/>
+      <c r="B17" s="78"/>
+      <c r="C17" s="78"/>
+      <c r="D17" s="78"/>
+      <c r="E17" s="78"/>
+      <c r="F17" s="78"/>
     </row>
     <row r="18" spans="1:6" ht="6.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="10"/>
@@ -3318,12 +3319,12 @@
       <c r="B27" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="C27" s="80" t="s">
+      <c r="C27" s="82" t="s">
         <v>112</v>
       </c>
-      <c r="D27" s="80"/>
-      <c r="E27" s="80"/>
-      <c r="F27" s="80"/>
+      <c r="D27" s="82"/>
+      <c r="E27" s="82"/>
+      <c r="F27" s="82"/>
     </row>
     <row r="28" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
@@ -3332,10 +3333,10 @@
       <c r="B28" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="C28" s="80"/>
-      <c r="D28" s="80"/>
-      <c r="E28" s="80"/>
-      <c r="F28" s="80"/>
+      <c r="C28" s="82"/>
+      <c r="D28" s="82"/>
+      <c r="E28" s="82"/>
+      <c r="F28" s="82"/>
     </row>
     <row r="29" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="64" t="s">
@@ -3388,7 +3389,7 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B35" s="5"/>
       <c r="C35" s="2"/>
@@ -3437,91 +3438,89 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B43" s="7"/>
-      <c r="C43" s="2" t="s">
-        <v>20</v>
-      </c>
+        <v>128</v>
+      </c>
+      <c r="B43" s="89"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B44" s="7"/>
       <c r="C44" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B45" s="2"/>
+        <v>21</v>
+      </c>
+      <c r="B45" s="7"/>
       <c r="C45" s="2" t="s">
-        <v>41</v>
+        <v>22</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B46" s="2"/>
+      <c r="C46" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="B47" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="C46" s="2" t="s">
+      <c r="C47" s="2" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="3"/>
-      <c r="C47" s="2"/>
-    </row>
-    <row r="48" spans="1:6" ht="6.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="10"/>
-      <c r="B48" s="11"/>
-      <c r="C48" s="11"/>
-      <c r="D48" s="11"/>
-      <c r="E48" s="11"/>
-      <c r="F48" s="11"/>
-    </row>
-    <row r="50" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A50" s="41" t="s">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="3"/>
+      <c r="C48" s="2"/>
+    </row>
+    <row r="49" spans="1:9" ht="6.65" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="10"/>
+      <c r="B49" s="11"/>
+      <c r="C49" s="11"/>
+      <c r="D49" s="11"/>
+      <c r="E49" s="11"/>
+      <c r="F49" s="11"/>
+    </row>
+    <row r="51" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A51" s="41" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="51" spans="1:9" ht="13" x14ac:dyDescent="0.3">
-      <c r="A51" s="18" t="s">
+    <row r="52" spans="1:9" ht="13" x14ac:dyDescent="0.3">
+      <c r="A52" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="B51" s="19" t="s">
+      <c r="B52" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C51" s="20" t="s">
+      <c r="C52" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="D51" s="20" t="s">
+      <c r="D52" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="E51" s="20" t="s">
+      <c r="E52" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="F51" s="20" t="s">
+      <c r="F52" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="I51" s="1"/>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A52" s="6"/>
-      <c r="B52" s="63"/>
-      <c r="D52" s="7"/>
-      <c r="E52" s="6"/>
-      <c r="F52" s="5"/>
+      <c r="I52" s="1"/>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="6"/>
-      <c r="B53" s="5"/>
-      <c r="C53" s="2"/>
+      <c r="B53" s="63"/>
       <c r="D53" s="7"/>
       <c r="E53" s="6"/>
       <c r="F53" s="5"/>
@@ -3536,7 +3535,7 @@
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="6"/>
-      <c r="B55" s="63"/>
+      <c r="B55" s="5"/>
       <c r="C55" s="2"/>
       <c r="D55" s="7"/>
       <c r="E55" s="6"/>
@@ -3545,9 +3544,10 @@
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="6"/>
       <c r="B56" s="63"/>
+      <c r="C56" s="2"/>
       <c r="D56" s="7"/>
       <c r="E56" s="6"/>
-      <c r="F56" s="63"/>
+      <c r="F56" s="5"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="6"/>
@@ -3691,10 +3691,10 @@
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="6"/>
-      <c r="B77" s="6"/>
+      <c r="B77" s="63"/>
       <c r="D77" s="7"/>
       <c r="E77" s="6"/>
-      <c r="F77" s="6"/>
+      <c r="F77" s="63"/>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="6"/>
@@ -4369,6 +4369,7 @@
       <c r="F173" s="6"/>
     </row>
     <row r="174" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A174" s="6"/>
       <c r="B174" s="6"/>
       <c r="D174" s="7"/>
       <c r="E174" s="6"/>
@@ -4507,6 +4508,7 @@
       <c r="F196" s="6"/>
     </row>
     <row r="197" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B197" s="6"/>
       <c r="D197" s="7"/>
       <c r="E197" s="6"/>
       <c r="F197" s="6"/>
@@ -5822,6 +5824,7 @@
       <c r="F459" s="6"/>
     </row>
     <row r="460" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D460" s="7"/>
       <c r="E460" s="6"/>
       <c r="F460" s="6"/>
     </row>
@@ -6256,6 +6259,10 @@
     <row r="568" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E568" s="6"/>
       <c r="F568" s="6"/>
+    </row>
+    <row r="569" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E569" s="6"/>
+      <c r="F569" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="15">
@@ -6276,18 +6283,18 @@
     <mergeCell ref="B11:F11"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="D52:D459">
-    <cfRule type="expression" dxfId="14" priority="3">
-      <formula>($B$43/$D52)&gt;(0.5*$B$44)</formula>
+  <conditionalFormatting sqref="D53:D460">
+    <cfRule type="expression" dxfId="6" priority="3">
+      <formula>($B$44/$D53)&gt;(0.5*$B$45)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B3 B21:B22 B34:B38 B43:B46 B27:B28">
-    <cfRule type="containsBlanks" dxfId="13" priority="2">
+  <conditionalFormatting sqref="B2:B3 B21:B22 B34:B38 B27:B28 B43:B47">
+    <cfRule type="containsBlanks" dxfId="5" priority="2">
       <formula>LEN(TRIM(B2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B43:B44" xr:uid="{1FDB8583-4725-454C-B804-F0E3C49A8048}">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B43:B45" xr:uid="{1FDB8583-4725-454C-B804-F0E3C49A8048}">
       <formula1>0</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Slot must be between 1 and 11" sqref="B32 B27" xr:uid="{A1CCD96F-92EF-46C5-BC01-61873CD50A4F}"/>
@@ -6387,135 +6394,135 @@
       <c r="A6" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="B6" s="82" t="s">
+      <c r="B6" s="80" t="s">
         <v>51</v>
       </c>
-      <c r="C6" s="82"/>
-      <c r="D6" s="82"/>
-      <c r="E6" s="82"/>
-      <c r="F6" s="82"/>
-      <c r="G6" s="82"/>
+      <c r="C6" s="80"/>
+      <c r="D6" s="80"/>
+      <c r="E6" s="80"/>
+      <c r="F6" s="80"/>
+      <c r="G6" s="80"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="79"/>
-      <c r="C7" s="79"/>
-      <c r="D7" s="79"/>
-      <c r="E7" s="79"/>
-      <c r="F7" s="79"/>
-      <c r="G7" s="79"/>
+      <c r="B7" s="78"/>
+      <c r="C7" s="78"/>
+      <c r="D7" s="78"/>
+      <c r="E7" s="78"/>
+      <c r="F7" s="78"/>
+      <c r="G7" s="78"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="78"/>
-      <c r="C8" s="78"/>
-      <c r="D8" s="78"/>
-      <c r="E8" s="78"/>
-      <c r="F8" s="78"/>
-      <c r="G8" s="78"/>
+      <c r="B8" s="81"/>
+      <c r="C8" s="81"/>
+      <c r="D8" s="81"/>
+      <c r="E8" s="81"/>
+      <c r="F8" s="81"/>
+      <c r="G8" s="81"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="79"/>
-      <c r="C9" s="79"/>
-      <c r="D9" s="79"/>
-      <c r="E9" s="79"/>
-      <c r="F9" s="79"/>
-      <c r="G9" s="79"/>
+      <c r="B9" s="78"/>
+      <c r="C9" s="78"/>
+      <c r="D9" s="78"/>
+      <c r="E9" s="78"/>
+      <c r="F9" s="78"/>
+      <c r="G9" s="78"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="78"/>
-      <c r="C10" s="78"/>
-      <c r="D10" s="78"/>
-      <c r="E10" s="78"/>
-      <c r="F10" s="78"/>
-      <c r="G10" s="78"/>
+      <c r="B10" s="81"/>
+      <c r="C10" s="81"/>
+      <c r="D10" s="81"/>
+      <c r="E10" s="81"/>
+      <c r="F10" s="81"/>
+      <c r="G10" s="81"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="79"/>
-      <c r="C11" s="79"/>
-      <c r="D11" s="79"/>
-      <c r="E11" s="79"/>
-      <c r="F11" s="79"/>
-      <c r="G11" s="79"/>
+      <c r="B11" s="78"/>
+      <c r="C11" s="78"/>
+      <c r="D11" s="78"/>
+      <c r="E11" s="78"/>
+      <c r="F11" s="78"/>
+      <c r="G11" s="78"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="78"/>
-      <c r="C12" s="78"/>
-      <c r="D12" s="78"/>
-      <c r="E12" s="78"/>
-      <c r="F12" s="78"/>
-      <c r="G12" s="78"/>
+      <c r="B12" s="81"/>
+      <c r="C12" s="81"/>
+      <c r="D12" s="81"/>
+      <c r="E12" s="81"/>
+      <c r="F12" s="81"/>
+      <c r="G12" s="81"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="79"/>
-      <c r="C13" s="79"/>
-      <c r="D13" s="79"/>
-      <c r="E13" s="79"/>
-      <c r="F13" s="79"/>
-      <c r="G13" s="79"/>
+      <c r="B13" s="78"/>
+      <c r="C13" s="78"/>
+      <c r="D13" s="78"/>
+      <c r="E13" s="78"/>
+      <c r="F13" s="78"/>
+      <c r="G13" s="78"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="78"/>
-      <c r="C14" s="78"/>
-      <c r="D14" s="78"/>
-      <c r="E14" s="78"/>
-      <c r="F14" s="78"/>
-      <c r="G14" s="78"/>
+      <c r="B14" s="81"/>
+      <c r="C14" s="81"/>
+      <c r="D14" s="81"/>
+      <c r="E14" s="81"/>
+      <c r="F14" s="81"/>
+      <c r="G14" s="81"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="79"/>
-      <c r="C15" s="79"/>
-      <c r="D15" s="79"/>
-      <c r="E15" s="79"/>
-      <c r="F15" s="79"/>
-      <c r="G15" s="79"/>
+      <c r="B15" s="78"/>
+      <c r="C15" s="78"/>
+      <c r="D15" s="78"/>
+      <c r="E15" s="78"/>
+      <c r="F15" s="78"/>
+      <c r="G15" s="78"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="78"/>
-      <c r="C16" s="78"/>
-      <c r="D16" s="78"/>
-      <c r="E16" s="78"/>
-      <c r="F16" s="78"/>
-      <c r="G16" s="78"/>
+      <c r="B16" s="81"/>
+      <c r="C16" s="81"/>
+      <c r="D16" s="81"/>
+      <c r="E16" s="81"/>
+      <c r="F16" s="81"/>
+      <c r="G16" s="81"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="79"/>
-      <c r="C17" s="79"/>
-      <c r="D17" s="79"/>
-      <c r="E17" s="79"/>
-      <c r="F17" s="79"/>
-      <c r="G17" s="79"/>
+      <c r="B17" s="78"/>
+      <c r="C17" s="78"/>
+      <c r="D17" s="78"/>
+      <c r="E17" s="78"/>
+      <c r="F17" s="78"/>
+      <c r="G17" s="78"/>
     </row>
     <row r="18" spans="1:7" ht="6.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="10"/>
@@ -6584,12 +6591,12 @@
       <c r="B27" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="C27" s="80" t="s">
+      <c r="C27" s="82" t="s">
         <v>112</v>
       </c>
-      <c r="D27" s="80"/>
-      <c r="E27" s="80"/>
-      <c r="F27" s="80"/>
+      <c r="D27" s="82"/>
+      <c r="E27" s="82"/>
+      <c r="F27" s="82"/>
     </row>
     <row r="28" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
@@ -6598,10 +6605,10 @@
       <c r="B28" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="C28" s="80"/>
-      <c r="D28" s="80"/>
-      <c r="E28" s="80"/>
-      <c r="F28" s="80"/>
+      <c r="C28" s="82"/>
+      <c r="D28" s="82"/>
+      <c r="E28" s="82"/>
+      <c r="F28" s="82"/>
     </row>
     <row r="29" spans="1:7" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="64" t="s">
@@ -9906,27 +9913,27 @@
   </mergeCells>
   <phoneticPr fontId="12" type="noConversion"/>
   <conditionalFormatting sqref="E73:E480">
-    <cfRule type="expression" dxfId="8" priority="6">
+    <cfRule type="expression" dxfId="4" priority="6">
       <formula>($B$66/$E73)&gt;(0.5*$B$67)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B3 B21:B22 B34 B39 B27:B28">
-    <cfRule type="containsBlanks" dxfId="7" priority="5">
+    <cfRule type="containsBlanks" dxfId="3" priority="5">
       <formula>LEN(TRIM(B2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B66:B67">
-    <cfRule type="containsBlanks" dxfId="6" priority="4">
+    <cfRule type="containsBlanks" dxfId="2" priority="4">
       <formula>LEN(TRIM(B66))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C73:C480">
-    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text=" ">
+    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text=" ">
       <formula>NOT(ISERROR(SEARCH(" ",C73)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B35:B38">
-    <cfRule type="containsBlanks" dxfId="4" priority="2">
+    <cfRule type="containsBlanks" dxfId="0" priority="2">
       <formula>LEN(TRIM(B35))=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
New Labware and Template
</commit_message>
<xml_diff>
--- a/Docs/Opentrons Program Templates.xlsx
+++ b/Docs/Opentrons Program Templates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://adminliveunc-my.sharepoint.com/personal/dennis_ad_unc_edu/Documents/Projects/Programs/Opentrons_Programs/Docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="186" documentId="8_{A09ADE7F-69E7-4EFD-A5B3-C1570A91AFDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7F9EB618-CAEF-4D81-A13A-9C25A6850EFF}"/>
+  <xr:revisionPtr revIDLastSave="194" documentId="8_{A09ADE7F-69E7-4EFD-A5B3-C1570A91AFDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{16673743-E09F-4F87-92CC-7120461AF73E}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plate Layout" sheetId="7" r:id="rId1"/>
@@ -22,7 +22,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Linked Values'!$A$2:$B$2</definedName>
   </definedNames>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191028" calcOnSave="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="150">
   <si>
     <t>Do NOT edit spacing, spelling, or word case.  Doing so will risk run failure!!!</t>
   </si>
@@ -477,13 +477,19 @@
     <t>--TotalReagentVolume</t>
   </si>
   <si>
-    <t>v1.0.1</t>
-  </si>
-  <si>
-    <t>8_well_strip_dilution_tubes</t>
-  </si>
-  <si>
     <t>Uncapped 8-well strip tubes</t>
+  </si>
+  <si>
+    <t>v1.1.0</t>
+  </si>
+  <si>
+    <t>bigwell_96_tuberack_200ul_dilution_tube</t>
+  </si>
+  <si>
+    <t>biorad_ddpcr_96_wellplate_100ul</t>
+  </si>
+  <si>
+    <t>Bio Rad ddPCR Plate</t>
   </si>
 </sst>
 </file>
@@ -1531,8 +1537,8 @@
   </sheetPr>
   <dimension ref="A1:F235"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13:F13"/>
+    <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7:F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1550,7 +1556,7 @@
         <v>139</v>
       </c>
       <c r="B1" s="47" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C1" s="60" t="s">
         <v>0</v>
@@ -3074,17 +3080,17 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{D0F7A710-9AB2-4682-9835-26809308D3E2}">
-          <x14:formula1>
-            <xm:f>'Linked Values'!$A$3:$A$15</xm:f>
-          </x14:formula1>
-          <xm:sqref>B7:F17</xm:sqref>
-        </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{1DA6AA3B-7DA5-4EF1-947E-BB913217EFC3}">
           <x14:formula1>
             <xm:f>'Linked Values'!$D$3:$D$6</xm:f>
           </x14:formula1>
           <xm:sqref>B21:B22</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{D0F7A710-9AB2-4682-9835-26809308D3E2}">
+          <x14:formula1>
+            <xm:f>'Linked Values'!$A$3:$A$16</xm:f>
+          </x14:formula1>
+          <xm:sqref>B7:F17</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3097,7 +3103,7 @@
   <dimension ref="A1:I577"/>
   <sheetViews>
     <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -3117,7 +3123,7 @@
         <v>138</v>
       </c>
       <c r="B1" s="47" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C1" s="60" t="s">
         <v>0</v>
@@ -6814,17 +6820,17 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A369DC21-720B-42E1-9EE8-7F22A83E9525}">
+          <x14:formula1>
+            <xm:f>'Linked Values'!$D$3:$D$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>B21:B22</xm:sqref>
+        </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{77DFBECE-7E49-49D8-BDA3-34A392C2D5A8}">
           <x14:formula1>
             <xm:f>'Linked Values'!$A$3:$A$16</xm:f>
           </x14:formula1>
           <xm:sqref>B7:B17 F7:F17</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A369DC21-720B-42E1-9EE8-7F22A83E9525}">
-          <x14:formula1>
-            <xm:f>'Linked Values'!$D$3:$D$6</xm:f>
-          </x14:formula1>
-          <xm:sqref>B21:B22</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -6837,7 +6843,7 @@
   <dimension ref="A1:I591"/>
   <sheetViews>
     <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:G7"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -6857,7 +6863,7 @@
         <v>142</v>
       </c>
       <c r="B1" s="47" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C1" s="57" t="s">
         <v>0</v>
@@ -10056,12 +10062,6 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{6B4F2C76-705B-43CC-89D4-F55E07A162C8}">
-          <x14:formula1>
-            <xm:f>'Linked Values'!$A$3:$A$15</xm:f>
-          </x14:formula1>
-          <xm:sqref>B7:G17</xm:sqref>
-        </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{03B032EE-0EFF-4AF8-A3C0-EA4AC4B1B7FF}">
           <x14:formula1>
             <xm:f>'Linked Values'!$D$3:$D$5</xm:f>
@@ -10074,6 +10074,12 @@
           </x14:formula1>
           <xm:sqref>B21:B22</xm:sqref>
         </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{6B4F2C76-705B-43CC-89D4-F55E07A162C8}">
+          <x14:formula1>
+            <xm:f>'Linked Values'!$A$3:$A$16</xm:f>
+          </x14:formula1>
+          <xm:sqref>B7:G17</xm:sqref>
+        </x14:dataValidation>
       </x14:dataValidations>
     </ext>
   </extLst>
@@ -10084,8 +10090,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CBCE2FF-AC7E-47F6-AFA7-5759B53B3059}">
   <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -10129,10 +10135,10 @@
     </row>
     <row r="4" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C4" s="7"/>
       <c r="D4" s="7" t="s">
@@ -10152,93 +10158,95 @@
       </c>
     </row>
     <row r="6" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="7"/>
-      <c r="B6" s="7"/>
+      <c r="A6" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>149</v>
+      </c>
       <c r="C6" s="7"/>
       <c r="D6" s="7" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>119</v>
-      </c>
       <c r="C7" s="7"/>
     </row>
     <row r="8" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
     </row>
     <row r="9" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
     </row>
     <row r="10" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>123</v>
+      </c>
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
     </row>
     <row r="11" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>125</v>
-      </c>
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
     </row>
     <row r="12" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A12" s="7" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
     </row>
     <row r="13" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A13" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>127</v>
+      </c>
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
     </row>
     <row r="14" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>129</v>
-      </c>
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
     </row>
     <row r="15" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A15" s="7" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
     </row>
     <row r="16" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="7"/>
-      <c r="B16" s="7"/>
+      <c r="A16" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>131</v>
+      </c>
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
     </row>

</xml_diff>

<commit_message>
Update template to v3.0.1
</commit_message>
<xml_diff>
--- a/Docs/Opentrons Program Templates.xlsx
+++ b/Docs/Opentrons Program Templates.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="343" documentId="8_{A09ADE7F-69E7-4EFD-A5B3-C1570A91AFDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E8FED44F-460C-4E50-84E9-F69EB2F89028}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plate Layout" sheetId="7" r:id="rId1"/>
@@ -1015,6 +1015,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1023,9 +1026,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="180"/>
@@ -1691,7 +1691,7 @@
   </sheetPr>
   <dimension ref="A1:F241"/>
   <sheetViews>
-    <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -1712,24 +1712,24 @@
       <c r="B1" s="46" t="s">
         <v>162</v>
       </c>
-      <c r="C1" s="70" t="s">
+      <c r="C1" s="71" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="70"/>
-      <c r="E1" s="70"/>
-      <c r="F1" s="70"/>
+      <c r="D1" s="71"/>
+      <c r="E1" s="71"/>
+      <c r="F1" s="71"/>
     </row>
     <row r="2" spans="1:6" ht="13" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="3"/>
-      <c r="C2" s="70" t="s">
+      <c r="C2" s="71" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="71"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -1752,123 +1752,123 @@
       <c r="A6" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="71" t="s">
+      <c r="B6" s="72" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="71"/>
-      <c r="D6" s="71"/>
-      <c r="E6" s="71"/>
-      <c r="F6" s="71"/>
+      <c r="C6" s="72"/>
+      <c r="D6" s="72"/>
+      <c r="E6" s="72"/>
+      <c r="F6" s="72"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="69"/>
-      <c r="C7" s="69"/>
-      <c r="D7" s="69"/>
-      <c r="E7" s="69"/>
-      <c r="F7" s="69"/>
+      <c r="B7" s="70"/>
+      <c r="C7" s="70"/>
+      <c r="D7" s="70"/>
+      <c r="E7" s="70"/>
+      <c r="F7" s="70"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="72"/>
-      <c r="C8" s="72"/>
-      <c r="D8" s="72"/>
-      <c r="E8" s="72"/>
-      <c r="F8" s="72"/>
+      <c r="B8" s="69"/>
+      <c r="C8" s="69"/>
+      <c r="D8" s="69"/>
+      <c r="E8" s="69"/>
+      <c r="F8" s="69"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="69"/>
-      <c r="C9" s="69"/>
-      <c r="D9" s="69"/>
-      <c r="E9" s="69"/>
-      <c r="F9" s="69"/>
+      <c r="B9" s="70"/>
+      <c r="C9" s="70"/>
+      <c r="D9" s="70"/>
+      <c r="E9" s="70"/>
+      <c r="F9" s="70"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="72"/>
-      <c r="C10" s="72"/>
-      <c r="D10" s="72"/>
-      <c r="E10" s="72"/>
-      <c r="F10" s="72"/>
+      <c r="B10" s="69"/>
+      <c r="C10" s="69"/>
+      <c r="D10" s="69"/>
+      <c r="E10" s="69"/>
+      <c r="F10" s="69"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="69"/>
-      <c r="C11" s="69"/>
-      <c r="D11" s="69"/>
-      <c r="E11" s="69"/>
-      <c r="F11" s="69"/>
+      <c r="B11" s="70"/>
+      <c r="C11" s="70"/>
+      <c r="D11" s="70"/>
+      <c r="E11" s="70"/>
+      <c r="F11" s="70"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="72"/>
-      <c r="C12" s="72"/>
-      <c r="D12" s="72"/>
-      <c r="E12" s="72"/>
-      <c r="F12" s="72"/>
+      <c r="B12" s="69"/>
+      <c r="C12" s="69"/>
+      <c r="D12" s="69"/>
+      <c r="E12" s="69"/>
+      <c r="F12" s="69"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="69"/>
-      <c r="C13" s="69"/>
-      <c r="D13" s="69"/>
-      <c r="E13" s="69"/>
-      <c r="F13" s="69"/>
+      <c r="B13" s="70"/>
+      <c r="C13" s="70"/>
+      <c r="D13" s="70"/>
+      <c r="E13" s="70"/>
+      <c r="F13" s="70"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="72"/>
-      <c r="C14" s="72"/>
-      <c r="D14" s="72"/>
-      <c r="E14" s="72"/>
-      <c r="F14" s="72"/>
+      <c r="B14" s="69"/>
+      <c r="C14" s="69"/>
+      <c r="D14" s="69"/>
+      <c r="E14" s="69"/>
+      <c r="F14" s="69"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="69"/>
-      <c r="C15" s="69"/>
-      <c r="D15" s="69"/>
-      <c r="E15" s="69"/>
-      <c r="F15" s="69"/>
+      <c r="B15" s="70"/>
+      <c r="C15" s="70"/>
+      <c r="D15" s="70"/>
+      <c r="E15" s="70"/>
+      <c r="F15" s="70"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="72"/>
-      <c r="C16" s="72"/>
-      <c r="D16" s="72"/>
-      <c r="E16" s="72"/>
-      <c r="F16" s="72"/>
+      <c r="B16" s="69"/>
+      <c r="C16" s="69"/>
+      <c r="D16" s="69"/>
+      <c r="E16" s="69"/>
+      <c r="F16" s="69"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="69"/>
-      <c r="C17" s="69"/>
-      <c r="D17" s="69"/>
-      <c r="E17" s="69"/>
-      <c r="F17" s="69"/>
+      <c r="B17" s="70"/>
+      <c r="C17" s="70"/>
+      <c r="D17" s="70"/>
+      <c r="E17" s="70"/>
+      <c r="F17" s="70"/>
     </row>
     <row r="18" spans="1:6" ht="6.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="9"/>
@@ -1932,12 +1932,12 @@
       <c r="B27" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="72" t="s">
+      <c r="C27" s="69" t="s">
         <v>25</v>
       </c>
-      <c r="D27" s="72"/>
-      <c r="E27" s="72"/>
-      <c r="F27" s="72"/>
+      <c r="D27" s="69"/>
+      <c r="E27" s="69"/>
+      <c r="F27" s="69"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="s">
@@ -1946,10 +1946,10 @@
       <c r="B28" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C28" s="72"/>
-      <c r="D28" s="72"/>
-      <c r="E28" s="72"/>
-      <c r="F28" s="72"/>
+      <c r="C28" s="69"/>
+      <c r="D28" s="69"/>
+      <c r="E28" s="69"/>
+      <c r="F28" s="69"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="s">
@@ -3241,6 +3241,12 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="B9:F9"/>
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="B6:F6"/>
+    <mergeCell ref="B7:F7"/>
+    <mergeCell ref="B8:F8"/>
     <mergeCell ref="B16:F16"/>
     <mergeCell ref="B17:F17"/>
     <mergeCell ref="C27:F28"/>
@@ -3250,12 +3256,6 @@
     <mergeCell ref="B13:F13"/>
     <mergeCell ref="B14:F14"/>
     <mergeCell ref="B15:F15"/>
-    <mergeCell ref="B9:F9"/>
-    <mergeCell ref="C1:F1"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="B6:F6"/>
-    <mergeCell ref="B7:F7"/>
-    <mergeCell ref="B8:F8"/>
   </mergeCells>
   <conditionalFormatting sqref="B2:B3 B21:B22 B27:B29 B40:B43">
     <cfRule type="containsBlanks" dxfId="14" priority="8">
@@ -3334,24 +3334,24 @@
       <c r="B1" s="46" t="s">
         <v>162</v>
       </c>
-      <c r="C1" s="70" t="s">
+      <c r="C1" s="71" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="70"/>
-      <c r="E1" s="70"/>
-      <c r="F1" s="70"/>
+      <c r="D1" s="71"/>
+      <c r="E1" s="71"/>
+      <c r="F1" s="71"/>
     </row>
     <row r="2" spans="1:7" ht="13" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="3"/>
-      <c r="C2" s="70" t="s">
+      <c r="C2" s="71" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="71"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -3375,12 +3375,12 @@
       <c r="A6" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="71" t="s">
+      <c r="B6" s="72" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="71"/>
-      <c r="D6" s="71"/>
-      <c r="E6" s="71"/>
+      <c r="C6" s="72"/>
+      <c r="D6" s="72"/>
+      <c r="E6" s="72"/>
       <c r="F6" s="18"/>
       <c r="G6" s="18"/>
     </row>
@@ -3388,110 +3388,110 @@
       <c r="A7" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="69"/>
-      <c r="C7" s="69"/>
-      <c r="D7" s="69"/>
-      <c r="E7" s="69"/>
+      <c r="B7" s="70"/>
+      <c r="C7" s="70"/>
+      <c r="D7" s="70"/>
+      <c r="E7" s="70"/>
       <c r="F7" s="57"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="72"/>
-      <c r="C8" s="72"/>
-      <c r="D8" s="72"/>
-      <c r="E8" s="72"/>
+      <c r="B8" s="69"/>
+      <c r="C8" s="69"/>
+      <c r="D8" s="69"/>
+      <c r="E8" s="69"/>
       <c r="F8" s="57"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="69"/>
-      <c r="C9" s="69"/>
-      <c r="D9" s="69"/>
-      <c r="E9" s="69"/>
+      <c r="B9" s="70"/>
+      <c r="C9" s="70"/>
+      <c r="D9" s="70"/>
+      <c r="E9" s="70"/>
       <c r="F9" s="57"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="72"/>
-      <c r="C10" s="72"/>
-      <c r="D10" s="72"/>
-      <c r="E10" s="72"/>
+      <c r="B10" s="69"/>
+      <c r="C10" s="69"/>
+      <c r="D10" s="69"/>
+      <c r="E10" s="69"/>
       <c r="F10" s="57"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="69"/>
-      <c r="C11" s="69"/>
-      <c r="D11" s="69"/>
-      <c r="E11" s="69"/>
+      <c r="B11" s="70"/>
+      <c r="C11" s="70"/>
+      <c r="D11" s="70"/>
+      <c r="E11" s="70"/>
       <c r="F11" s="57"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="72"/>
-      <c r="C12" s="72"/>
-      <c r="D12" s="72"/>
-      <c r="E12" s="72"/>
+      <c r="B12" s="69"/>
+      <c r="C12" s="69"/>
+      <c r="D12" s="69"/>
+      <c r="E12" s="69"/>
       <c r="F12" s="57"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="69"/>
-      <c r="C13" s="69"/>
-      <c r="D13" s="69"/>
-      <c r="E13" s="69"/>
+      <c r="B13" s="70"/>
+      <c r="C13" s="70"/>
+      <c r="D13" s="70"/>
+      <c r="E13" s="70"/>
       <c r="F13" s="57"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="72"/>
-      <c r="C14" s="72"/>
-      <c r="D14" s="72"/>
-      <c r="E14" s="72"/>
+      <c r="B14" s="69"/>
+      <c r="C14" s="69"/>
+      <c r="D14" s="69"/>
+      <c r="E14" s="69"/>
       <c r="F14" s="57"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="69"/>
-      <c r="C15" s="69"/>
-      <c r="D15" s="69"/>
-      <c r="E15" s="69"/>
+      <c r="B15" s="70"/>
+      <c r="C15" s="70"/>
+      <c r="D15" s="70"/>
+      <c r="E15" s="70"/>
       <c r="F15" s="57"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="72"/>
-      <c r="C16" s="72"/>
-      <c r="D16" s="72"/>
-      <c r="E16" s="72"/>
+      <c r="B16" s="69"/>
+      <c r="C16" s="69"/>
+      <c r="D16" s="69"/>
+      <c r="E16" s="69"/>
       <c r="F16" s="57"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="69"/>
-      <c r="C17" s="69"/>
-      <c r="D17" s="69"/>
-      <c r="E17" s="69"/>
+      <c r="B17" s="70"/>
+      <c r="C17" s="70"/>
+      <c r="D17" s="70"/>
+      <c r="E17" s="70"/>
       <c r="F17" s="57"/>
     </row>
     <row r="18" spans="1:7" ht="6.65" customHeight="1" x14ac:dyDescent="0.25">
@@ -3559,12 +3559,12 @@
       <c r="B27" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="72" t="s">
+      <c r="C27" s="69" t="s">
         <v>25</v>
       </c>
-      <c r="D27" s="72"/>
-      <c r="E27" s="72"/>
-      <c r="F27" s="72"/>
+      <c r="D27" s="69"/>
+      <c r="E27" s="69"/>
+      <c r="F27" s="69"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="s">
@@ -3573,10 +3573,10 @@
       <c r="B28" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="C28" s="72"/>
-      <c r="D28" s="72"/>
-      <c r="E28" s="72"/>
-      <c r="F28" s="72"/>
+      <c r="C28" s="69"/>
+      <c r="D28" s="69"/>
+      <c r="E28" s="69"/>
+      <c r="F28" s="69"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="s">
@@ -7046,6 +7046,11 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B8:E8"/>
     <mergeCell ref="B9:E9"/>
     <mergeCell ref="C27:F28"/>
     <mergeCell ref="B15:E15"/>
@@ -7056,11 +7061,6 @@
     <mergeCell ref="B12:E12"/>
     <mergeCell ref="B13:E13"/>
     <mergeCell ref="B14:E14"/>
-    <mergeCell ref="C1:F1"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B8:E8"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="B2:B3 B27:B28 B40:B42 B58:B61">
@@ -7128,7 +7128,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{547A22CE-6B5B-419C-B571-1556B7859EB9}">
   <dimension ref="A1:I596"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+    <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -7193,135 +7193,135 @@
       <c r="A6" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="71" t="s">
+      <c r="B6" s="72" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="71"/>
-      <c r="D6" s="71"/>
-      <c r="E6" s="71"/>
-      <c r="F6" s="71"/>
-      <c r="G6" s="71"/>
+      <c r="C6" s="72"/>
+      <c r="D6" s="72"/>
+      <c r="E6" s="72"/>
+      <c r="F6" s="72"/>
+      <c r="G6" s="72"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="69"/>
-      <c r="C7" s="69"/>
-      <c r="D7" s="69"/>
-      <c r="E7" s="69"/>
-      <c r="F7" s="69"/>
-      <c r="G7" s="69"/>
+      <c r="B7" s="70"/>
+      <c r="C7" s="70"/>
+      <c r="D7" s="70"/>
+      <c r="E7" s="70"/>
+      <c r="F7" s="70"/>
+      <c r="G7" s="70"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="72"/>
-      <c r="C8" s="72"/>
-      <c r="D8" s="72"/>
-      <c r="E8" s="72"/>
-      <c r="F8" s="72"/>
-      <c r="G8" s="72"/>
+      <c r="B8" s="69"/>
+      <c r="C8" s="69"/>
+      <c r="D8" s="69"/>
+      <c r="E8" s="69"/>
+      <c r="F8" s="69"/>
+      <c r="G8" s="69"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="69"/>
-      <c r="C9" s="69"/>
-      <c r="D9" s="69"/>
-      <c r="E9" s="69"/>
-      <c r="F9" s="69"/>
-      <c r="G9" s="69"/>
+      <c r="B9" s="70"/>
+      <c r="C9" s="70"/>
+      <c r="D9" s="70"/>
+      <c r="E9" s="70"/>
+      <c r="F9" s="70"/>
+      <c r="G9" s="70"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="72"/>
-      <c r="C10" s="72"/>
-      <c r="D10" s="72"/>
-      <c r="E10" s="72"/>
-      <c r="F10" s="72"/>
-      <c r="G10" s="72"/>
+      <c r="B10" s="69"/>
+      <c r="C10" s="69"/>
+      <c r="D10" s="69"/>
+      <c r="E10" s="69"/>
+      <c r="F10" s="69"/>
+      <c r="G10" s="69"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="69"/>
-      <c r="C11" s="69"/>
-      <c r="D11" s="69"/>
-      <c r="E11" s="69"/>
-      <c r="F11" s="69"/>
-      <c r="G11" s="69"/>
+      <c r="B11" s="70"/>
+      <c r="C11" s="70"/>
+      <c r="D11" s="70"/>
+      <c r="E11" s="70"/>
+      <c r="F11" s="70"/>
+      <c r="G11" s="70"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="72"/>
-      <c r="C12" s="72"/>
-      <c r="D12" s="72"/>
-      <c r="E12" s="72"/>
-      <c r="F12" s="72"/>
-      <c r="G12" s="72"/>
+      <c r="B12" s="69"/>
+      <c r="C12" s="69"/>
+      <c r="D12" s="69"/>
+      <c r="E12" s="69"/>
+      <c r="F12" s="69"/>
+      <c r="G12" s="69"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="69"/>
-      <c r="C13" s="69"/>
-      <c r="D13" s="69"/>
-      <c r="E13" s="69"/>
-      <c r="F13" s="69"/>
-      <c r="G13" s="69"/>
+      <c r="B13" s="70"/>
+      <c r="C13" s="70"/>
+      <c r="D13" s="70"/>
+      <c r="E13" s="70"/>
+      <c r="F13" s="70"/>
+      <c r="G13" s="70"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="72"/>
-      <c r="C14" s="72"/>
-      <c r="D14" s="72"/>
-      <c r="E14" s="72"/>
-      <c r="F14" s="72"/>
-      <c r="G14" s="72"/>
+      <c r="B14" s="69"/>
+      <c r="C14" s="69"/>
+      <c r="D14" s="69"/>
+      <c r="E14" s="69"/>
+      <c r="F14" s="69"/>
+      <c r="G14" s="69"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="69"/>
-      <c r="C15" s="69"/>
-      <c r="D15" s="69"/>
-      <c r="E15" s="69"/>
-      <c r="F15" s="69"/>
-      <c r="G15" s="69"/>
+      <c r="B15" s="70"/>
+      <c r="C15" s="70"/>
+      <c r="D15" s="70"/>
+      <c r="E15" s="70"/>
+      <c r="F15" s="70"/>
+      <c r="G15" s="70"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="72"/>
-      <c r="C16" s="72"/>
-      <c r="D16" s="72"/>
-      <c r="E16" s="72"/>
-      <c r="F16" s="72"/>
-      <c r="G16" s="72"/>
+      <c r="B16" s="69"/>
+      <c r="C16" s="69"/>
+      <c r="D16" s="69"/>
+      <c r="E16" s="69"/>
+      <c r="F16" s="69"/>
+      <c r="G16" s="69"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="69"/>
-      <c r="C17" s="69"/>
-      <c r="D17" s="69"/>
-      <c r="E17" s="69"/>
-      <c r="F17" s="69"/>
-      <c r="G17" s="69"/>
+      <c r="B17" s="70"/>
+      <c r="C17" s="70"/>
+      <c r="D17" s="70"/>
+      <c r="E17" s="70"/>
+      <c r="F17" s="70"/>
+      <c r="G17" s="70"/>
     </row>
     <row r="18" spans="1:7" ht="6.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="9"/>
@@ -7389,12 +7389,12 @@
       <c r="B27" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="72" t="s">
+      <c r="C27" s="69" t="s">
         <v>25</v>
       </c>
-      <c r="D27" s="72"/>
-      <c r="E27" s="72"/>
-      <c r="F27" s="72"/>
+      <c r="D27" s="69"/>
+      <c r="E27" s="69"/>
+      <c r="F27" s="69"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="s">
@@ -7403,10 +7403,10 @@
       <c r="B28" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C28" s="72"/>
-      <c r="D28" s="72"/>
-      <c r="E28" s="72"/>
-      <c r="F28" s="72"/>
+      <c r="C28" s="69"/>
+      <c r="D28" s="69"/>
+      <c r="E28" s="69"/>
+      <c r="F28" s="69"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="s">

</xml_diff>

<commit_message>
Fix issues with Indexing PCR
</commit_message>
<xml_diff>
--- a/Docs/Opentrons Program Templates.xlsx
+++ b/Docs/Opentrons Program Templates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://adminliveunc-my.sharepoint.com/personal/dennis_ad_unc_edu/Documents/Projects/Programs/Opentrons_Programs/Docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="8_{258D0F35-6C49-4B4F-B70E-038B83016047}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7967AE4C-48F5-4453-82B6-ECF6821638A6}"/>
+  <xr:revisionPtr revIDLastSave="23" documentId="8_{258D0F35-6C49-4B4F-B70E-038B83016047}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{05925AEC-76E3-4656-9D17-0A03B3D7FCC1}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,6 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Linked Values'!$A$2:$B$2</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -41,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="165">
   <si>
     <t>Do NOT edit spacing, spelling, or word case.  Doing so will risk run failure!!!</t>
   </si>
@@ -373,12 +372,6 @@
     <t>Our 8-well PCR Tubes in one of the yellow racks</t>
   </si>
   <si>
-    <t>stacked_96_well</t>
-  </si>
-  <si>
-    <t>Gupta lab 96-well PCR plate stacked on a 96 well rack</t>
-  </si>
-  <si>
     <t>opentrons_96_tiprack_300ul</t>
   </si>
   <si>
@@ -524,6 +517,24 @@
   </si>
   <si>
     <t>v2.0.0</t>
+  </si>
+  <si>
+    <t>opentrons_15_tuberack_5000ul_Diamond_Tubes</t>
+  </si>
+  <si>
+    <t>5 mL Red Capped Conical tubes in one of the 15 well Opentrons racks</t>
+  </si>
+  <si>
+    <t>stacked_vwr_96_well_semi_skirt_96_well_plate_200ul</t>
+  </si>
+  <si>
+    <t>VWR Brand 96-well PCR plate stacked on a 96 well rack</t>
+  </si>
+  <si>
+    <t>stacked_eppendorf_twin.tec_pcr_96_well_plate_200ul</t>
+  </si>
+  <si>
+    <t>Eppendorf Twin Tec 96-well PCR plate stacked on a 96 well rack</t>
   </si>
 </sst>
 </file>
@@ -1009,6 +1020,9 @@
     <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1017,9 +1031,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="180"/>
@@ -1696,8 +1707,8 @@
   </sheetPr>
   <dimension ref="A1:F241"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41:B41"/>
+    <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1712,29 +1723,29 @@
   <sheetData>
     <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.4">
       <c r="A1" s="44" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B1" s="45" t="s">
-        <v>157</v>
-      </c>
-      <c r="C1" s="70" t="s">
+        <v>155</v>
+      </c>
+      <c r="C1" s="71" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="70"/>
-      <c r="E1" s="70"/>
-      <c r="F1" s="70"/>
+      <c r="D1" s="71"/>
+      <c r="E1" s="71"/>
+      <c r="F1" s="71"/>
     </row>
     <row r="2" spans="1:6" ht="13" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="3"/>
-      <c r="C2" s="70" t="s">
+      <c r="C2" s="71" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="71"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -1757,123 +1768,123 @@
       <c r="A6" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="71" t="s">
+      <c r="B6" s="72" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="71"/>
-      <c r="D6" s="71"/>
-      <c r="E6" s="71"/>
-      <c r="F6" s="71"/>
+      <c r="C6" s="72"/>
+      <c r="D6" s="72"/>
+      <c r="E6" s="72"/>
+      <c r="F6" s="72"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="69"/>
-      <c r="C7" s="69"/>
-      <c r="D7" s="69"/>
-      <c r="E7" s="69"/>
-      <c r="F7" s="69"/>
+      <c r="B7" s="70"/>
+      <c r="C7" s="70"/>
+      <c r="D7" s="70"/>
+      <c r="E7" s="70"/>
+      <c r="F7" s="70"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="72"/>
-      <c r="C8" s="72"/>
-      <c r="D8" s="72"/>
-      <c r="E8" s="72"/>
-      <c r="F8" s="72"/>
+      <c r="B8" s="69"/>
+      <c r="C8" s="69"/>
+      <c r="D8" s="69"/>
+      <c r="E8" s="69"/>
+      <c r="F8" s="69"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="69"/>
-      <c r="C9" s="69"/>
-      <c r="D9" s="69"/>
-      <c r="E9" s="69"/>
-      <c r="F9" s="69"/>
+      <c r="B9" s="70"/>
+      <c r="C9" s="70"/>
+      <c r="D9" s="70"/>
+      <c r="E9" s="70"/>
+      <c r="F9" s="70"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="72"/>
-      <c r="C10" s="72"/>
-      <c r="D10" s="72"/>
-      <c r="E10" s="72"/>
-      <c r="F10" s="72"/>
+      <c r="B10" s="69"/>
+      <c r="C10" s="69"/>
+      <c r="D10" s="69"/>
+      <c r="E10" s="69"/>
+      <c r="F10" s="69"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="69"/>
-      <c r="C11" s="69"/>
-      <c r="D11" s="69"/>
-      <c r="E11" s="69"/>
-      <c r="F11" s="69"/>
+      <c r="B11" s="70"/>
+      <c r="C11" s="70"/>
+      <c r="D11" s="70"/>
+      <c r="E11" s="70"/>
+      <c r="F11" s="70"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="72"/>
-      <c r="C12" s="72"/>
-      <c r="D12" s="72"/>
-      <c r="E12" s="72"/>
-      <c r="F12" s="72"/>
+      <c r="B12" s="69"/>
+      <c r="C12" s="69"/>
+      <c r="D12" s="69"/>
+      <c r="E12" s="69"/>
+      <c r="F12" s="69"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="69"/>
-      <c r="C13" s="69"/>
-      <c r="D13" s="69"/>
-      <c r="E13" s="69"/>
-      <c r="F13" s="69"/>
+      <c r="B13" s="70"/>
+      <c r="C13" s="70"/>
+      <c r="D13" s="70"/>
+      <c r="E13" s="70"/>
+      <c r="F13" s="70"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="72"/>
-      <c r="C14" s="72"/>
-      <c r="D14" s="72"/>
-      <c r="E14" s="72"/>
-      <c r="F14" s="72"/>
+      <c r="B14" s="69"/>
+      <c r="C14" s="69"/>
+      <c r="D14" s="69"/>
+      <c r="E14" s="69"/>
+      <c r="F14" s="69"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="69"/>
-      <c r="C15" s="69"/>
-      <c r="D15" s="69"/>
-      <c r="E15" s="69"/>
-      <c r="F15" s="69"/>
+      <c r="B15" s="70"/>
+      <c r="C15" s="70"/>
+      <c r="D15" s="70"/>
+      <c r="E15" s="70"/>
+      <c r="F15" s="70"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="72"/>
-      <c r="C16" s="72"/>
-      <c r="D16" s="72"/>
-      <c r="E16" s="72"/>
-      <c r="F16" s="72"/>
+      <c r="B16" s="69"/>
+      <c r="C16" s="69"/>
+      <c r="D16" s="69"/>
+      <c r="E16" s="69"/>
+      <c r="F16" s="69"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="69"/>
-      <c r="C17" s="69"/>
-      <c r="D17" s="69"/>
-      <c r="E17" s="69"/>
-      <c r="F17" s="69"/>
+      <c r="B17" s="70"/>
+      <c r="C17" s="70"/>
+      <c r="D17" s="70"/>
+      <c r="E17" s="70"/>
+      <c r="F17" s="70"/>
     </row>
     <row r="18" spans="1:6" ht="6.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="9"/>
@@ -1891,12 +1902,12 @@
         <v>17</v>
       </c>
       <c r="B20" s="67" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B21" t="s">
         <v>19</v>
@@ -1904,7 +1915,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>18</v>
@@ -1937,12 +1948,12 @@
       <c r="B27" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C27" s="72" t="s">
+      <c r="C27" s="69" t="s">
         <v>23</v>
       </c>
-      <c r="D27" s="72"/>
-      <c r="E27" s="72"/>
-      <c r="F27" s="72"/>
+      <c r="D27" s="69"/>
+      <c r="E27" s="69"/>
+      <c r="F27" s="69"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="s">
@@ -1951,10 +1962,10 @@
       <c r="B28" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C28" s="72"/>
-      <c r="D28" s="72"/>
-      <c r="E28" s="72"/>
-      <c r="F28" s="72"/>
+      <c r="C28" s="69"/>
+      <c r="D28" s="69"/>
+      <c r="E28" s="69"/>
+      <c r="F28" s="69"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="s">
@@ -1990,7 +2001,7 @@
     </row>
     <row r="33" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A33" s="26" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D33" s="54"/>
       <c r="E33" s="54"/>
@@ -1998,7 +2009,7 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B34" s="63" t="b">
         <v>0</v>
@@ -2009,11 +2020,11 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B35" s="64"/>
       <c r="C35" s="64" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D35" s="65"/>
       <c r="E35" s="65"/>
@@ -2095,12 +2106,12 @@
       </c>
       <c r="B48" s="5"/>
       <c r="D48" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>33</v>
@@ -2140,7 +2151,7 @@
         <v>42</v>
       </c>
       <c r="D53" s="46" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
@@ -3246,6 +3257,12 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="B9:F9"/>
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="B6:F6"/>
+    <mergeCell ref="B7:F7"/>
+    <mergeCell ref="B8:F8"/>
     <mergeCell ref="B16:F16"/>
     <mergeCell ref="B17:F17"/>
     <mergeCell ref="C27:F28"/>
@@ -3255,12 +3272,6 @@
     <mergeCell ref="B13:F13"/>
     <mergeCell ref="B14:F14"/>
     <mergeCell ref="B15:F15"/>
-    <mergeCell ref="B9:F9"/>
-    <mergeCell ref="C1:F1"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="B6:F6"/>
-    <mergeCell ref="B7:F7"/>
-    <mergeCell ref="B8:F8"/>
   </mergeCells>
   <conditionalFormatting sqref="B2:B3 B21:B22 B27:B29 B40:B43">
     <cfRule type="containsBlanks" dxfId="16" priority="8">
@@ -3280,7 +3291,7 @@
       <formula>LEN(TRIM(B48))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations disablePrompts="1" count="2">
+  <dataValidations count="2">
     <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B40:B43" xr:uid="{B2A947F0-E894-4D3B-A808-2C4D31EEFB25}">
       <formula1>0</formula1>
     </dataValidation>
@@ -3293,7 +3304,7 @@
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="2">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{1DA6AA3B-7DA5-4EF1-947E-BB913217EFC3}">
           <x14:formula1>
             <xm:f>'Linked Values'!$D$3:$D$6</xm:f>
@@ -3302,7 +3313,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Labware Selection" prompt="Select labware from list" xr:uid="{D0F7A710-9AB2-4682-9835-26809308D3E2}">
           <x14:formula1>
-            <xm:f>'Linked Values'!$A$3:$A$30</xm:f>
+            <xm:f>'Linked Values'!$A$3:$A$31</xm:f>
           </x14:formula1>
           <xm:sqref>B7:F17</xm:sqref>
         </x14:dataValidation>
@@ -3334,29 +3345,29 @@
   <sheetData>
     <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.4">
       <c r="A1" s="44" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B1" s="45" t="s">
-        <v>157</v>
-      </c>
-      <c r="C1" s="70" t="s">
+        <v>155</v>
+      </c>
+      <c r="C1" s="71" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="70"/>
-      <c r="E1" s="70"/>
-      <c r="F1" s="70"/>
+      <c r="D1" s="71"/>
+      <c r="E1" s="71"/>
+      <c r="F1" s="71"/>
     </row>
     <row r="2" spans="1:7" ht="13" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="3"/>
-      <c r="C2" s="70" t="s">
+      <c r="C2" s="71" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="71"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -3380,12 +3391,12 @@
       <c r="A6" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="71" t="s">
+      <c r="B6" s="72" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="71"/>
-      <c r="D6" s="71"/>
-      <c r="E6" s="71"/>
+      <c r="C6" s="72"/>
+      <c r="D6" s="72"/>
+      <c r="E6" s="72"/>
       <c r="F6" s="17"/>
       <c r="G6" s="17"/>
     </row>
@@ -3393,110 +3404,110 @@
       <c r="A7" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="69"/>
-      <c r="C7" s="69"/>
-      <c r="D7" s="69"/>
-      <c r="E7" s="69"/>
+      <c r="B7" s="70"/>
+      <c r="C7" s="70"/>
+      <c r="D7" s="70"/>
+      <c r="E7" s="70"/>
       <c r="F7" s="56"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="72"/>
-      <c r="C8" s="72"/>
-      <c r="D8" s="72"/>
-      <c r="E8" s="72"/>
+      <c r="B8" s="69"/>
+      <c r="C8" s="69"/>
+      <c r="D8" s="69"/>
+      <c r="E8" s="69"/>
       <c r="F8" s="56"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="69"/>
-      <c r="C9" s="69"/>
-      <c r="D9" s="69"/>
-      <c r="E9" s="69"/>
+      <c r="B9" s="70"/>
+      <c r="C9" s="70"/>
+      <c r="D9" s="70"/>
+      <c r="E9" s="70"/>
       <c r="F9" s="56"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="72"/>
-      <c r="C10" s="72"/>
-      <c r="D10" s="72"/>
-      <c r="E10" s="72"/>
+      <c r="B10" s="69"/>
+      <c r="C10" s="69"/>
+      <c r="D10" s="69"/>
+      <c r="E10" s="69"/>
       <c r="F10" s="56"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="69"/>
-      <c r="C11" s="69"/>
-      <c r="D11" s="69"/>
-      <c r="E11" s="69"/>
+      <c r="B11" s="70"/>
+      <c r="C11" s="70"/>
+      <c r="D11" s="70"/>
+      <c r="E11" s="70"/>
       <c r="F11" s="56"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="72"/>
-      <c r="C12" s="72"/>
-      <c r="D12" s="72"/>
-      <c r="E12" s="72"/>
+      <c r="B12" s="69"/>
+      <c r="C12" s="69"/>
+      <c r="D12" s="69"/>
+      <c r="E12" s="69"/>
       <c r="F12" s="56"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="69"/>
-      <c r="C13" s="69"/>
-      <c r="D13" s="69"/>
-      <c r="E13" s="69"/>
+      <c r="B13" s="70"/>
+      <c r="C13" s="70"/>
+      <c r="D13" s="70"/>
+      <c r="E13" s="70"/>
       <c r="F13" s="56"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="72"/>
-      <c r="C14" s="72"/>
-      <c r="D14" s="72"/>
-      <c r="E14" s="72"/>
+      <c r="B14" s="69"/>
+      <c r="C14" s="69"/>
+      <c r="D14" s="69"/>
+      <c r="E14" s="69"/>
       <c r="F14" s="56"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="69"/>
-      <c r="C15" s="69"/>
-      <c r="D15" s="69"/>
-      <c r="E15" s="69"/>
+      <c r="B15" s="70"/>
+      <c r="C15" s="70"/>
+      <c r="D15" s="70"/>
+      <c r="E15" s="70"/>
       <c r="F15" s="56"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="72"/>
-      <c r="C16" s="72"/>
-      <c r="D16" s="72"/>
-      <c r="E16" s="72"/>
+      <c r="B16" s="69"/>
+      <c r="C16" s="69"/>
+      <c r="D16" s="69"/>
+      <c r="E16" s="69"/>
       <c r="F16" s="56"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="69"/>
-      <c r="C17" s="69"/>
-      <c r="D17" s="69"/>
-      <c r="E17" s="69"/>
+      <c r="B17" s="70"/>
+      <c r="C17" s="70"/>
+      <c r="D17" s="70"/>
+      <c r="E17" s="70"/>
       <c r="F17" s="56"/>
     </row>
     <row r="18" spans="1:7" ht="6.65" customHeight="1" x14ac:dyDescent="0.25">
@@ -3516,13 +3527,13 @@
         <v>17</v>
       </c>
       <c r="B20" s="67" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C20" s="7"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B21" t="s">
         <v>19</v>
@@ -3530,7 +3541,7 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>18</v>
@@ -3564,12 +3575,12 @@
       <c r="B27" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C27" s="72" t="s">
+      <c r="C27" s="69" t="s">
         <v>23</v>
       </c>
-      <c r="D27" s="72"/>
-      <c r="E27" s="72"/>
-      <c r="F27" s="72"/>
+      <c r="D27" s="69"/>
+      <c r="E27" s="69"/>
+      <c r="F27" s="69"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="s">
@@ -3578,10 +3589,10 @@
       <c r="B28" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C28" s="72"/>
-      <c r="D28" s="72"/>
-      <c r="E28" s="72"/>
-      <c r="F28" s="72"/>
+      <c r="C28" s="69"/>
+      <c r="D28" s="69"/>
+      <c r="E28" s="69"/>
+      <c r="F28" s="69"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="s">
@@ -3624,7 +3635,7 @@
     </row>
     <row r="33" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A33" s="26" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D33" s="54"/>
       <c r="E33" s="54"/>
@@ -3632,7 +3643,7 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B34" s="63" t="b">
         <v>0</v>
@@ -3643,11 +3654,11 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B35" s="64"/>
       <c r="C35" s="64" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D35" s="65"/>
       <c r="E35" s="65"/>
@@ -3719,7 +3730,7 @@
         <v>42</v>
       </c>
       <c r="D44" s="46" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E44" s="28"/>
       <c r="F44" s="28"/>
@@ -3838,20 +3849,20 @@
         <v>33</v>
       </c>
       <c r="D60" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F60" s="3"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B61" s="6"/>
       <c r="C61" s="2" t="s">
         <v>33</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
@@ -3886,13 +3897,13 @@
         <v>57</v>
       </c>
       <c r="E66" s="15" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F66" s="15" t="s">
         <v>59</v>
       </c>
       <c r="G66" s="15" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
@@ -7051,6 +7062,11 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B8:E8"/>
     <mergeCell ref="B9:E9"/>
     <mergeCell ref="C27:F28"/>
     <mergeCell ref="B15:E15"/>
@@ -7061,11 +7077,6 @@
     <mergeCell ref="B12:E12"/>
     <mergeCell ref="B13:E13"/>
     <mergeCell ref="B14:E14"/>
-    <mergeCell ref="C1:F1"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B8:E8"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="B2:B3 B27:B28 B40:B42 B58:B61">
@@ -7113,13 +7124,13 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{77DFBECE-7E49-49D8-BDA3-34A392C2D5A8}">
           <x14:formula1>
-            <xm:f>'Linked Values'!$A$3:$A$22</xm:f>
+            <xm:f>'Linked Values'!$A$3:$A$23</xm:f>
           </x14:formula1>
           <xm:sqref>F7:F17</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Labware Selection" prompt="Select labware from list" xr:uid="{C95FA7BD-C91E-4674-87EB-14764875FDA8}">
           <x14:formula1>
-            <xm:f>'Linked Values'!$A$3:$A$30</xm:f>
+            <xm:f>'Linked Values'!$A$3:$A$31</xm:f>
           </x14:formula1>
           <xm:sqref>B7:E17</xm:sqref>
         </x14:dataValidation>
@@ -7134,7 +7145,7 @@
   <dimension ref="A1:G597"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="G77" sqref="G77"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -7151,10 +7162,10 @@
   <sheetData>
     <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.4">
       <c r="A1" s="44" t="s">
+        <v>156</v>
+      </c>
+      <c r="B1" s="45" t="s">
         <v>158</v>
-      </c>
-      <c r="B1" s="45" t="s">
-        <v>160</v>
       </c>
       <c r="C1" s="55" t="s">
         <v>0</v>
@@ -7198,147 +7209,135 @@
       <c r="A6" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="71" t="s">
+      <c r="B6" s="72" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="71"/>
-      <c r="D6" s="71"/>
-      <c r="E6" s="71"/>
-      <c r="F6" s="71"/>
-      <c r="G6" s="71"/>
+      <c r="C6" s="72"/>
+      <c r="D6" s="72"/>
+      <c r="E6" s="72"/>
+      <c r="F6" s="72"/>
+      <c r="G6" s="72"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="69" t="s">
-        <v>116</v>
-      </c>
-      <c r="C7" s="69"/>
-      <c r="D7" s="69"/>
-      <c r="E7" s="69"/>
-      <c r="F7" s="69"/>
-      <c r="G7" s="69"/>
+      <c r="B7" s="70"/>
+      <c r="C7" s="70"/>
+      <c r="D7" s="70"/>
+      <c r="E7" s="70"/>
+      <c r="F7" s="70"/>
+      <c r="G7" s="70"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="72" t="s">
-        <v>134</v>
-      </c>
-      <c r="C8" s="72"/>
-      <c r="D8" s="72"/>
-      <c r="E8" s="72"/>
-      <c r="F8" s="72"/>
-      <c r="G8" s="72"/>
+      <c r="B8" s="69"/>
+      <c r="C8" s="69"/>
+      <c r="D8" s="69"/>
+      <c r="E8" s="69"/>
+      <c r="F8" s="69"/>
+      <c r="G8" s="69"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="69" t="s">
-        <v>156</v>
-      </c>
-      <c r="C9" s="69"/>
-      <c r="D9" s="69"/>
-      <c r="E9" s="69"/>
-      <c r="F9" s="69"/>
-      <c r="G9" s="69"/>
+      <c r="B9" s="70"/>
+      <c r="C9" s="70"/>
+      <c r="D9" s="70"/>
+      <c r="E9" s="70"/>
+      <c r="F9" s="70"/>
+      <c r="G9" s="70"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="72"/>
-      <c r="C10" s="72"/>
-      <c r="D10" s="72"/>
-      <c r="E10" s="72"/>
-      <c r="F10" s="72"/>
-      <c r="G10" s="72"/>
+      <c r="B10" s="69"/>
+      <c r="C10" s="69"/>
+      <c r="D10" s="69"/>
+      <c r="E10" s="69"/>
+      <c r="F10" s="69"/>
+      <c r="G10" s="69"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="69" t="s">
-        <v>143</v>
-      </c>
-      <c r="C11" s="69"/>
-      <c r="D11" s="69"/>
-      <c r="E11" s="69"/>
-      <c r="F11" s="69"/>
-      <c r="G11" s="69"/>
+      <c r="B11" s="70"/>
+      <c r="C11" s="70"/>
+      <c r="D11" s="70"/>
+      <c r="E11" s="70"/>
+      <c r="F11" s="70"/>
+      <c r="G11" s="70"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="72" t="s">
-        <v>112</v>
-      </c>
-      <c r="C12" s="72"/>
-      <c r="D12" s="72"/>
-      <c r="E12" s="72"/>
-      <c r="F12" s="72"/>
-      <c r="G12" s="72"/>
+      <c r="B12" s="69"/>
+      <c r="C12" s="69"/>
+      <c r="D12" s="69"/>
+      <c r="E12" s="69"/>
+      <c r="F12" s="69"/>
+      <c r="G12" s="69"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="69"/>
-      <c r="C13" s="69"/>
-      <c r="D13" s="69"/>
-      <c r="E13" s="69"/>
-      <c r="F13" s="69"/>
-      <c r="G13" s="69"/>
+      <c r="B13" s="70"/>
+      <c r="C13" s="70"/>
+      <c r="D13" s="70"/>
+      <c r="E13" s="70"/>
+      <c r="F13" s="70"/>
+      <c r="G13" s="70"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="72"/>
-      <c r="C14" s="72"/>
-      <c r="D14" s="72"/>
-      <c r="E14" s="72"/>
-      <c r="F14" s="72"/>
-      <c r="G14" s="72"/>
+      <c r="B14" s="69"/>
+      <c r="C14" s="69"/>
+      <c r="D14" s="69"/>
+      <c r="E14" s="69"/>
+      <c r="F14" s="69"/>
+      <c r="G14" s="69"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="69" t="s">
-        <v>139</v>
-      </c>
-      <c r="C15" s="69"/>
-      <c r="D15" s="69"/>
-      <c r="E15" s="69"/>
-      <c r="F15" s="69"/>
-      <c r="G15" s="69"/>
+      <c r="B15" s="70"/>
+      <c r="C15" s="70"/>
+      <c r="D15" s="70"/>
+      <c r="E15" s="70"/>
+      <c r="F15" s="70"/>
+      <c r="G15" s="70"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="72"/>
-      <c r="C16" s="72"/>
-      <c r="D16" s="72"/>
-      <c r="E16" s="72"/>
-      <c r="F16" s="72"/>
-      <c r="G16" s="72"/>
+      <c r="B16" s="69"/>
+      <c r="C16" s="69"/>
+      <c r="D16" s="69"/>
+      <c r="E16" s="69"/>
+      <c r="F16" s="69"/>
+      <c r="G16" s="69"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="69"/>
-      <c r="C17" s="69"/>
-      <c r="D17" s="69"/>
-      <c r="E17" s="69"/>
-      <c r="F17" s="69"/>
-      <c r="G17" s="69"/>
+      <c r="B17" s="70"/>
+      <c r="C17" s="70"/>
+      <c r="D17" s="70"/>
+      <c r="E17" s="70"/>
+      <c r="F17" s="70"/>
+      <c r="G17" s="70"/>
     </row>
     <row r="18" spans="1:7" ht="6.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="9"/>
@@ -7357,14 +7356,14 @@
         <v>17</v>
       </c>
       <c r="B20" s="67" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C20" s="5"/>
       <c r="D20" s="2"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B21" t="s">
         <v>19</v>
@@ -7372,7 +7371,7 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>18</v>
@@ -7408,12 +7407,12 @@
       <c r="B27" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C27" s="72" t="s">
+      <c r="C27" s="69" t="s">
         <v>23</v>
       </c>
-      <c r="D27" s="72"/>
-      <c r="E27" s="72"/>
-      <c r="F27" s="72"/>
+      <c r="D27" s="69"/>
+      <c r="E27" s="69"/>
+      <c r="F27" s="69"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="s">
@@ -7422,10 +7421,10 @@
       <c r="B28" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C28" s="72"/>
-      <c r="D28" s="72"/>
-      <c r="E28" s="72"/>
-      <c r="F28" s="72"/>
+      <c r="C28" s="69"/>
+      <c r="D28" s="69"/>
+      <c r="E28" s="69"/>
+      <c r="F28" s="69"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="s">
@@ -7460,7 +7459,7 @@
     </row>
     <row r="32" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A32" s="26" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D32" s="54"/>
       <c r="E32" s="54"/>
@@ -7468,7 +7467,7 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B33" s="63" t="b">
         <v>0</v>
@@ -7479,11 +7478,11 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B34" s="64"/>
       <c r="C34" s="64" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D34" s="65"/>
       <c r="E34" s="65"/>
@@ -7545,14 +7544,14 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B42" s="12"/>
       <c r="C42" s="2"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B43" s="12"/>
       <c r="C43" s="2" t="s">
@@ -7561,7 +7560,7 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B44" s="12"/>
       <c r="C44" s="2"/>
@@ -7581,7 +7580,7 @@
         <v>41</v>
       </c>
       <c r="C46" s="73" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D46" s="37"/>
     </row>
@@ -7821,7 +7820,7 @@
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B73" s="6"/>
       <c r="C73" s="2" t="s">
@@ -10450,7 +10449,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{6B4F2C76-705B-43CC-89D4-F55E07A162C8}">
           <x14:formula1>
-            <xm:f>'Linked Values'!$A$3:$A$22</xm:f>
+            <xm:f>'Linked Values'!$A$3:$A$23</xm:f>
           </x14:formula1>
           <xm:sqref>B7:G17</xm:sqref>
         </x14:dataValidation>
@@ -10462,10 +10461,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CBCE2FF-AC7E-47F6-AFA7-5759B53B3059}">
-  <dimension ref="A1:E45"/>
+  <dimension ref="A1:E46"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -10508,10 +10507,10 @@
     </row>
     <row r="4" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A4" s="57" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B4" s="57" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
@@ -10524,10 +10523,10 @@
     </row>
     <row r="6" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A6" s="58" t="s">
-        <v>110</v>
+        <v>163</v>
       </c>
       <c r="B6" s="58" t="s">
-        <v>111</v>
+        <v>164</v>
       </c>
       <c r="C6" s="7"/>
       <c r="D6" s="7" t="s">
@@ -10536,150 +10535,160 @@
     </row>
     <row r="7" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A7" s="58" t="s">
-        <v>135</v>
+        <v>161</v>
       </c>
       <c r="B7" s="58" t="s">
-        <v>137</v>
+        <v>162</v>
       </c>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
     </row>
     <row r="8" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A8" s="58" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="B8" s="58" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
     </row>
     <row r="9" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="58" t="s">
+        <v>138</v>
+      </c>
+      <c r="B9" s="58" t="s">
+        <v>139</v>
+      </c>
       <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
     </row>
     <row r="10" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="59" t="s">
-        <v>136</v>
-      </c>
-      <c r="B10" s="59" t="s">
-        <v>138</v>
-      </c>
       <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
     </row>
     <row r="11" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A11" s="59" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="B11" s="59" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
     </row>
     <row r="12" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A12" s="59" t="s">
+        <v>137</v>
+      </c>
+      <c r="B12" s="59" t="s">
+        <v>140</v>
+      </c>
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
     </row>
     <row r="13" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="60" t="s">
-        <v>112</v>
-      </c>
-      <c r="B13" s="60" t="s">
-        <v>151</v>
-      </c>
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
     </row>
     <row r="14" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A14" s="60" t="s">
-        <v>155</v>
+        <v>110</v>
       </c>
       <c r="B14" s="60" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
     </row>
     <row r="15" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A15" s="60" t="s">
-        <v>143</v>
+        <v>153</v>
       </c>
       <c r="B15" s="60" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
     </row>
     <row r="16" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A16" s="60" t="s">
-        <v>113</v>
+        <v>141</v>
       </c>
       <c r="B16" s="60" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
     </row>
     <row r="17" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A17" s="60" t="s">
+        <v>111</v>
+      </c>
+      <c r="B17" s="60" t="s">
+        <v>147</v>
+      </c>
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
     </row>
     <row r="18" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="61" t="s">
-        <v>114</v>
-      </c>
-      <c r="B18" s="61" t="s">
-        <v>115</v>
-      </c>
       <c r="C18" s="7"/>
       <c r="D18" s="7"/>
     </row>
     <row r="19" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A19" s="61" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B19" s="61" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C19" s="7"/>
       <c r="D19" s="7"/>
     </row>
     <row r="20" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A20" s="61" t="s">
+        <v>114</v>
+      </c>
+      <c r="B20" s="61" t="s">
+        <v>115</v>
+      </c>
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
     </row>
     <row r="21" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A21" s="62" t="s">
-        <v>156</v>
-      </c>
-      <c r="B21" s="62" t="s">
-        <v>118</v>
-      </c>
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
     </row>
     <row r="22" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A22" s="62" t="s">
-        <v>119</v>
+        <v>154</v>
       </c>
       <c r="B22" s="62" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
     </row>
     <row r="23" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A23" s="62" t="s">
+        <v>117</v>
+      </c>
+      <c r="B23" s="62" t="s">
+        <v>118</v>
+      </c>
       <c r="C23" s="7"/>
       <c r="D23" s="7"/>
     </row>
     <row r="24" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A24" s="62" t="s">
+        <v>159</v>
+      </c>
+      <c r="B24" s="62" t="s">
+        <v>160</v>
+      </c>
       <c r="C24" s="7"/>
       <c r="D24" s="7"/>
     </row>
     <row r="25" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A25" s="7"/>
-      <c r="B25" s="7"/>
       <c r="C25" s="7"/>
       <c r="D25" s="7"/>
     </row>
@@ -10800,6 +10809,12 @@
     <row r="45" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A45" s="7"/>
       <c r="B45" s="7"/>
+      <c r="C45" s="7"/>
+      <c r="D45" s="7"/>
+    </row>
+    <row r="46" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A46" s="7"/>
+      <c r="B46" s="7"/>
     </row>
   </sheetData>
   <autoFilter ref="A2:B2" xr:uid="{17BFE908-7FFA-4697-8D4E-ABB14ED1A3B9}">

</xml_diff>

<commit_message>
Add Beithir Template tab
</commit_message>
<xml_diff>
--- a/Docs/Opentrons Program Templates.xlsx
+++ b/Docs/Opentrons Program Templates.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://adminliveunc-my.sharepoint.com/personal/dennis_ad_unc_edu/Documents/Projects/Programs/Opentrons_Programs/Docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="28" documentId="8_{258D0F35-6C49-4B4F-B70E-038B83016047}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FBDB02DE-E83C-48B1-A130-1B41BAE48310}"/>
+  <xr:revisionPtr revIDLastSave="46" documentId="13_ncr:1_{D985E8EB-94F2-4441-A4EC-A5C038F7B2FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{02BBD2DE-30AF-4362-9798-8C5BC16CC580}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plate Layout" sheetId="7" r:id="rId1"/>
-    <sheet name="ddPCR" sheetId="6" r:id="rId2"/>
-    <sheet name="Generic PCR" sheetId="2" r:id="rId3"/>
-    <sheet name="Illumina Indexing" sheetId="4" r:id="rId4"/>
-    <sheet name="Linked Values" sheetId="3" r:id="rId5"/>
+    <sheet name="Beithir ddPCR Template" sheetId="8" r:id="rId2"/>
+    <sheet name="ddPCR" sheetId="6" r:id="rId3"/>
+    <sheet name="Generic PCR" sheetId="2" r:id="rId4"/>
+    <sheet name="Illumina Indexing" sheetId="4" r:id="rId5"/>
+    <sheet name="Linked Values" sheetId="3" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Linked Values'!$A$2:$B$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Linked Values'!$A$2:$B$2</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="171">
   <si>
     <t>Do NOT edit spacing, spelling, or word case.  Doing so will risk run failure!!!</t>
   </si>
@@ -535,6 +536,24 @@
   </si>
   <si>
     <t>opentrons_15_tuberack_5000ul_diamond_tubes</t>
+  </si>
+  <si>
+    <t># Deck Layout</t>
+  </si>
+  <si>
+    <t># Temperature Module Settings</t>
+  </si>
+  <si>
+    <t># Location of Reagents and Volumes</t>
+  </si>
+  <si>
+    <t># ddPCR Parameters</t>
+  </si>
+  <si>
+    <t>Open Plate Layout in a text editor, copy, and paste here</t>
+  </si>
+  <si>
+    <t>Open Beithir parameter output file in a text editor.  Copy all, click on A1 then past</t>
   </si>
 </sst>
 </file>
@@ -545,7 +564,7 @@
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yyyy;@"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -679,6 +698,13 @@
     </font>
     <font>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -900,7 +926,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1023,6 +1049,18 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1047,11 +1085,14 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="29">
+  <dxfs count="34">
     <dxf>
       <fill>
         <patternFill>
@@ -1154,6 +1195,13 @@
       <fill>
         <patternFill patternType="none">
           <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1348,6 +1396,64 @@
       </fill>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1379,46 +1485,61 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{DED5D25C-9472-45DF-A5A9-7AE013ADEDBE}" name="Table145" displayName="Table145" ref="A67:F163" totalsRowShown="0" headerRowDxfId="28">
-  <autoFilter ref="A67:F163" xr:uid="{E9F71635-090B-4C48-B890-1CC5A8BA778F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{A0B8057B-9C21-43B2-BA8C-A379AB01B1F9}" name="Table1454" displayName="Table1454" ref="A58:F154" totalsRowShown="0" headerRowDxfId="33">
+  <autoFilter ref="A58:F154" xr:uid="{E9F71635-090B-4C48-B890-1CC5A8BA778F}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{6612BCA6-F4EF-4AEA-9AD0-76196FD98128}" name="# Source Slot"/>
-    <tableColumn id="2" xr3:uid="{5F3EDDD0-EEFB-4C72-BFFB-FE7C21AD55A4}" name="Source Well"/>
-    <tableColumn id="3" xr3:uid="{C4F715B5-092C-4402-8CEE-00EA82DFB39D}" name="Sample Name"/>
-    <tableColumn id="4" xr3:uid="{84ACEE16-885F-421C-9A1E-F0D15E2C7A09}" name="Concentration ng/uL" dataDxfId="27"/>
-    <tableColumn id="5" xr3:uid="{2188F77B-A461-4751-ADE0-A1432AFC9E78}" name="Target(s)" dataDxfId="26"/>
-    <tableColumn id="6" xr3:uid="{C1FA056C-8826-486C-B642-AB895FD3075E}" name="Replicates" dataDxfId="25"/>
+    <tableColumn id="1" xr3:uid="{C904AA61-E727-4615-8B15-B2DD0C1B4F01}" name="# Source Slot"/>
+    <tableColumn id="2" xr3:uid="{6343DA0C-A287-4A05-8534-DB11EFD5D572}" name="Source Well"/>
+    <tableColumn id="3" xr3:uid="{EE59D56B-CEC9-45C7-900D-7951EED3F38B}" name="Sample Name"/>
+    <tableColumn id="4" xr3:uid="{91258183-8330-47A5-B40E-D96446CD9D04}" name="Concentration ng/uL" dataDxfId="32"/>
+    <tableColumn id="5" xr3:uid="{2400CEFE-D624-4B3F-ADEA-D4ACFCBD7195}" name="Target(s)" dataDxfId="31"/>
+    <tableColumn id="6" xr3:uid="{45E2A527-C789-4A37-B143-6F8CF5C0EA87}" name="Replicates" dataDxfId="30"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6E2D2C82-AED1-4EFD-B514-45C88869B632}" name="Table1" displayName="Table1" ref="A66:G474" totalsRowShown="0" headerRowDxfId="24">
-  <autoFilter ref="A66:G474" xr:uid="{E9F71635-090B-4C48-B890-1CC5A8BA778F}"/>
-  <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{869EDE9B-E883-4A3E-BC84-177627B77820}" name="# Source Slot"/>
-    <tableColumn id="2" xr3:uid="{BFF29CE8-BC36-441D-BF7C-4D3ECA705071}" name="Source Well"/>
-    <tableColumn id="3" xr3:uid="{BE3B5A50-56B7-458D-A1B8-EA325514A953}" name="Sample Name"/>
-    <tableColumn id="4" xr3:uid="{51C9CB7B-3C83-4DF7-B90E-3B3B2F0517EB}" name="Concentration ng/uL" dataDxfId="23"/>
-    <tableColumn id="5" xr3:uid="{F1CA2FD2-DD2B-44E5-934D-9BDE08DCFF66}" name="Targets" dataDxfId="22"/>
-    <tableColumn id="7" xr3:uid="{729081AE-1D1F-419B-BC70-D7092D3EB321}" name="Replicates" dataDxfId="21"/>
-    <tableColumn id="6" xr3:uid="{7F589CB2-9FD4-4968-8CE1-91953E95F345}" name="Template in Rxn (ng)" dataDxfId="20"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{DED5D25C-9472-45DF-A5A9-7AE013ADEDBE}" name="Table145" displayName="Table145" ref="A67:F163" totalsRowShown="0" headerRowDxfId="29">
+  <autoFilter ref="A67:F163" xr:uid="{E9F71635-090B-4C48-B890-1CC5A8BA778F}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{6612BCA6-F4EF-4AEA-9AD0-76196FD98128}" name="# Source Slot"/>
+    <tableColumn id="2" xr3:uid="{5F3EDDD0-EEFB-4C72-BFFB-FE7C21AD55A4}" name="Source Well"/>
+    <tableColumn id="3" xr3:uid="{C4F715B5-092C-4402-8CEE-00EA82DFB39D}" name="Sample Name"/>
+    <tableColumn id="4" xr3:uid="{84ACEE16-885F-421C-9A1E-F0D15E2C7A09}" name="Concentration ng/uL" dataDxfId="28"/>
+    <tableColumn id="5" xr3:uid="{2188F77B-A461-4751-ADE0-A1432AFC9E78}" name="Target(s)" dataDxfId="27"/>
+    <tableColumn id="6" xr3:uid="{C1FA056C-8826-486C-B642-AB895FD3075E}" name="Replicates" dataDxfId="26"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4A1EA636-4A66-4384-BAA4-76D238021771}" name="Table13" displayName="Table13" ref="A80:F488" totalsRowShown="0" headerRowDxfId="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6E2D2C82-AED1-4EFD-B514-45C88869B632}" name="Table1" displayName="Table1" ref="A66:G474" totalsRowShown="0" headerRowDxfId="25">
+  <autoFilter ref="A66:G474" xr:uid="{E9F71635-090B-4C48-B890-1CC5A8BA778F}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{869EDE9B-E883-4A3E-BC84-177627B77820}" name="# Source Slot"/>
+    <tableColumn id="2" xr3:uid="{BFF29CE8-BC36-441D-BF7C-4D3ECA705071}" name="Source Well"/>
+    <tableColumn id="3" xr3:uid="{BE3B5A50-56B7-458D-A1B8-EA325514A953}" name="Sample Name"/>
+    <tableColumn id="4" xr3:uid="{51C9CB7B-3C83-4DF7-B90E-3B3B2F0517EB}" name="Concentration ng/uL" dataDxfId="24"/>
+    <tableColumn id="5" xr3:uid="{F1CA2FD2-DD2B-44E5-934D-9BDE08DCFF66}" name="Targets" dataDxfId="23"/>
+    <tableColumn id="7" xr3:uid="{729081AE-1D1F-419B-BC70-D7092D3EB321}" name="Replicates" dataDxfId="22"/>
+    <tableColumn id="6" xr3:uid="{7F589CB2-9FD4-4968-8CE1-91953E95F345}" name="Template in Rxn (ng)" dataDxfId="21"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4A1EA636-4A66-4384-BAA4-76D238021771}" name="Table13" displayName="Table13" ref="A80:F488" totalsRowShown="0" headerRowDxfId="20">
   <autoFilter ref="A80:F488" xr:uid="{E9F71635-090B-4C48-B890-1CC5A8BA778F}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{F86BB3DB-CF90-48B8-8F35-E42977442672}" name="# Source Slot"/>
     <tableColumn id="2" xr3:uid="{C0F53F8F-C6A8-4F67-BF04-2D1C3AE40DC7}" name="Source Well"/>
     <tableColumn id="8" xr3:uid="{466B28CD-7413-41AF-A6D9-1A9460F0F6F4}" name="Sample Name"/>
     <tableColumn id="3" xr3:uid="{FB50DE30-1861-4AAD-B46A-522A9F77B092}" name="Concentration ng/uL"/>
-    <tableColumn id="4" xr3:uid="{624B6C14-EDFA-405E-9149-7A4DAA0A5782}" name="Index" dataDxfId="18"/>
-    <tableColumn id="6" xr3:uid="{28DE797A-4F93-44BF-AC9A-BA038C116648}" name="Destination Well" dataDxfId="17"/>
+    <tableColumn id="4" xr3:uid="{624B6C14-EDFA-405E-9149-7A4DAA0A5782}" name="Index" dataDxfId="19"/>
+    <tableColumn id="6" xr3:uid="{28DE797A-4F93-44BF-AC9A-BA038C116648}" name="Destination Well" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1690,25 +1811,1570 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5337BE81-82E1-4557-B966-5EA4C274941B}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:M16"/>
   <sheetViews>
-    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0"/>
+    <sheetView zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
+      <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
+      <selection pane="bottomRight" activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="18.1796875" customWidth="1"/>
+    <col min="2" max="2" width="39.1796875" customWidth="1"/>
+    <col min="3" max="3" width="53" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="63.6328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="65.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="68.08984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="66.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="68.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="60.36328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" s="72" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8"/>
+      <c r="M6" s="8"/>
+    </row>
+    <row r="7" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="8"/>
+    </row>
+    <row r="8" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="8"/>
+    </row>
+    <row r="9" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="8"/>
+    </row>
+    <row r="10" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="8"/>
+    </row>
+    <row r="11" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="8"/>
+    </row>
+    <row r="12" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A12" s="8"/>
+    </row>
+    <row r="13" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A13" s="8"/>
+    </row>
+    <row r="14" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A14" s="8"/>
+    </row>
+    <row r="15" spans="1:13" ht="13" x14ac:dyDescent="0.3">
+      <c r="A15" s="72"/>
+    </row>
+    <row r="16" spans="1:13" ht="13" x14ac:dyDescent="0.3">
+      <c r="A16" s="72"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E5D9040-74C4-412D-879C-66A6A599E00E}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:F232"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.453125" customWidth="1"/>
+    <col min="2" max="2" width="16.81640625" customWidth="1"/>
+    <col min="3" max="3" width="19.7265625" customWidth="1"/>
+    <col min="4" max="4" width="22.1796875" customWidth="1"/>
+    <col min="5" max="5" width="19.26953125" customWidth="1"/>
+    <col min="6" max="6" width="20.54296875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.4">
+      <c r="A1" s="44" t="s">
+        <v>168</v>
+      </c>
+      <c r="B1" s="45" t="s">
+        <v>155</v>
+      </c>
+      <c r="C1" s="55" t="s">
+        <v>170</v>
+      </c>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+    </row>
+    <row r="2" spans="1:6" ht="14" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="44"/>
+      <c r="B2" s="45"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="6.65" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="9"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+    </row>
+    <row r="7" spans="1:6" ht="13" x14ac:dyDescent="0.3">
+      <c r="A7" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="B7" s="70"/>
+      <c r="C7" s="70"/>
+      <c r="D7" s="70"/>
+      <c r="E7" s="70"/>
+      <c r="F7" s="70"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="69"/>
+      <c r="C8" s="69"/>
+      <c r="D8" s="69"/>
+      <c r="E8" s="69"/>
+      <c r="F8" s="69"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="54"/>
+      <c r="C9" s="54"/>
+      <c r="D9" s="54"/>
+      <c r="E9" s="54"/>
+      <c r="F9" s="54"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="69"/>
+      <c r="C10" s="69"/>
+      <c r="D10" s="69"/>
+      <c r="E10" s="69"/>
+      <c r="F10" s="69"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="54"/>
+      <c r="C11" s="54"/>
+      <c r="D11" s="54"/>
+      <c r="E11" s="54"/>
+      <c r="F11" s="54"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="69"/>
+      <c r="C12" s="69"/>
+      <c r="D12" s="69"/>
+      <c r="E12" s="69"/>
+      <c r="F12" s="69"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="54"/>
+      <c r="C13" s="54"/>
+      <c r="D13" s="54"/>
+      <c r="E13" s="54"/>
+      <c r="F13" s="54"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="69"/>
+      <c r="C14" s="69"/>
+      <c r="D14" s="69"/>
+      <c r="E14" s="69"/>
+      <c r="F14" s="69"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="54"/>
+      <c r="C15" s="54"/>
+      <c r="D15" s="54"/>
+      <c r="E15" s="54"/>
+      <c r="F15" s="54"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="69"/>
+      <c r="C16" s="69"/>
+      <c r="D16" s="69"/>
+      <c r="E16" s="69"/>
+      <c r="F16" s="69"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="54"/>
+      <c r="C17" s="54"/>
+      <c r="D17" s="54"/>
+      <c r="E17" s="54"/>
+      <c r="F17" s="54"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="69"/>
+      <c r="C18" s="69"/>
+      <c r="D18" s="69"/>
+      <c r="E18" s="69"/>
+      <c r="F18" s="69"/>
+    </row>
+    <row r="19" spans="1:6" ht="6.65" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="9"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+    </row>
+    <row r="21" spans="1:6" s="7" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A21" s="25" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" s="7" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A22" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" s="82">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="3"/>
+    </row>
+    <row r="26" spans="1:6" ht="6.65" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="B26" s="10"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="10"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C27" s="2"/>
+    </row>
+    <row r="28" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A28" s="26" t="s">
+        <v>142</v>
+      </c>
+      <c r="C28" s="2"/>
+    </row>
+    <row r="29" spans="1:6" s="7" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A29" s="3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="C30" s="54"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C31" s="54"/>
+    </row>
+    <row r="32" spans="1:6" ht="6.65" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B32" s="10">
+        <v>2</v>
+      </c>
+      <c r="C32" s="10"/>
+      <c r="D32" s="10"/>
+      <c r="E32" s="10"/>
+      <c r="F32" s="10"/>
+    </row>
+    <row r="33" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A33" s="26" t="s">
+        <v>167</v>
+      </c>
+      <c r="D33" s="54"/>
+      <c r="E33" s="54"/>
+      <c r="F33" s="54"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B34" s="5"/>
+      <c r="D34" s="54"/>
+      <c r="E34" s="54"/>
+      <c r="F34" s="54"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B35" s="5"/>
+      <c r="D35" s="54"/>
+      <c r="E35" s="54"/>
+      <c r="F35" s="54"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B36" s="5"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B37" s="12"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B38" s="5"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B39" s="5"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="B40" s="5"/>
+      <c r="D40" s="54"/>
+      <c r="E40" s="54"/>
+      <c r="F40" s="54"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="66" t="s">
+        <v>30</v>
+      </c>
+      <c r="B41" s="71"/>
+      <c r="C41" s="65"/>
+      <c r="D41" s="65"/>
+      <c r="E41" s="65"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C42" s="65"/>
+      <c r="D42" s="65"/>
+      <c r="E42" s="65"/>
+      <c r="F42" s="65"/>
+    </row>
+    <row r="43" spans="1:6" ht="6.65" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="9"/>
+      <c r="B43" s="10"/>
+      <c r="C43" s="10"/>
+      <c r="D43" s="10"/>
+      <c r="E43" s="10"/>
+      <c r="F43" s="10"/>
+    </row>
+    <row r="44" spans="1:6" ht="14" x14ac:dyDescent="0.3">
+      <c r="A44" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="B44" s="46" t="s">
+        <v>42</v>
+      </c>
+      <c r="C44" s="46" t="s">
+        <v>41</v>
+      </c>
+      <c r="D44" s="46" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" s="7" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A45" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="B45" s="47"/>
+      <c r="C45" s="47"/>
+      <c r="D45" s="51"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="B46" s="23"/>
+      <c r="C46" s="49"/>
+      <c r="D46" s="52"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="B47" s="47"/>
+      <c r="C47" s="47"/>
+      <c r="D47" s="51"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="B48" s="23"/>
+      <c r="C48" s="49"/>
+      <c r="D48" s="52"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="B49" s="47"/>
+      <c r="C49" s="47"/>
+      <c r="D49" s="51"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="B50" s="23"/>
+      <c r="C50" s="49"/>
+      <c r="D50" s="52"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="B51" s="47"/>
+      <c r="C51" s="47"/>
+      <c r="D51" s="51"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="B52" s="23"/>
+      <c r="C52" s="49"/>
+      <c r="D52" s="52"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="B53" s="47"/>
+      <c r="C53" s="47"/>
+      <c r="D53" s="51"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="B54" s="24"/>
+      <c r="C54" s="48"/>
+      <c r="D54" s="53"/>
+    </row>
+    <row r="55" spans="1:6" ht="6.65" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B55" s="10"/>
+      <c r="C55" s="10"/>
+      <c r="D55" s="10"/>
+      <c r="E55" s="10"/>
+      <c r="F55" s="10"/>
+    </row>
+    <row r="57" spans="1:6" s="7" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A57" s="26" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" s="28" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+      <c r="A58" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="B58" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="C58" s="31" t="s">
+        <v>56</v>
+      </c>
+      <c r="D58" s="31" t="s">
+        <v>57</v>
+      </c>
+      <c r="E58" s="31" t="s">
+        <v>58</v>
+      </c>
+      <c r="F58" s="31" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" s="5"/>
+      <c r="B59" s="12"/>
+      <c r="C59" s="2"/>
+      <c r="D59" s="6"/>
+      <c r="E59" s="5"/>
+      <c r="F59" s="12"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" s="5"/>
+      <c r="B60" s="12"/>
+      <c r="C60" s="2"/>
+      <c r="D60" s="6"/>
+      <c r="E60" s="12"/>
+      <c r="F60" s="12"/>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" s="5"/>
+      <c r="B61" s="12"/>
+      <c r="C61" s="2"/>
+      <c r="D61" s="6"/>
+      <c r="E61" s="5"/>
+      <c r="F61" s="12"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" s="5"/>
+      <c r="B62" s="12"/>
+      <c r="C62" s="2"/>
+      <c r="D62" s="6"/>
+      <c r="E62" s="5"/>
+      <c r="F62" s="12"/>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" s="5"/>
+      <c r="B63" s="5"/>
+      <c r="D63" s="6"/>
+      <c r="E63" s="5"/>
+      <c r="F63" s="5"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" s="5"/>
+      <c r="B64" s="5"/>
+      <c r="D64" s="6"/>
+      <c r="E64" s="5"/>
+      <c r="F64" s="5"/>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" s="5"/>
+      <c r="B65" s="5"/>
+      <c r="D65" s="6"/>
+      <c r="E65" s="5"/>
+      <c r="F65" s="5"/>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" s="5"/>
+      <c r="B66" s="5"/>
+      <c r="D66" s="6"/>
+      <c r="E66" s="5"/>
+      <c r="F66" s="5"/>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" s="5"/>
+      <c r="B67" s="5"/>
+      <c r="D67" s="6"/>
+      <c r="E67" s="5"/>
+      <c r="F67" s="5"/>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" s="5"/>
+      <c r="B68" s="5"/>
+      <c r="D68" s="6"/>
+      <c r="E68" s="5"/>
+      <c r="F68" s="5"/>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69" s="5"/>
+      <c r="B69" s="5"/>
+      <c r="D69" s="6"/>
+      <c r="E69" s="5"/>
+      <c r="F69" s="5"/>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70" s="5"/>
+      <c r="B70" s="5"/>
+      <c r="D70" s="6"/>
+      <c r="E70" s="5"/>
+      <c r="F70" s="5"/>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71" s="5"/>
+      <c r="B71" s="5"/>
+      <c r="D71" s="6"/>
+      <c r="E71" s="5"/>
+      <c r="F71" s="5"/>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72" s="5"/>
+      <c r="B72" s="5"/>
+      <c r="D72" s="6"/>
+      <c r="E72" s="5"/>
+      <c r="F72" s="5"/>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73" s="5"/>
+      <c r="B73" s="5"/>
+      <c r="D73" s="6"/>
+      <c r="E73" s="5"/>
+      <c r="F73" s="5"/>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74" s="5"/>
+      <c r="B74" s="5"/>
+      <c r="D74" s="6"/>
+      <c r="E74" s="5"/>
+      <c r="F74" s="5"/>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75" s="5"/>
+      <c r="B75" s="5"/>
+      <c r="D75" s="6"/>
+      <c r="E75" s="5"/>
+      <c r="F75" s="5"/>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A76" s="5"/>
+      <c r="B76" s="5"/>
+      <c r="D76" s="6"/>
+      <c r="E76" s="5"/>
+      <c r="F76" s="5"/>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77" s="5"/>
+      <c r="B77" s="5"/>
+      <c r="D77" s="6"/>
+      <c r="E77" s="5"/>
+      <c r="F77" s="5"/>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78" s="5"/>
+      <c r="B78" s="5"/>
+      <c r="D78" s="6"/>
+      <c r="E78" s="5"/>
+      <c r="F78" s="5"/>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79" s="5"/>
+      <c r="B79" s="5"/>
+      <c r="D79" s="6"/>
+      <c r="E79" s="5"/>
+      <c r="F79" s="5"/>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A80" s="5"/>
+      <c r="B80" s="5"/>
+      <c r="D80" s="6"/>
+      <c r="E80" s="5"/>
+      <c r="F80" s="5"/>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A81" s="5"/>
+      <c r="B81" s="5"/>
+      <c r="D81" s="6"/>
+      <c r="E81" s="5"/>
+      <c r="F81" s="5"/>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82" s="5"/>
+      <c r="B82" s="5"/>
+      <c r="D82" s="6"/>
+      <c r="E82" s="5"/>
+      <c r="F82" s="5"/>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A83" s="5"/>
+      <c r="B83" s="5"/>
+      <c r="D83" s="6"/>
+      <c r="E83" s="5"/>
+      <c r="F83" s="5"/>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A84" s="5"/>
+      <c r="B84" s="5"/>
+      <c r="D84" s="6"/>
+      <c r="E84" s="5"/>
+      <c r="F84" s="5"/>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A85" s="5"/>
+      <c r="B85" s="5"/>
+      <c r="D85" s="6"/>
+      <c r="E85" s="5"/>
+      <c r="F85" s="5"/>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A86" s="5"/>
+      <c r="B86" s="5"/>
+      <c r="D86" s="6"/>
+      <c r="E86" s="5"/>
+      <c r="F86" s="5"/>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A87" s="5"/>
+      <c r="B87" s="5"/>
+      <c r="D87" s="6"/>
+      <c r="E87" s="5"/>
+      <c r="F87" s="5"/>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A88" s="5"/>
+      <c r="B88" s="5"/>
+      <c r="D88" s="6"/>
+      <c r="E88" s="5"/>
+      <c r="F88" s="5"/>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A89" s="5"/>
+      <c r="B89" s="5"/>
+      <c r="D89" s="6"/>
+      <c r="E89" s="5"/>
+      <c r="F89" s="5"/>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A90" s="5"/>
+      <c r="B90" s="5"/>
+      <c r="D90" s="6"/>
+      <c r="E90" s="5"/>
+      <c r="F90" s="5"/>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A91" s="5"/>
+      <c r="B91" s="5"/>
+      <c r="D91" s="6"/>
+      <c r="E91" s="5"/>
+      <c r="F91" s="5"/>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A92" s="5"/>
+      <c r="B92" s="5"/>
+      <c r="D92" s="6"/>
+      <c r="E92" s="5"/>
+      <c r="F92" s="5"/>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A93" s="5"/>
+      <c r="B93" s="5"/>
+      <c r="D93" s="6"/>
+      <c r="E93" s="5"/>
+      <c r="F93" s="5"/>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A94" s="5"/>
+      <c r="B94" s="5"/>
+      <c r="D94" s="6"/>
+      <c r="E94" s="5"/>
+      <c r="F94" s="5"/>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A95" s="5"/>
+      <c r="B95" s="5"/>
+      <c r="D95" s="6"/>
+      <c r="E95" s="5"/>
+      <c r="F95" s="5"/>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A96" s="5"/>
+      <c r="B96" s="5"/>
+      <c r="D96" s="6"/>
+      <c r="E96" s="5"/>
+      <c r="F96" s="5"/>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A97" s="5"/>
+      <c r="B97" s="5"/>
+      <c r="D97" s="6"/>
+      <c r="E97" s="5"/>
+      <c r="F97" s="5"/>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A98" s="5"/>
+      <c r="B98" s="5"/>
+      <c r="D98" s="6"/>
+      <c r="E98" s="5"/>
+      <c r="F98" s="5"/>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A99" s="5"/>
+      <c r="B99" s="5"/>
+      <c r="D99" s="6"/>
+      <c r="E99" s="5"/>
+      <c r="F99" s="5"/>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A100" s="5"/>
+      <c r="B100" s="5"/>
+      <c r="D100" s="6"/>
+      <c r="E100" s="5"/>
+      <c r="F100" s="5"/>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A101" s="5"/>
+      <c r="B101" s="5"/>
+      <c r="D101" s="6"/>
+      <c r="E101" s="5"/>
+      <c r="F101" s="5"/>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A102" s="5"/>
+      <c r="B102" s="5"/>
+      <c r="D102" s="6"/>
+      <c r="E102" s="5"/>
+      <c r="F102" s="5"/>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A103" s="5"/>
+      <c r="B103" s="5"/>
+      <c r="D103" s="6"/>
+      <c r="E103" s="5"/>
+      <c r="F103" s="5"/>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A104" s="5"/>
+      <c r="B104" s="5"/>
+      <c r="D104" s="6"/>
+      <c r="E104" s="5"/>
+      <c r="F104" s="5"/>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A105" s="5"/>
+      <c r="B105" s="5"/>
+      <c r="D105" s="6"/>
+      <c r="E105" s="5"/>
+      <c r="F105" s="5"/>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A106" s="5"/>
+      <c r="B106" s="5"/>
+      <c r="D106" s="6"/>
+      <c r="E106" s="5"/>
+      <c r="F106" s="5"/>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A107" s="5"/>
+      <c r="B107" s="5"/>
+      <c r="D107" s="6"/>
+      <c r="E107" s="5"/>
+      <c r="F107" s="5"/>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A108" s="5"/>
+      <c r="B108" s="5"/>
+      <c r="D108" s="6"/>
+      <c r="E108" s="5"/>
+      <c r="F108" s="5"/>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A109" s="5"/>
+      <c r="B109" s="5"/>
+      <c r="D109" s="6"/>
+      <c r="E109" s="5"/>
+      <c r="F109" s="5"/>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A110" s="5"/>
+      <c r="B110" s="5"/>
+      <c r="D110" s="6"/>
+      <c r="E110" s="5"/>
+      <c r="F110" s="5"/>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A111" s="5"/>
+      <c r="B111" s="5"/>
+      <c r="D111" s="6"/>
+      <c r="E111" s="5"/>
+      <c r="F111" s="5"/>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A112" s="5"/>
+      <c r="B112" s="5"/>
+      <c r="D112" s="6"/>
+      <c r="E112" s="5"/>
+      <c r="F112" s="5"/>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A113" s="5"/>
+      <c r="B113" s="5"/>
+      <c r="D113" s="6"/>
+      <c r="E113" s="5"/>
+      <c r="F113" s="5"/>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A114" s="5"/>
+      <c r="B114" s="5"/>
+      <c r="D114" s="6"/>
+      <c r="E114" s="5"/>
+      <c r="F114" s="5"/>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A115" s="5"/>
+      <c r="B115" s="5"/>
+      <c r="D115" s="6"/>
+      <c r="E115" s="5"/>
+      <c r="F115" s="5"/>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A116" s="5"/>
+      <c r="B116" s="5"/>
+      <c r="D116" s="6"/>
+      <c r="E116" s="5"/>
+      <c r="F116" s="5"/>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A117" s="5"/>
+      <c r="B117" s="5"/>
+      <c r="D117" s="6"/>
+      <c r="E117" s="5"/>
+      <c r="F117" s="5"/>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A118" s="5"/>
+      <c r="B118" s="5"/>
+      <c r="D118" s="6"/>
+      <c r="E118" s="5"/>
+      <c r="F118" s="5"/>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A119" s="5"/>
+      <c r="B119" s="5"/>
+      <c r="D119" s="6"/>
+      <c r="E119" s="5"/>
+      <c r="F119" s="5"/>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A120" s="5"/>
+      <c r="B120" s="5"/>
+      <c r="D120" s="6"/>
+      <c r="E120" s="5"/>
+      <c r="F120" s="5"/>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A121" s="5"/>
+      <c r="B121" s="5"/>
+      <c r="D121" s="6"/>
+      <c r="E121" s="5"/>
+      <c r="F121" s="5"/>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A122" s="5"/>
+      <c r="B122" s="5"/>
+      <c r="D122" s="6"/>
+      <c r="E122" s="5"/>
+      <c r="F122" s="5"/>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A123" s="5"/>
+      <c r="B123" s="5"/>
+      <c r="D123" s="6"/>
+      <c r="E123" s="5"/>
+      <c r="F123" s="5"/>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A124" s="5"/>
+      <c r="B124" s="5"/>
+      <c r="D124" s="6"/>
+      <c r="E124" s="5"/>
+      <c r="F124" s="5"/>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A125" s="5"/>
+      <c r="B125" s="5"/>
+      <c r="D125" s="6"/>
+      <c r="E125" s="5"/>
+      <c r="F125" s="5"/>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A126" s="5"/>
+      <c r="B126" s="5"/>
+      <c r="D126" s="6"/>
+      <c r="E126" s="5"/>
+      <c r="F126" s="5"/>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A127" s="5"/>
+      <c r="B127" s="5"/>
+      <c r="D127" s="6"/>
+      <c r="E127" s="5"/>
+      <c r="F127" s="5"/>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A128" s="5"/>
+      <c r="B128" s="5"/>
+      <c r="D128" s="6"/>
+      <c r="E128" s="5"/>
+      <c r="F128" s="5"/>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A129" s="5"/>
+      <c r="B129" s="5"/>
+      <c r="D129" s="6"/>
+      <c r="E129" s="5"/>
+      <c r="F129" s="5"/>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A130" s="5"/>
+      <c r="B130" s="5"/>
+      <c r="D130" s="6"/>
+      <c r="E130" s="5"/>
+      <c r="F130" s="5"/>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A131" s="5"/>
+      <c r="B131" s="5"/>
+      <c r="D131" s="6"/>
+      <c r="E131" s="5"/>
+      <c r="F131" s="5"/>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A132" s="5"/>
+      <c r="B132" s="5"/>
+      <c r="D132" s="6"/>
+      <c r="E132" s="5"/>
+      <c r="F132" s="5"/>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A133" s="5"/>
+      <c r="B133" s="5"/>
+      <c r="D133" s="6"/>
+      <c r="E133" s="5"/>
+      <c r="F133" s="5"/>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A134" s="5"/>
+      <c r="B134" s="5"/>
+      <c r="D134" s="6"/>
+      <c r="E134" s="5"/>
+      <c r="F134" s="5"/>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A135" s="5"/>
+      <c r="B135" s="5"/>
+      <c r="D135" s="6"/>
+      <c r="E135" s="5"/>
+      <c r="F135" s="5"/>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A136" s="5"/>
+      <c r="B136" s="5"/>
+      <c r="D136" s="6"/>
+      <c r="E136" s="5"/>
+      <c r="F136" s="5"/>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A137" s="5"/>
+      <c r="B137" s="5"/>
+      <c r="D137" s="6"/>
+      <c r="E137" s="5"/>
+      <c r="F137" s="5"/>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A138" s="5"/>
+      <c r="B138" s="5"/>
+      <c r="D138" s="6"/>
+      <c r="E138" s="5"/>
+      <c r="F138" s="5"/>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A139" s="5"/>
+      <c r="B139" s="5"/>
+      <c r="D139" s="6"/>
+      <c r="E139" s="5"/>
+      <c r="F139" s="5"/>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A140" s="5"/>
+      <c r="B140" s="5"/>
+      <c r="D140" s="6"/>
+      <c r="E140" s="5"/>
+      <c r="F140" s="5"/>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A141" s="5"/>
+      <c r="B141" s="5"/>
+      <c r="D141" s="6"/>
+      <c r="E141" s="5"/>
+      <c r="F141" s="5"/>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A142" s="5"/>
+      <c r="B142" s="5"/>
+      <c r="D142" s="6"/>
+      <c r="E142" s="5"/>
+      <c r="F142" s="5"/>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A143" s="5"/>
+      <c r="B143" s="5"/>
+      <c r="D143" s="6"/>
+      <c r="E143" s="5"/>
+      <c r="F143" s="5"/>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A144" s="5"/>
+      <c r="B144" s="5"/>
+      <c r="D144" s="6"/>
+      <c r="E144" s="5"/>
+      <c r="F144" s="5"/>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A145" s="5"/>
+      <c r="B145" s="5"/>
+      <c r="D145" s="6"/>
+      <c r="E145" s="5"/>
+      <c r="F145" s="5"/>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A146" s="5"/>
+      <c r="B146" s="5"/>
+      <c r="D146" s="6"/>
+      <c r="E146" s="5"/>
+      <c r="F146" s="5"/>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A147" s="5"/>
+      <c r="B147" s="5"/>
+      <c r="D147" s="6"/>
+      <c r="E147" s="5"/>
+      <c r="F147" s="5"/>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A148" s="5"/>
+      <c r="B148" s="5"/>
+      <c r="D148" s="6"/>
+      <c r="E148" s="5"/>
+      <c r="F148" s="5"/>
+    </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A149" s="5"/>
+      <c r="B149" s="5"/>
+      <c r="D149" s="6"/>
+      <c r="E149" s="5"/>
+      <c r="F149" s="5"/>
+    </row>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A150" s="5"/>
+      <c r="B150" s="5"/>
+      <c r="D150" s="6"/>
+      <c r="E150" s="5"/>
+      <c r="F150" s="5"/>
+    </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A151" s="5"/>
+      <c r="B151" s="5"/>
+      <c r="D151" s="6"/>
+      <c r="E151" s="5"/>
+      <c r="F151" s="5"/>
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A152" s="5"/>
+      <c r="B152" s="5"/>
+      <c r="D152" s="6"/>
+      <c r="E152" s="5"/>
+      <c r="F152" s="5"/>
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A153" s="5"/>
+      <c r="B153" s="5"/>
+      <c r="D153" s="6"/>
+      <c r="E153" s="5"/>
+      <c r="F153" s="5"/>
+    </row>
+    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A154" s="5"/>
+      <c r="B154" s="5"/>
+      <c r="D154" s="6"/>
+      <c r="E154" s="5"/>
+      <c r="F154" s="5"/>
+    </row>
+    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E155" s="5"/>
+      <c r="F155" s="5"/>
+    </row>
+    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E156" s="5"/>
+      <c r="F156" s="5"/>
+    </row>
+    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E157" s="5"/>
+      <c r="F157" s="5"/>
+    </row>
+    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E158" s="5"/>
+      <c r="F158" s="5"/>
+    </row>
+    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E159" s="5"/>
+      <c r="F159" s="5"/>
+    </row>
+    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E160" s="5"/>
+      <c r="F160" s="5"/>
+    </row>
+    <row r="161" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E161" s="5"/>
+      <c r="F161" s="5"/>
+    </row>
+    <row r="162" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E162" s="5"/>
+      <c r="F162" s="5"/>
+    </row>
+    <row r="163" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E163" s="5"/>
+      <c r="F163" s="5"/>
+    </row>
+    <row r="164" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E164" s="5"/>
+      <c r="F164" s="5"/>
+    </row>
+    <row r="165" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E165" s="5"/>
+      <c r="F165" s="5"/>
+    </row>
+    <row r="166" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E166" s="5"/>
+      <c r="F166" s="5"/>
+    </row>
+    <row r="167" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E167" s="5"/>
+      <c r="F167" s="5"/>
+    </row>
+    <row r="168" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E168" s="5"/>
+      <c r="F168" s="5"/>
+    </row>
+    <row r="169" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E169" s="5"/>
+      <c r="F169" s="5"/>
+    </row>
+    <row r="170" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E170" s="5"/>
+      <c r="F170" s="5"/>
+    </row>
+    <row r="171" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E171" s="5"/>
+      <c r="F171" s="5"/>
+    </row>
+    <row r="172" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E172" s="5"/>
+      <c r="F172" s="5"/>
+    </row>
+    <row r="173" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E173" s="5"/>
+      <c r="F173" s="5"/>
+    </row>
+    <row r="174" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E174" s="5"/>
+      <c r="F174" s="5"/>
+    </row>
+    <row r="175" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E175" s="5"/>
+      <c r="F175" s="5"/>
+    </row>
+    <row r="176" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E176" s="5"/>
+      <c r="F176" s="5"/>
+    </row>
+    <row r="177" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E177" s="5"/>
+      <c r="F177" s="5"/>
+    </row>
+    <row r="178" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E178" s="5"/>
+      <c r="F178" s="5"/>
+    </row>
+    <row r="179" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E179" s="5"/>
+      <c r="F179" s="5"/>
+    </row>
+    <row r="180" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E180" s="5"/>
+      <c r="F180" s="5"/>
+    </row>
+    <row r="181" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E181" s="5"/>
+      <c r="F181" s="5"/>
+    </row>
+    <row r="182" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E182" s="5"/>
+      <c r="F182" s="5"/>
+    </row>
+    <row r="183" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E183" s="5"/>
+      <c r="F183" s="5"/>
+    </row>
+    <row r="184" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E184" s="5"/>
+      <c r="F184" s="5"/>
+    </row>
+    <row r="185" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E185" s="5"/>
+      <c r="F185" s="5"/>
+    </row>
+    <row r="186" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E186" s="5"/>
+      <c r="F186" s="5"/>
+    </row>
+    <row r="187" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E187" s="5"/>
+      <c r="F187" s="5"/>
+    </row>
+    <row r="188" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E188" s="5"/>
+      <c r="F188" s="5"/>
+    </row>
+    <row r="189" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E189" s="5"/>
+      <c r="F189" s="5"/>
+    </row>
+    <row r="190" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E190" s="5"/>
+      <c r="F190" s="5"/>
+    </row>
+    <row r="191" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E191" s="5"/>
+      <c r="F191" s="5"/>
+    </row>
+    <row r="192" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E192" s="5"/>
+      <c r="F192" s="5"/>
+    </row>
+    <row r="193" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E193" s="5"/>
+      <c r="F193" s="5"/>
+    </row>
+    <row r="194" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E194" s="5"/>
+      <c r="F194" s="5"/>
+    </row>
+    <row r="195" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E195" s="5"/>
+      <c r="F195" s="5"/>
+    </row>
+    <row r="196" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E196" s="5"/>
+      <c r="F196" s="5"/>
+    </row>
+    <row r="197" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E197" s="5"/>
+      <c r="F197" s="5"/>
+    </row>
+    <row r="198" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E198" s="5"/>
+      <c r="F198" s="5"/>
+    </row>
+    <row r="199" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E199" s="5"/>
+      <c r="F199" s="5"/>
+    </row>
+    <row r="200" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E200" s="5"/>
+      <c r="F200" s="5"/>
+    </row>
+    <row r="201" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E201" s="5"/>
+      <c r="F201" s="5"/>
+    </row>
+    <row r="202" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E202" s="5"/>
+      <c r="F202" s="5"/>
+    </row>
+    <row r="203" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E203" s="5"/>
+      <c r="F203" s="5"/>
+    </row>
+    <row r="204" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E204" s="5"/>
+      <c r="F204" s="5"/>
+    </row>
+    <row r="205" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E205" s="5"/>
+      <c r="F205" s="5"/>
+    </row>
+    <row r="206" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E206" s="5"/>
+      <c r="F206" s="5"/>
+    </row>
+    <row r="207" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E207" s="5"/>
+      <c r="F207" s="5"/>
+    </row>
+    <row r="208" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E208" s="5"/>
+      <c r="F208" s="5"/>
+    </row>
+    <row r="209" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E209" s="5"/>
+      <c r="F209" s="5"/>
+    </row>
+    <row r="210" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E210" s="5"/>
+      <c r="F210" s="5"/>
+    </row>
+    <row r="211" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E211" s="5"/>
+      <c r="F211" s="5"/>
+    </row>
+    <row r="212" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E212" s="5"/>
+      <c r="F212" s="5"/>
+    </row>
+    <row r="213" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E213" s="5"/>
+      <c r="F213" s="5"/>
+    </row>
+    <row r="214" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E214" s="5"/>
+      <c r="F214" s="5"/>
+    </row>
+    <row r="215" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E215" s="5"/>
+      <c r="F215" s="5"/>
+    </row>
+    <row r="216" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E216" s="5"/>
+      <c r="F216" s="5"/>
+    </row>
+    <row r="217" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E217" s="5"/>
+      <c r="F217" s="5"/>
+    </row>
+    <row r="218" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E218" s="5"/>
+      <c r="F218" s="5"/>
+    </row>
+    <row r="219" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E219" s="5"/>
+      <c r="F219" s="5"/>
+    </row>
+    <row r="220" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E220" s="5"/>
+      <c r="F220" s="5"/>
+    </row>
+    <row r="221" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E221" s="5"/>
+      <c r="F221" s="5"/>
+    </row>
+    <row r="222" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E222" s="5"/>
+      <c r="F222" s="5"/>
+    </row>
+    <row r="223" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E223" s="5"/>
+      <c r="F223" s="5"/>
+    </row>
+    <row r="224" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E224" s="5"/>
+      <c r="F224" s="5"/>
+    </row>
+    <row r="225" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E225" s="5"/>
+      <c r="F225" s="5"/>
+    </row>
+    <row r="226" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E226" s="5"/>
+      <c r="F226" s="5"/>
+    </row>
+    <row r="227" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E227" s="5"/>
+      <c r="F227" s="5"/>
+    </row>
+    <row r="228" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E228" s="5"/>
+      <c r="F228" s="5"/>
+    </row>
+    <row r="229" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E229" s="5"/>
+      <c r="F229" s="5"/>
+    </row>
+    <row r="230" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E230" s="5"/>
+      <c r="F230" s="5"/>
+    </row>
+    <row r="231" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E231" s="5"/>
+      <c r="F231" s="5"/>
+    </row>
+    <row r="232" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E232" s="5"/>
+      <c r="F232" s="5"/>
+    </row>
+  </sheetData>
+  <dataConsolidate/>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <conditionalFormatting sqref="B22:B23">
+    <cfRule type="containsBlanks" dxfId="17" priority="1">
+      <formula>LEN(TRIM(B22))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="5" scale="83" fitToHeight="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9EDFB13-CC9D-4AE8-A510-666896E1D552}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:F241"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="C53" sqref="C53"/>
+    <sheetView topLeftCell="A44" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="A66" sqref="A66:F67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1728,24 +3394,24 @@
       <c r="B1" s="45" t="s">
         <v>155</v>
       </c>
-      <c r="C1" s="70" t="s">
+      <c r="C1" s="74" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="70"/>
-      <c r="E1" s="70"/>
-      <c r="F1" s="70"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="74"/>
     </row>
     <row r="2" spans="1:6" ht="13" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="3"/>
-      <c r="C2" s="70" t="s">
+      <c r="C2" s="74" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
+      <c r="D2" s="74"/>
+      <c r="E2" s="74"/>
+      <c r="F2" s="74"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -1768,123 +3434,123 @@
       <c r="A6" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="71" t="s">
+      <c r="B6" s="75" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="71"/>
-      <c r="D6" s="71"/>
-      <c r="E6" s="71"/>
-      <c r="F6" s="71"/>
+      <c r="C6" s="75"/>
+      <c r="D6" s="75"/>
+      <c r="E6" s="75"/>
+      <c r="F6" s="75"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="69"/>
-      <c r="C7" s="69"/>
-      <c r="D7" s="69"/>
-      <c r="E7" s="69"/>
-      <c r="F7" s="69"/>
+      <c r="B7" s="73"/>
+      <c r="C7" s="73"/>
+      <c r="D7" s="73"/>
+      <c r="E7" s="73"/>
+      <c r="F7" s="73"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="72"/>
-      <c r="C8" s="72"/>
-      <c r="D8" s="72"/>
-      <c r="E8" s="72"/>
-      <c r="F8" s="72"/>
+      <c r="B8" s="76"/>
+      <c r="C8" s="76"/>
+      <c r="D8" s="76"/>
+      <c r="E8" s="76"/>
+      <c r="F8" s="76"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="69"/>
-      <c r="C9" s="69"/>
-      <c r="D9" s="69"/>
-      <c r="E9" s="69"/>
-      <c r="F9" s="69"/>
+      <c r="B9" s="73"/>
+      <c r="C9" s="73"/>
+      <c r="D9" s="73"/>
+      <c r="E9" s="73"/>
+      <c r="F9" s="73"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="72"/>
-      <c r="C10" s="72"/>
-      <c r="D10" s="72"/>
-      <c r="E10" s="72"/>
-      <c r="F10" s="72"/>
+      <c r="B10" s="76"/>
+      <c r="C10" s="76"/>
+      <c r="D10" s="76"/>
+      <c r="E10" s="76"/>
+      <c r="F10" s="76"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="69"/>
-      <c r="C11" s="69"/>
-      <c r="D11" s="69"/>
-      <c r="E11" s="69"/>
-      <c r="F11" s="69"/>
+      <c r="B11" s="73"/>
+      <c r="C11" s="73"/>
+      <c r="D11" s="73"/>
+      <c r="E11" s="73"/>
+      <c r="F11" s="73"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="72"/>
-      <c r="C12" s="72"/>
-      <c r="D12" s="72"/>
-      <c r="E12" s="72"/>
-      <c r="F12" s="72"/>
+      <c r="B12" s="76"/>
+      <c r="C12" s="76"/>
+      <c r="D12" s="76"/>
+      <c r="E12" s="76"/>
+      <c r="F12" s="76"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="69"/>
-      <c r="C13" s="69"/>
-      <c r="D13" s="69"/>
-      <c r="E13" s="69"/>
-      <c r="F13" s="69"/>
+      <c r="B13" s="73"/>
+      <c r="C13" s="73"/>
+      <c r="D13" s="73"/>
+      <c r="E13" s="73"/>
+      <c r="F13" s="73"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="72"/>
-      <c r="C14" s="72"/>
-      <c r="D14" s="72"/>
-      <c r="E14" s="72"/>
-      <c r="F14" s="72"/>
+      <c r="B14" s="76"/>
+      <c r="C14" s="76"/>
+      <c r="D14" s="76"/>
+      <c r="E14" s="76"/>
+      <c r="F14" s="76"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="69"/>
-      <c r="C15" s="69"/>
-      <c r="D15" s="69"/>
-      <c r="E15" s="69"/>
-      <c r="F15" s="69"/>
+      <c r="B15" s="73"/>
+      <c r="C15" s="73"/>
+      <c r="D15" s="73"/>
+      <c r="E15" s="73"/>
+      <c r="F15" s="73"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="72"/>
-      <c r="C16" s="72"/>
-      <c r="D16" s="72"/>
-      <c r="E16" s="72"/>
-      <c r="F16" s="72"/>
+      <c r="B16" s="76"/>
+      <c r="C16" s="76"/>
+      <c r="D16" s="76"/>
+      <c r="E16" s="76"/>
+      <c r="F16" s="76"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="69"/>
-      <c r="C17" s="69"/>
-      <c r="D17" s="69"/>
-      <c r="E17" s="69"/>
-      <c r="F17" s="69"/>
+      <c r="B17" s="73"/>
+      <c r="C17" s="73"/>
+      <c r="D17" s="73"/>
+      <c r="E17" s="73"/>
+      <c r="F17" s="73"/>
     </row>
     <row r="18" spans="1:6" ht="6.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="9"/>
@@ -1948,12 +3614,12 @@
       <c r="B27" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C27" s="72" t="s">
+      <c r="C27" s="76" t="s">
         <v>23</v>
       </c>
-      <c r="D27" s="72"/>
-      <c r="E27" s="72"/>
-      <c r="F27" s="72"/>
+      <c r="D27" s="76"/>
+      <c r="E27" s="76"/>
+      <c r="F27" s="76"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="s">
@@ -1962,10 +3628,10 @@
       <c r="B28" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C28" s="72"/>
-      <c r="D28" s="72"/>
-      <c r="E28" s="72"/>
-      <c r="F28" s="72"/>
+      <c r="C28" s="76"/>
+      <c r="D28" s="76"/>
+      <c r="E28" s="76"/>
+      <c r="F28" s="76"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="s">
@@ -2012,7 +3678,7 @@
         <v>143</v>
       </c>
       <c r="B34" s="63" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D34" s="54"/>
       <c r="E34" s="54"/>
@@ -3323,11 +4989,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B096AE39-CBE9-438B-8EF5-43BA511A3359}">
   <dimension ref="A1:I583"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+    <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
       <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
@@ -3350,24 +5016,24 @@
       <c r="B1" s="45" t="s">
         <v>155</v>
       </c>
-      <c r="C1" s="70" t="s">
+      <c r="C1" s="74" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="70"/>
-      <c r="E1" s="70"/>
-      <c r="F1" s="70"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="74"/>
     </row>
     <row r="2" spans="1:7" ht="13" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="3"/>
-      <c r="C2" s="70" t="s">
+      <c r="C2" s="74" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
+      <c r="D2" s="74"/>
+      <c r="E2" s="74"/>
+      <c r="F2" s="74"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -3391,12 +5057,12 @@
       <c r="A6" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="71" t="s">
+      <c r="B6" s="75" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="71"/>
-      <c r="D6" s="71"/>
-      <c r="E6" s="71"/>
+      <c r="C6" s="75"/>
+      <c r="D6" s="75"/>
+      <c r="E6" s="75"/>
       <c r="F6" s="17"/>
       <c r="G6" s="17"/>
     </row>
@@ -3404,110 +5070,110 @@
       <c r="A7" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="69"/>
-      <c r="C7" s="69"/>
-      <c r="D7" s="69"/>
-      <c r="E7" s="69"/>
+      <c r="B7" s="73"/>
+      <c r="C7" s="73"/>
+      <c r="D7" s="73"/>
+      <c r="E7" s="73"/>
       <c r="F7" s="56"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="72"/>
-      <c r="C8" s="72"/>
-      <c r="D8" s="72"/>
-      <c r="E8" s="72"/>
+      <c r="B8" s="76"/>
+      <c r="C8" s="76"/>
+      <c r="D8" s="76"/>
+      <c r="E8" s="76"/>
       <c r="F8" s="56"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="69"/>
-      <c r="C9" s="69"/>
-      <c r="D9" s="69"/>
-      <c r="E9" s="69"/>
+      <c r="B9" s="73"/>
+      <c r="C9" s="73"/>
+      <c r="D9" s="73"/>
+      <c r="E9" s="73"/>
       <c r="F9" s="56"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="72"/>
-      <c r="C10" s="72"/>
-      <c r="D10" s="72"/>
-      <c r="E10" s="72"/>
+      <c r="B10" s="76"/>
+      <c r="C10" s="76"/>
+      <c r="D10" s="76"/>
+      <c r="E10" s="76"/>
       <c r="F10" s="56"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="69"/>
-      <c r="C11" s="69"/>
-      <c r="D11" s="69"/>
-      <c r="E11" s="69"/>
+      <c r="B11" s="73"/>
+      <c r="C11" s="73"/>
+      <c r="D11" s="73"/>
+      <c r="E11" s="73"/>
       <c r="F11" s="56"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="72"/>
-      <c r="C12" s="72"/>
-      <c r="D12" s="72"/>
-      <c r="E12" s="72"/>
+      <c r="B12" s="76"/>
+      <c r="C12" s="76"/>
+      <c r="D12" s="76"/>
+      <c r="E12" s="76"/>
       <c r="F12" s="56"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="69"/>
-      <c r="C13" s="69"/>
-      <c r="D13" s="69"/>
-      <c r="E13" s="69"/>
+      <c r="B13" s="73"/>
+      <c r="C13" s="73"/>
+      <c r="D13" s="73"/>
+      <c r="E13" s="73"/>
       <c r="F13" s="56"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="72"/>
-      <c r="C14" s="72"/>
-      <c r="D14" s="72"/>
-      <c r="E14" s="72"/>
+      <c r="B14" s="76"/>
+      <c r="C14" s="76"/>
+      <c r="D14" s="76"/>
+      <c r="E14" s="76"/>
       <c r="F14" s="56"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="69"/>
-      <c r="C15" s="69"/>
-      <c r="D15" s="69"/>
-      <c r="E15" s="69"/>
+      <c r="B15" s="73"/>
+      <c r="C15" s="73"/>
+      <c r="D15" s="73"/>
+      <c r="E15" s="73"/>
       <c r="F15" s="56"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="72"/>
-      <c r="C16" s="72"/>
-      <c r="D16" s="72"/>
-      <c r="E16" s="72"/>
+      <c r="B16" s="76"/>
+      <c r="C16" s="76"/>
+      <c r="D16" s="76"/>
+      <c r="E16" s="76"/>
       <c r="F16" s="56"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="69"/>
-      <c r="C17" s="69"/>
-      <c r="D17" s="69"/>
-      <c r="E17" s="69"/>
+      <c r="B17" s="73"/>
+      <c r="C17" s="73"/>
+      <c r="D17" s="73"/>
+      <c r="E17" s="73"/>
       <c r="F17" s="56"/>
     </row>
     <row r="18" spans="1:7" ht="6.65" customHeight="1" x14ac:dyDescent="0.25">
@@ -3575,12 +5241,12 @@
       <c r="B27" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C27" s="72" t="s">
+      <c r="C27" s="76" t="s">
         <v>23</v>
       </c>
-      <c r="D27" s="72"/>
-      <c r="E27" s="72"/>
-      <c r="F27" s="72"/>
+      <c r="D27" s="76"/>
+      <c r="E27" s="76"/>
+      <c r="F27" s="76"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="s">
@@ -3589,10 +5255,10 @@
       <c r="B28" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C28" s="72"/>
-      <c r="D28" s="72"/>
-      <c r="E28" s="72"/>
-      <c r="F28" s="72"/>
+      <c r="C28" s="76"/>
+      <c r="D28" s="76"/>
+      <c r="E28" s="76"/>
+      <c r="F28" s="76"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="s">
@@ -7140,7 +8806,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{547A22CE-6B5B-419C-B571-1556B7859EB9}">
   <dimension ref="A1:G597"/>
   <sheetViews>
@@ -7209,135 +8875,135 @@
       <c r="A6" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="71" t="s">
+      <c r="B6" s="75" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="71"/>
-      <c r="D6" s="71"/>
-      <c r="E6" s="71"/>
-      <c r="F6" s="71"/>
-      <c r="G6" s="71"/>
+      <c r="C6" s="75"/>
+      <c r="D6" s="75"/>
+      <c r="E6" s="75"/>
+      <c r="F6" s="75"/>
+      <c r="G6" s="75"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="69"/>
-      <c r="C7" s="69"/>
-      <c r="D7" s="69"/>
-      <c r="E7" s="69"/>
-      <c r="F7" s="69"/>
-      <c r="G7" s="69"/>
+      <c r="B7" s="73"/>
+      <c r="C7" s="73"/>
+      <c r="D7" s="73"/>
+      <c r="E7" s="73"/>
+      <c r="F7" s="73"/>
+      <c r="G7" s="73"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="72"/>
-      <c r="C8" s="72"/>
-      <c r="D8" s="72"/>
-      <c r="E8" s="72"/>
-      <c r="F8" s="72"/>
-      <c r="G8" s="72"/>
+      <c r="B8" s="76"/>
+      <c r="C8" s="76"/>
+      <c r="D8" s="76"/>
+      <c r="E8" s="76"/>
+      <c r="F8" s="76"/>
+      <c r="G8" s="76"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="69"/>
-      <c r="C9" s="69"/>
-      <c r="D9" s="69"/>
-      <c r="E9" s="69"/>
-      <c r="F9" s="69"/>
-      <c r="G9" s="69"/>
+      <c r="B9" s="73"/>
+      <c r="C9" s="73"/>
+      <c r="D9" s="73"/>
+      <c r="E9" s="73"/>
+      <c r="F9" s="73"/>
+      <c r="G9" s="73"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="72"/>
-      <c r="C10" s="72"/>
-      <c r="D10" s="72"/>
-      <c r="E10" s="72"/>
-      <c r="F10" s="72"/>
-      <c r="G10" s="72"/>
+      <c r="B10" s="76"/>
+      <c r="C10" s="76"/>
+      <c r="D10" s="76"/>
+      <c r="E10" s="76"/>
+      <c r="F10" s="76"/>
+      <c r="G10" s="76"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="69"/>
-      <c r="C11" s="69"/>
-      <c r="D11" s="69"/>
-      <c r="E11" s="69"/>
-      <c r="F11" s="69"/>
-      <c r="G11" s="69"/>
+      <c r="B11" s="73"/>
+      <c r="C11" s="73"/>
+      <c r="D11" s="73"/>
+      <c r="E11" s="73"/>
+      <c r="F11" s="73"/>
+      <c r="G11" s="73"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="72"/>
-      <c r="C12" s="72"/>
-      <c r="D12" s="72"/>
-      <c r="E12" s="72"/>
-      <c r="F12" s="72"/>
-      <c r="G12" s="72"/>
+      <c r="B12" s="76"/>
+      <c r="C12" s="76"/>
+      <c r="D12" s="76"/>
+      <c r="E12" s="76"/>
+      <c r="F12" s="76"/>
+      <c r="G12" s="76"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="69"/>
-      <c r="C13" s="69"/>
-      <c r="D13" s="69"/>
-      <c r="E13" s="69"/>
-      <c r="F13" s="69"/>
-      <c r="G13" s="69"/>
+      <c r="B13" s="73"/>
+      <c r="C13" s="73"/>
+      <c r="D13" s="73"/>
+      <c r="E13" s="73"/>
+      <c r="F13" s="73"/>
+      <c r="G13" s="73"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="72"/>
-      <c r="C14" s="72"/>
-      <c r="D14" s="72"/>
-      <c r="E14" s="72"/>
-      <c r="F14" s="72"/>
-      <c r="G14" s="72"/>
+      <c r="B14" s="76"/>
+      <c r="C14" s="76"/>
+      <c r="D14" s="76"/>
+      <c r="E14" s="76"/>
+      <c r="F14" s="76"/>
+      <c r="G14" s="76"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="69"/>
-      <c r="C15" s="69"/>
-      <c r="D15" s="69"/>
-      <c r="E15" s="69"/>
-      <c r="F15" s="69"/>
-      <c r="G15" s="69"/>
+      <c r="B15" s="73"/>
+      <c r="C15" s="73"/>
+      <c r="D15" s="73"/>
+      <c r="E15" s="73"/>
+      <c r="F15" s="73"/>
+      <c r="G15" s="73"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="72"/>
-      <c r="C16" s="72"/>
-      <c r="D16" s="72"/>
-      <c r="E16" s="72"/>
-      <c r="F16" s="72"/>
-      <c r="G16" s="72"/>
+      <c r="B16" s="76"/>
+      <c r="C16" s="76"/>
+      <c r="D16" s="76"/>
+      <c r="E16" s="76"/>
+      <c r="F16" s="76"/>
+      <c r="G16" s="76"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="69"/>
-      <c r="C17" s="69"/>
-      <c r="D17" s="69"/>
-      <c r="E17" s="69"/>
-      <c r="F17" s="69"/>
-      <c r="G17" s="69"/>
+      <c r="B17" s="73"/>
+      <c r="C17" s="73"/>
+      <c r="D17" s="73"/>
+      <c r="E17" s="73"/>
+      <c r="F17" s="73"/>
+      <c r="G17" s="73"/>
     </row>
     <row r="18" spans="1:7" ht="6.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="9"/>
@@ -7407,12 +9073,12 @@
       <c r="B27" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C27" s="72" t="s">
+      <c r="C27" s="76" t="s">
         <v>23</v>
       </c>
-      <c r="D27" s="72"/>
-      <c r="E27" s="72"/>
-      <c r="F27" s="72"/>
+      <c r="D27" s="76"/>
+      <c r="E27" s="76"/>
+      <c r="F27" s="76"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="s">
@@ -7421,10 +9087,10 @@
       <c r="B28" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C28" s="72"/>
-      <c r="D28" s="72"/>
-      <c r="E28" s="72"/>
-      <c r="F28" s="72"/>
+      <c r="C28" s="76"/>
+      <c r="D28" s="76"/>
+      <c r="E28" s="76"/>
+      <c r="F28" s="76"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="s">
@@ -7512,11 +9178,11 @@
       <c r="D37" s="2"/>
     </row>
     <row r="38" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A38" s="76" t="s">
+      <c r="A38" s="80" t="s">
         <v>60</v>
       </c>
-      <c r="B38" s="76"/>
-      <c r="C38" s="76"/>
+      <c r="B38" s="80"/>
+      <c r="C38" s="80"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
@@ -7579,7 +9245,7 @@
       <c r="B46" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="C46" s="73" t="s">
+      <c r="C46" s="77" t="s">
         <v>157</v>
       </c>
       <c r="D46" s="37"/>
@@ -7591,7 +9257,7 @@
       <c r="B47" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="C47" s="74"/>
+      <c r="C47" s="78"/>
       <c r="D47" s="37"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
@@ -7601,7 +9267,7 @@
       <c r="B48" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="C48" s="74"/>
+      <c r="C48" s="78"/>
       <c r="D48" s="37"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -7611,7 +9277,7 @@
       <c r="B49" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="C49" s="74"/>
+      <c r="C49" s="78"/>
       <c r="D49" s="37"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -7621,7 +9287,7 @@
       <c r="B50" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="C50" s="74"/>
+      <c r="C50" s="78"/>
       <c r="D50" s="37"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -7631,7 +9297,7 @@
       <c r="B51" s="20" t="s">
         <v>72</v>
       </c>
-      <c r="C51" s="74"/>
+      <c r="C51" s="78"/>
       <c r="D51" s="37"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -7641,7 +9307,7 @@
       <c r="B52" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="C52" s="74"/>
+      <c r="C52" s="78"/>
       <c r="D52" s="37"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -7651,7 +9317,7 @@
       <c r="B53" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="C53" s="74"/>
+      <c r="C53" s="78"/>
       <c r="D53" s="37"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -7661,7 +9327,7 @@
       <c r="B54" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="C54" s="74"/>
+      <c r="C54" s="78"/>
       <c r="D54" s="37"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -7671,7 +9337,7 @@
       <c r="B55" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="C55" s="74"/>
+      <c r="C55" s="78"/>
       <c r="D55" s="37"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -7681,7 +9347,7 @@
       <c r="B56" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="C56" s="74"/>
+      <c r="C56" s="78"/>
       <c r="D56" s="37"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -7691,7 +9357,7 @@
       <c r="B57" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="C57" s="74"/>
+      <c r="C57" s="78"/>
       <c r="D57" s="37"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -7701,7 +9367,7 @@
       <c r="B58" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="C58" s="74"/>
+      <c r="C58" s="78"/>
       <c r="D58" s="37"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -7711,7 +9377,7 @@
       <c r="B59" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="C59" s="74"/>
+      <c r="C59" s="78"/>
       <c r="D59" s="37"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -7721,7 +9387,7 @@
       <c r="B60" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="C60" s="74"/>
+      <c r="C60" s="78"/>
       <c r="D60" s="37"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -7731,7 +9397,7 @@
       <c r="B61" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="C61" s="74"/>
+      <c r="C61" s="78"/>
       <c r="D61" s="37"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -7741,7 +9407,7 @@
       <c r="B62" s="20" t="s">
         <v>94</v>
       </c>
-      <c r="C62" s="74"/>
+      <c r="C62" s="78"/>
       <c r="D62" s="37"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -7751,7 +9417,7 @@
       <c r="B63" s="20" t="s">
         <v>96</v>
       </c>
-      <c r="C63" s="74"/>
+      <c r="C63" s="78"/>
       <c r="D63" s="37"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -7761,7 +9427,7 @@
       <c r="B64" s="20" t="s">
         <v>98</v>
       </c>
-      <c r="C64" s="74"/>
+      <c r="C64" s="78"/>
       <c r="D64" s="37"/>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
@@ -7771,7 +9437,7 @@
       <c r="B65" s="20" t="s">
         <v>100</v>
       </c>
-      <c r="C65" s="74"/>
+      <c r="C65" s="78"/>
       <c r="D65" s="37"/>
     </row>
     <row r="66" spans="1:7" ht="13" thickBot="1" x14ac:dyDescent="0.3">
@@ -7781,7 +9447,7 @@
       <c r="B66" s="34" t="s">
         <v>102</v>
       </c>
-      <c r="C66" s="75"/>
+      <c r="C66" s="79"/>
       <c r="D66" s="38"/>
     </row>
     <row r="67" spans="1:7" s="35" customFormat="1" ht="13" thickTop="1" x14ac:dyDescent="0.25">
@@ -10459,7 +12125,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CBCE2FF-AC7E-47F6-AFA7-5759B53B3059}">
   <dimension ref="A1:E46"/>
   <sheetViews>
@@ -10475,12 +12141,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="18" customFormat="1" ht="20" x14ac:dyDescent="0.4">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="81" t="s">
         <v>104</v>
       </c>
-      <c r="B1" s="77"/>
-      <c r="C1" s="77"/>
-      <c r="D1" s="77"/>
+      <c r="B1" s="81"/>
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
     </row>
     <row r="2" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">

</xml_diff>